<commit_message>
multiasset-equity-VaR-ES-ptf optimization(malino so far)
</commit_message>
<xml_diff>
--- a/input/multiassets.xlsx
+++ b/input/multiassets.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/935cc860ba0efd68/GitHub/myportfolio/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="68" documentId="13_ncr:1_{B10D7187-5546-4483-8DEF-63838578FBF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0B9E339D-7743-4C49-8537-FEFFAFEA1532}"/>
+  <xr:revisionPtr revIDLastSave="81" documentId="13_ncr:1_{B10D7187-5546-4483-8DEF-63838578FBF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8697EC8E-8124-448D-80A6-1090337D679B}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -302,7 +302,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="389" uniqueCount="211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="390" uniqueCount="212">
   <si>
     <t>iShares Core MSCI World UCITS ETF USD</t>
   </si>
@@ -1061,9 +1061,6 @@
     <t>Small Cap Global</t>
   </si>
   <si>
-    <t>WHEA.L</t>
-  </si>
-  <si>
     <t>iShares Edge MSCI World Momentum Factor UCITS ETF</t>
   </si>
   <si>
@@ -1076,9 +1073,6 @@
     <t>WSML.L</t>
   </si>
   <si>
-    <t>IE00BYTRRB94</t>
-  </si>
-  <si>
     <t>Xtrackers MSCI World Consumer Staples UCITS ETF (Acc)</t>
   </si>
   <si>
@@ -1094,9 +1088,6 @@
     <t>Link</t>
   </si>
   <si>
-    <t>SPDR MSCI World Health Care UCITS ETF</t>
-  </si>
-  <si>
     <t>Consumer Staples Global</t>
   </si>
   <si>
@@ -1106,9 +1097,6 @@
     <t>iShares Edge MSCI World Momentum Factor UCITS ETF (Acc) | IWMO | IE00BP3QZ825</t>
   </si>
   <si>
-    <t>SPDR MSCI World Health Care UCITS ETF | WHEA | IE00BYTRRB94</t>
-  </si>
-  <si>
     <t>iShares MSCI World Small Cap UCITS ETF | IUSN | IE00BF4RFH31</t>
   </si>
   <si>
@@ -1223,13 +1211,28 @@
     <t>World Low Volatility</t>
   </si>
   <si>
-    <t>World Healthcare</t>
-  </si>
-  <si>
     <t>iShares Edge MSCI USA Quality Factor UCITS ETF | QDVB | IE00BD1F4L37</t>
   </si>
   <si>
     <t>iShares Edge MSCI World Minimum Volatility UCITS ETF USD (Acc) | MVOL | IE00B8FHGS14</t>
+  </si>
+  <si>
+    <t>IBCX.AS</t>
+  </si>
+  <si>
+    <t>0.2%</t>
+  </si>
+  <si>
+    <t>iShares Euro Corporate Bond Large Cap UCITS ETF | IBCX | IE0032523478</t>
+  </si>
+  <si>
+    <t>iShares Euro Corporate Bond Large Cap UCITS ETF</t>
+  </si>
+  <si>
+    <t>EU Corp Large Cap bonds</t>
+  </si>
+  <si>
+    <t>IE0032523478</t>
   </si>
 </sst>
 </file>
@@ -1665,7 +1668,7 @@
     <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="103">
+  <cellXfs count="102">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1719,122 +1722,17 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="3"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -1863,58 +1761,162 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Collegamento ipertestuale" xfId="3" builtinId="8"/>
@@ -2201,7 +2203,7 @@
   <dimension ref="A1:L9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -2221,7 +2223,7 @@
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" s="2" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>19</v>
@@ -2259,19 +2261,19 @@
     </row>
     <row r="2" spans="1:12">
       <c r="A2" s="36" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="B2" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="C2" t="s">
+        <v>154</v>
+      </c>
+      <c r="D2" t="s">
         <v>155</v>
       </c>
-      <c r="D2" t="s">
-        <v>156</v>
-      </c>
       <c r="E2" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="F2" t="s">
         <v>17</v>
@@ -2280,7 +2282,7 @@
         <v>7</v>
       </c>
       <c r="H2" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="I2" s="1">
         <v>2.5000000000000001E-3</v>
@@ -2297,19 +2299,19 @@
     </row>
     <row r="3" spans="1:12">
       <c r="A3" s="36" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="B3" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="C3" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="D3" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="E3" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="F3" t="s">
         <v>11</v>
@@ -2329,19 +2331,19 @@
     </row>
     <row r="4" spans="1:12">
       <c r="A4" s="36" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="B4" t="s">
-        <v>207</v>
-      </c>
-      <c r="C4" s="102" t="s">
-        <v>196</v>
+        <v>203</v>
+      </c>
+      <c r="C4" t="s">
+        <v>192</v>
       </c>
       <c r="D4" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="E4" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="F4" t="s">
         <v>11</v>
@@ -2361,51 +2363,57 @@
     </row>
     <row r="5" spans="1:12">
       <c r="A5" s="36" t="s">
+        <v>167</v>
+      </c>
+      <c r="B5" t="s">
         <v>169</v>
       </c>
-      <c r="B5" t="s">
-        <v>208</v>
-      </c>
       <c r="C5" t="s">
-        <v>165</v>
+        <v>175</v>
       </c>
       <c r="D5" t="s">
-        <v>159</v>
+        <v>168</v>
       </c>
       <c r="E5" t="s">
-        <v>154</v>
+        <v>174</v>
       </c>
       <c r="F5" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="G5" t="s">
         <v>7</v>
       </c>
       <c r="H5" t="s">
-        <v>184</v>
+        <v>172</v>
       </c>
       <c r="I5" s="1">
-        <v>3.0000000000000001E-3</v>
+        <v>1.5E-3</v>
       </c>
       <c r="J5" t="s">
-        <v>54</v>
+        <v>34</v>
+      </c>
+      <c r="K5" t="s">
+        <v>84</v>
+      </c>
+      <c r="L5" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="6" spans="1:12">
       <c r="A6" s="36" t="s">
-        <v>171</v>
+        <v>208</v>
       </c>
       <c r="B6" t="s">
-        <v>173</v>
+        <v>210</v>
       </c>
       <c r="C6" t="s">
-        <v>179</v>
+        <v>209</v>
       </c>
       <c r="D6" t="s">
-        <v>172</v>
+        <v>211</v>
       </c>
       <c r="E6" t="s">
-        <v>178</v>
+        <v>206</v>
       </c>
       <c r="F6" t="s">
         <v>17</v>
@@ -2414,36 +2422,30 @@
         <v>7</v>
       </c>
       <c r="H6" t="s">
-        <v>176</v>
-      </c>
-      <c r="I6" s="1">
-        <v>1.5E-3</v>
+        <v>172</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>207</v>
       </c>
       <c r="J6" t="s">
         <v>34</v>
       </c>
-      <c r="K6" t="s">
-        <v>84</v>
-      </c>
-      <c r="L6" t="s">
-        <v>88</v>
-      </c>
     </row>
     <row r="7" spans="1:12">
       <c r="A7" s="36" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="B7" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="C7" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="D7" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="E7" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="F7" t="s">
         <v>11</v>
@@ -2452,7 +2454,7 @@
         <v>7</v>
       </c>
       <c r="H7" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="I7" s="1">
         <v>1E-3</v>
@@ -2469,19 +2471,19 @@
     </row>
     <row r="8" spans="1:12">
       <c r="A8" s="36" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B8" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="C8" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="D8" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="E8" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="F8" t="s">
         <v>11</v>
@@ -2490,7 +2492,7 @@
         <v>7</v>
       </c>
       <c r="H8" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="I8" s="1">
         <v>6.9999999999999999E-4</v>
@@ -2504,19 +2506,19 @@
     </row>
     <row r="9" spans="1:12">
       <c r="A9" s="36" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="B9" t="s">
         <v>75</v>
       </c>
       <c r="C9" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="D9" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="E9" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="F9" t="s">
         <v>17</v>
@@ -2525,7 +2527,7 @@
         <v>7</v>
       </c>
       <c r="H9" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="I9" s="1">
         <v>1.1999999999999999E-3</v>
@@ -2543,13 +2545,13 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" display="https://www.justetf.com/it/etf-profile.html?isin=IE00BP3QZ825" xr:uid="{5E561C16-8B8B-483B-AA10-D0DDAD2EE0FF}"/>
-    <hyperlink ref="A5" r:id="rId2" display="https://www.justetf.com/it/etf-profile.html?isin=IE00BYTRRB94" xr:uid="{7F0259C1-E0BF-4DDA-8122-BE9F2BE69234}"/>
-    <hyperlink ref="A6" r:id="rId3" display="https://www.justetf.com/it/etf-profile.html?isin=IE00B3VTN290" xr:uid="{6AB80B8F-0CAF-4297-B9BB-D72ED9AFBF01}"/>
-    <hyperlink ref="A8" r:id="rId4" display="https://www.justetf.com/it/etf-profile.html?isin=IE00BGR7L912" xr:uid="{69029A56-B54E-49FD-A0F5-77171229A26E}"/>
-    <hyperlink ref="A9" r:id="rId5" display="https://www.justetf.com/it/etf-profile.html?isin=IE00B579F325" xr:uid="{42CB0A67-6EA5-4F8A-A191-29BAAE4A4956}"/>
-    <hyperlink ref="A7" r:id="rId6" display="https://www.justetf.com/it/etf-profile.html?isin=IE00BDQYWQ65" xr:uid="{6C04B138-97D3-42C8-B6E1-00870CCBE0B4}"/>
-    <hyperlink ref="A3" r:id="rId7" display="https://www.justetf.com/it/etf-profile.html?isin=IE00BD1F4L37" xr:uid="{DF84D7C7-B8F6-477A-8C9A-D4997B54C865}"/>
-    <hyperlink ref="A4" r:id="rId8" display="https://www.justetf.com/it/etf-profile.html?isin=IE00B8FHGS14" xr:uid="{47A684AB-EAC0-4609-B6F5-2C135D16A87D}"/>
+    <hyperlink ref="A5" r:id="rId2" display="https://www.justetf.com/it/etf-profile.html?isin=IE00B3VTN290" xr:uid="{6AB80B8F-0CAF-4297-B9BB-D72ED9AFBF01}"/>
+    <hyperlink ref="A8" r:id="rId3" display="https://www.justetf.com/it/etf-profile.html?isin=IE00BGR7L912" xr:uid="{69029A56-B54E-49FD-A0F5-77171229A26E}"/>
+    <hyperlink ref="A9" r:id="rId4" display="https://www.justetf.com/it/etf-profile.html?isin=IE00B579F325" xr:uid="{42CB0A67-6EA5-4F8A-A191-29BAAE4A4956}"/>
+    <hyperlink ref="A7" r:id="rId5" display="https://www.justetf.com/it/etf-profile.html?isin=IE00BDQYWQ65" xr:uid="{6C04B138-97D3-42C8-B6E1-00870CCBE0B4}"/>
+    <hyperlink ref="A3" r:id="rId6" display="https://www.justetf.com/it/etf-profile.html?isin=IE00BD1F4L37" xr:uid="{DF84D7C7-B8F6-477A-8C9A-D4997B54C865}"/>
+    <hyperlink ref="A4" r:id="rId7" display="https://www.justetf.com/it/etf-profile.html?isin=IE00B8FHGS14" xr:uid="{47A684AB-EAC0-4609-B6F5-2C135D16A87D}"/>
+    <hyperlink ref="A6" r:id="rId8" display="https://www.justetf.com/it/etf-profile.html?isin=IE0032523478" xr:uid="{20C7AF50-87F2-4FC4-B8A4-93B98529FB55}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3223,16 +3225,16 @@
     </row>
     <row r="10" spans="1:12">
       <c r="B10" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="C10" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="D10" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="E10" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="F10" t="s">
         <v>11</v>
@@ -3252,16 +3254,16 @@
     </row>
     <row r="11" spans="1:12" ht="14.7" customHeight="1">
       <c r="B11" t="s">
-        <v>199</v>
-      </c>
-      <c r="C11" s="101" t="s">
-        <v>196</v>
+        <v>195</v>
+      </c>
+      <c r="C11" s="37" t="s">
+        <v>192</v>
       </c>
       <c r="D11" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="E11" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="F11" t="s">
         <v>11</v>
@@ -3281,16 +3283,16 @@
     </row>
     <row r="12" spans="1:12">
       <c r="B12" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="C12" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="D12" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="E12" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="F12" t="s">
         <v>11</v>
@@ -3310,19 +3312,19 @@
     </row>
     <row r="13" spans="1:12">
       <c r="A13" s="36" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="B13" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="C13" t="s">
+        <v>158</v>
+      </c>
+      <c r="D13" t="s">
+        <v>159</v>
+      </c>
+      <c r="E13" t="s">
         <v>160</v>
-      </c>
-      <c r="D13" t="s">
-        <v>161</v>
-      </c>
-      <c r="E13" t="s">
-        <v>162</v>
       </c>
       <c r="F13" t="s">
         <v>11</v>
@@ -3331,7 +3333,7 @@
         <v>7</v>
       </c>
       <c r="H13" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="I13" s="1">
         <v>2.5000000000000001E-3</v>
@@ -3342,19 +3344,19 @@
     </row>
     <row r="14" spans="1:12">
       <c r="A14" s="36" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="B14" t="s">
         <v>153</v>
       </c>
       <c r="C14" t="s">
+        <v>156</v>
+      </c>
+      <c r="D14" t="s">
+        <v>188</v>
+      </c>
+      <c r="E14" t="s">
         <v>157</v>
-      </c>
-      <c r="D14" t="s">
-        <v>192</v>
-      </c>
-      <c r="E14" t="s">
-        <v>158</v>
       </c>
       <c r="F14" t="s">
         <v>11</v>
@@ -3363,7 +3365,7 @@
         <v>7</v>
       </c>
       <c r="H14" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="I14" s="1">
         <v>3.5000000000000001E-3</v>
@@ -3425,18 +3427,18 @@
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="str">
-        <v>WHEA.L</v>
+        <v>IBGM.AS</v>
       </c>
       <c r="B5" t="str">
-        <v>World Healthcare</v>
+        <v>EU Gov bonds 7-10y</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="str">
-        <v>IBGM.AS</v>
+        <v>IBCX.AS</v>
       </c>
       <c r="B6" t="str">
-        <v>EU Gov bonds 7-10y</v>
+        <v>EU Corp Large Cap bonds</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -3501,12 +3503,12 @@
     </row>
     <row r="5" spans="1:1">
       <c r="A5" t="str">
-        <v>SPDR MSCI World Health Care UCITS ETF</v>
+        <v>iShares € Govt Bond 7-10yr UCITS ETF EUR (Dist)</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" t="str">
-        <v>iShares € Govt Bond 7-10yr UCITS ETF EUR (Dist)</v>
+        <v>iShares Euro Corporate Bond Large Cap UCITS ETF</v>
       </c>
     </row>
     <row r="7" spans="1:1">
@@ -3549,118 +3551,118 @@
     </row>
     <row r="3" spans="1:18" ht="14.7" thickBot="1"/>
     <row r="4" spans="1:18" ht="16" customHeight="1">
-      <c r="B4" s="37" t="s">
+      <c r="B4" s="60" t="s">
         <v>97</v>
       </c>
-      <c r="C4" s="38"/>
-      <c r="D4" s="38"/>
-      <c r="E4" s="38"/>
-      <c r="F4" s="39"/>
-      <c r="H4" s="43" t="s">
+      <c r="C4" s="61"/>
+      <c r="D4" s="61"/>
+      <c r="E4" s="61"/>
+      <c r="F4" s="62"/>
+      <c r="H4" s="96" t="s">
         <v>98</v>
       </c>
-      <c r="I4" s="44"/>
-      <c r="J4" s="44"/>
-      <c r="K4" s="44"/>
-      <c r="L4" s="45"/>
-      <c r="N4" s="49" t="s">
+      <c r="I4" s="97"/>
+      <c r="J4" s="97"/>
+      <c r="K4" s="97"/>
+      <c r="L4" s="98"/>
+      <c r="N4" s="72" t="s">
         <v>99</v>
       </c>
-      <c r="O4" s="50"/>
-      <c r="P4" s="50"/>
-      <c r="Q4" s="50"/>
-      <c r="R4" s="51"/>
+      <c r="O4" s="73"/>
+      <c r="P4" s="73"/>
+      <c r="Q4" s="73"/>
+      <c r="R4" s="74"/>
     </row>
     <row r="5" spans="1:18" ht="17.100000000000001" customHeight="1" thickBot="1">
-      <c r="B5" s="40"/>
-      <c r="C5" s="41"/>
-      <c r="D5" s="41"/>
-      <c r="E5" s="41"/>
-      <c r="F5" s="42"/>
-      <c r="H5" s="46"/>
-      <c r="I5" s="47"/>
-      <c r="J5" s="47"/>
-      <c r="K5" s="47"/>
-      <c r="L5" s="48"/>
-      <c r="N5" s="52"/>
-      <c r="O5" s="53"/>
-      <c r="P5" s="53"/>
-      <c r="Q5" s="53"/>
-      <c r="R5" s="54"/>
+      <c r="B5" s="63"/>
+      <c r="C5" s="64"/>
+      <c r="D5" s="64"/>
+      <c r="E5" s="64"/>
+      <c r="F5" s="65"/>
+      <c r="H5" s="99"/>
+      <c r="I5" s="100"/>
+      <c r="J5" s="100"/>
+      <c r="K5" s="100"/>
+      <c r="L5" s="101"/>
+      <c r="N5" s="75"/>
+      <c r="O5" s="76"/>
+      <c r="P5" s="76"/>
+      <c r="Q5" s="76"/>
+      <c r="R5" s="77"/>
     </row>
     <row r="6" spans="1:18">
-      <c r="B6" s="55" t="s">
+      <c r="B6" s="51" t="s">
         <v>100</v>
       </c>
-      <c r="C6" s="56"/>
-      <c r="D6" s="56"/>
-      <c r="E6" s="56"/>
-      <c r="F6" s="57"/>
-      <c r="H6" s="55" t="s">
+      <c r="C6" s="52"/>
+      <c r="D6" s="52"/>
+      <c r="E6" s="52"/>
+      <c r="F6" s="53"/>
+      <c r="H6" s="51" t="s">
         <v>101</v>
       </c>
-      <c r="I6" s="56"/>
-      <c r="J6" s="56"/>
-      <c r="K6" s="56"/>
-      <c r="L6" s="57"/>
-      <c r="N6" s="55" t="s">
+      <c r="I6" s="52"/>
+      <c r="J6" s="52"/>
+      <c r="K6" s="52"/>
+      <c r="L6" s="53"/>
+      <c r="N6" s="51" t="s">
         <v>101</v>
       </c>
-      <c r="O6" s="56"/>
-      <c r="P6" s="56"/>
-      <c r="Q6" s="56"/>
-      <c r="R6" s="57"/>
+      <c r="O6" s="52"/>
+      <c r="P6" s="52"/>
+      <c r="Q6" s="52"/>
+      <c r="R6" s="53"/>
     </row>
     <row r="7" spans="1:18">
-      <c r="B7" s="58"/>
-      <c r="C7" s="59"/>
-      <c r="D7" s="59"/>
-      <c r="E7" s="59"/>
-      <c r="F7" s="60"/>
-      <c r="H7" s="58"/>
-      <c r="I7" s="59"/>
-      <c r="J7" s="59"/>
-      <c r="K7" s="59"/>
-      <c r="L7" s="60"/>
-      <c r="N7" s="58"/>
-      <c r="O7" s="59"/>
-      <c r="P7" s="59"/>
-      <c r="Q7" s="59"/>
-      <c r="R7" s="60"/>
+      <c r="B7" s="54"/>
+      <c r="C7" s="55"/>
+      <c r="D7" s="55"/>
+      <c r="E7" s="55"/>
+      <c r="F7" s="56"/>
+      <c r="H7" s="54"/>
+      <c r="I7" s="55"/>
+      <c r="J7" s="55"/>
+      <c r="K7" s="55"/>
+      <c r="L7" s="56"/>
+      <c r="N7" s="54"/>
+      <c r="O7" s="55"/>
+      <c r="P7" s="55"/>
+      <c r="Q7" s="55"/>
+      <c r="R7" s="56"/>
     </row>
     <row r="8" spans="1:18">
-      <c r="B8" s="58"/>
-      <c r="C8" s="59"/>
-      <c r="D8" s="59"/>
-      <c r="E8" s="59"/>
-      <c r="F8" s="60"/>
-      <c r="H8" s="58"/>
-      <c r="I8" s="59"/>
-      <c r="J8" s="59"/>
-      <c r="K8" s="59"/>
-      <c r="L8" s="60"/>
-      <c r="N8" s="58"/>
-      <c r="O8" s="59"/>
-      <c r="P8" s="59"/>
-      <c r="Q8" s="59"/>
-      <c r="R8" s="60"/>
+      <c r="B8" s="54"/>
+      <c r="C8" s="55"/>
+      <c r="D8" s="55"/>
+      <c r="E8" s="55"/>
+      <c r="F8" s="56"/>
+      <c r="H8" s="54"/>
+      <c r="I8" s="55"/>
+      <c r="J8" s="55"/>
+      <c r="K8" s="55"/>
+      <c r="L8" s="56"/>
+      <c r="N8" s="54"/>
+      <c r="O8" s="55"/>
+      <c r="P8" s="55"/>
+      <c r="Q8" s="55"/>
+      <c r="R8" s="56"/>
     </row>
     <row r="9" spans="1:18">
-      <c r="B9" s="61"/>
-      <c r="C9" s="62"/>
-      <c r="D9" s="62"/>
-      <c r="E9" s="62"/>
-      <c r="F9" s="63"/>
-      <c r="H9" s="61"/>
-      <c r="I9" s="62"/>
-      <c r="J9" s="62"/>
-      <c r="K9" s="62"/>
-      <c r="L9" s="63"/>
-      <c r="N9" s="61"/>
-      <c r="O9" s="62"/>
-      <c r="P9" s="62"/>
-      <c r="Q9" s="62"/>
-      <c r="R9" s="63"/>
+      <c r="B9" s="57"/>
+      <c r="C9" s="58"/>
+      <c r="D9" s="58"/>
+      <c r="E9" s="58"/>
+      <c r="F9" s="59"/>
+      <c r="H9" s="57"/>
+      <c r="I9" s="58"/>
+      <c r="J9" s="58"/>
+      <c r="K9" s="58"/>
+      <c r="L9" s="59"/>
+      <c r="N9" s="57"/>
+      <c r="O9" s="58"/>
+      <c r="P9" s="58"/>
+      <c r="Q9" s="58"/>
+      <c r="R9" s="59"/>
     </row>
     <row r="10" spans="1:18">
       <c r="B10" s="5"/>
@@ -3681,226 +3683,226 @@
     </row>
     <row r="11" spans="1:18" ht="14.7" thickBot="1"/>
     <row r="12" spans="1:18" ht="16" customHeight="1">
-      <c r="B12" s="37" t="s">
+      <c r="B12" s="60" t="s">
         <v>102</v>
       </c>
-      <c r="C12" s="38"/>
-      <c r="D12" s="38"/>
-      <c r="E12" s="38"/>
-      <c r="F12" s="39"/>
-      <c r="H12" s="64" t="s">
+      <c r="C12" s="61"/>
+      <c r="D12" s="61"/>
+      <c r="E12" s="61"/>
+      <c r="F12" s="62"/>
+      <c r="H12" s="84" t="s">
         <v>102</v>
       </c>
-      <c r="I12" s="65"/>
-      <c r="J12" s="65"/>
-      <c r="K12" s="65"/>
-      <c r="L12" s="66"/>
-      <c r="N12" s="70" t="s">
+      <c r="I12" s="85"/>
+      <c r="J12" s="85"/>
+      <c r="K12" s="85"/>
+      <c r="L12" s="86"/>
+      <c r="N12" s="90" t="s">
         <v>102</v>
       </c>
-      <c r="O12" s="71"/>
-      <c r="P12" s="71"/>
-      <c r="Q12" s="71"/>
-      <c r="R12" s="72"/>
+      <c r="O12" s="91"/>
+      <c r="P12" s="91"/>
+      <c r="Q12" s="91"/>
+      <c r="R12" s="92"/>
     </row>
     <row r="13" spans="1:18" ht="16" customHeight="1">
-      <c r="B13" s="40"/>
-      <c r="C13" s="41"/>
-      <c r="D13" s="41"/>
-      <c r="E13" s="41"/>
-      <c r="F13" s="42"/>
-      <c r="H13" s="67"/>
-      <c r="I13" s="68"/>
-      <c r="J13" s="68"/>
-      <c r="K13" s="68"/>
-      <c r="L13" s="69"/>
-      <c r="N13" s="73"/>
-      <c r="O13" s="74"/>
-      <c r="P13" s="74"/>
-      <c r="Q13" s="74"/>
-      <c r="R13" s="75"/>
+      <c r="B13" s="63"/>
+      <c r="C13" s="64"/>
+      <c r="D13" s="64"/>
+      <c r="E13" s="64"/>
+      <c r="F13" s="65"/>
+      <c r="H13" s="87"/>
+      <c r="I13" s="88"/>
+      <c r="J13" s="88"/>
+      <c r="K13" s="88"/>
+      <c r="L13" s="89"/>
+      <c r="N13" s="93"/>
+      <c r="O13" s="94"/>
+      <c r="P13" s="94"/>
+      <c r="Q13" s="94"/>
+      <c r="R13" s="95"/>
     </row>
     <row r="14" spans="1:18" ht="16" customHeight="1">
-      <c r="B14" s="76" t="s">
+      <c r="B14" s="41" t="s">
         <v>103</v>
       </c>
-      <c r="C14" s="77"/>
-      <c r="D14" s="77"/>
-      <c r="E14" s="77"/>
-      <c r="F14" s="78"/>
-      <c r="H14" s="76" t="s">
+      <c r="C14" s="42"/>
+      <c r="D14" s="42"/>
+      <c r="E14" s="42"/>
+      <c r="F14" s="43"/>
+      <c r="H14" s="41" t="s">
         <v>104</v>
       </c>
-      <c r="I14" s="77"/>
-      <c r="J14" s="77"/>
-      <c r="K14" s="77"/>
-      <c r="L14" s="78"/>
-      <c r="N14" s="76" t="s">
+      <c r="I14" s="42"/>
+      <c r="J14" s="42"/>
+      <c r="K14" s="42"/>
+      <c r="L14" s="43"/>
+      <c r="N14" s="41" t="s">
         <v>105</v>
       </c>
-      <c r="O14" s="77"/>
-      <c r="P14" s="77"/>
-      <c r="Q14" s="77"/>
-      <c r="R14" s="78"/>
+      <c r="O14" s="42"/>
+      <c r="P14" s="42"/>
+      <c r="Q14" s="42"/>
+      <c r="R14" s="43"/>
     </row>
     <row r="15" spans="1:18">
-      <c r="B15" s="79"/>
-      <c r="C15" s="80"/>
-      <c r="D15" s="80"/>
-      <c r="E15" s="80"/>
-      <c r="F15" s="81"/>
-      <c r="H15" s="79"/>
-      <c r="I15" s="80"/>
-      <c r="J15" s="80"/>
-      <c r="K15" s="80"/>
-      <c r="L15" s="81"/>
-      <c r="N15" s="79"/>
-      <c r="O15" s="80"/>
-      <c r="P15" s="80"/>
-      <c r="Q15" s="80"/>
-      <c r="R15" s="81"/>
+      <c r="B15" s="44"/>
+      <c r="C15" s="45"/>
+      <c r="D15" s="45"/>
+      <c r="E15" s="45"/>
+      <c r="F15" s="46"/>
+      <c r="H15" s="44"/>
+      <c r="I15" s="45"/>
+      <c r="J15" s="45"/>
+      <c r="K15" s="45"/>
+      <c r="L15" s="46"/>
+      <c r="N15" s="44"/>
+      <c r="O15" s="45"/>
+      <c r="P15" s="45"/>
+      <c r="Q15" s="45"/>
+      <c r="R15" s="46"/>
     </row>
     <row r="16" spans="1:18">
-      <c r="B16" s="79"/>
-      <c r="C16" s="80"/>
-      <c r="D16" s="80"/>
-      <c r="E16" s="80"/>
-      <c r="F16" s="81"/>
-      <c r="H16" s="79"/>
-      <c r="I16" s="80"/>
-      <c r="J16" s="80"/>
-      <c r="K16" s="80"/>
-      <c r="L16" s="81"/>
-      <c r="N16" s="79"/>
-      <c r="O16" s="80"/>
-      <c r="P16" s="80"/>
-      <c r="Q16" s="80"/>
-      <c r="R16" s="81"/>
+      <c r="B16" s="44"/>
+      <c r="C16" s="45"/>
+      <c r="D16" s="45"/>
+      <c r="E16" s="45"/>
+      <c r="F16" s="46"/>
+      <c r="H16" s="44"/>
+      <c r="I16" s="45"/>
+      <c r="J16" s="45"/>
+      <c r="K16" s="45"/>
+      <c r="L16" s="46"/>
+      <c r="N16" s="44"/>
+      <c r="O16" s="45"/>
+      <c r="P16" s="45"/>
+      <c r="Q16" s="45"/>
+      <c r="R16" s="46"/>
     </row>
     <row r="17" spans="2:18">
-      <c r="B17" s="79"/>
-      <c r="C17" s="80"/>
-      <c r="D17" s="80"/>
-      <c r="E17" s="80"/>
-      <c r="F17" s="81"/>
-      <c r="H17" s="79"/>
-      <c r="I17" s="80"/>
-      <c r="J17" s="80"/>
-      <c r="K17" s="80"/>
-      <c r="L17" s="81"/>
-      <c r="N17" s="79"/>
-      <c r="O17" s="80"/>
-      <c r="P17" s="80"/>
-      <c r="Q17" s="80"/>
-      <c r="R17" s="81"/>
+      <c r="B17" s="44"/>
+      <c r="C17" s="45"/>
+      <c r="D17" s="45"/>
+      <c r="E17" s="45"/>
+      <c r="F17" s="46"/>
+      <c r="H17" s="44"/>
+      <c r="I17" s="45"/>
+      <c r="J17" s="45"/>
+      <c r="K17" s="45"/>
+      <c r="L17" s="46"/>
+      <c r="N17" s="44"/>
+      <c r="O17" s="45"/>
+      <c r="P17" s="45"/>
+      <c r="Q17" s="45"/>
+      <c r="R17" s="46"/>
     </row>
     <row r="18" spans="2:18">
-      <c r="B18" s="82"/>
-      <c r="C18" s="83"/>
-      <c r="D18" s="83"/>
-      <c r="E18" s="83"/>
-      <c r="F18" s="84"/>
-      <c r="H18" s="82"/>
-      <c r="I18" s="83"/>
-      <c r="J18" s="83"/>
-      <c r="K18" s="83"/>
-      <c r="L18" s="84"/>
-      <c r="N18" s="82"/>
-      <c r="O18" s="83"/>
-      <c r="P18" s="83"/>
-      <c r="Q18" s="83"/>
-      <c r="R18" s="84"/>
+      <c r="B18" s="47"/>
+      <c r="C18" s="48"/>
+      <c r="D18" s="48"/>
+      <c r="E18" s="48"/>
+      <c r="F18" s="49"/>
+      <c r="H18" s="47"/>
+      <c r="I18" s="48"/>
+      <c r="J18" s="48"/>
+      <c r="K18" s="48"/>
+      <c r="L18" s="49"/>
+      <c r="N18" s="47"/>
+      <c r="O18" s="48"/>
+      <c r="P18" s="48"/>
+      <c r="Q18" s="48"/>
+      <c r="R18" s="49"/>
     </row>
     <row r="19" spans="2:18" ht="16" customHeight="1">
-      <c r="B19" s="76" t="s">
+      <c r="B19" s="41" t="s">
         <v>106</v>
       </c>
-      <c r="C19" s="77"/>
-      <c r="D19" s="77"/>
-      <c r="E19" s="77"/>
-      <c r="F19" s="78"/>
-      <c r="H19" s="76" t="s">
+      <c r="C19" s="42"/>
+      <c r="D19" s="42"/>
+      <c r="E19" s="42"/>
+      <c r="F19" s="43"/>
+      <c r="H19" s="41" t="s">
         <v>106</v>
       </c>
-      <c r="I19" s="77"/>
-      <c r="J19" s="77"/>
-      <c r="K19" s="77"/>
-      <c r="L19" s="78"/>
-      <c r="N19" s="76" t="s">
+      <c r="I19" s="42"/>
+      <c r="J19" s="42"/>
+      <c r="K19" s="42"/>
+      <c r="L19" s="43"/>
+      <c r="N19" s="41" t="s">
         <v>107</v>
       </c>
-      <c r="O19" s="77"/>
-      <c r="P19" s="77"/>
-      <c r="Q19" s="77"/>
-      <c r="R19" s="78"/>
+      <c r="O19" s="42"/>
+      <c r="P19" s="42"/>
+      <c r="Q19" s="42"/>
+      <c r="R19" s="43"/>
     </row>
     <row r="20" spans="2:18">
-      <c r="B20" s="79"/>
-      <c r="C20" s="80"/>
-      <c r="D20" s="80"/>
-      <c r="E20" s="80"/>
-      <c r="F20" s="81"/>
-      <c r="H20" s="79"/>
-      <c r="I20" s="80"/>
-      <c r="J20" s="80"/>
-      <c r="K20" s="80"/>
-      <c r="L20" s="81"/>
-      <c r="N20" s="79"/>
-      <c r="O20" s="80"/>
-      <c r="P20" s="80"/>
-      <c r="Q20" s="80"/>
-      <c r="R20" s="81"/>
+      <c r="B20" s="44"/>
+      <c r="C20" s="45"/>
+      <c r="D20" s="45"/>
+      <c r="E20" s="45"/>
+      <c r="F20" s="46"/>
+      <c r="H20" s="44"/>
+      <c r="I20" s="45"/>
+      <c r="J20" s="45"/>
+      <c r="K20" s="45"/>
+      <c r="L20" s="46"/>
+      <c r="N20" s="44"/>
+      <c r="O20" s="45"/>
+      <c r="P20" s="45"/>
+      <c r="Q20" s="45"/>
+      <c r="R20" s="46"/>
     </row>
     <row r="21" spans="2:18">
-      <c r="B21" s="79"/>
-      <c r="C21" s="80"/>
-      <c r="D21" s="80"/>
-      <c r="E21" s="80"/>
-      <c r="F21" s="81"/>
-      <c r="H21" s="79"/>
-      <c r="I21" s="80"/>
-      <c r="J21" s="80"/>
-      <c r="K21" s="80"/>
-      <c r="L21" s="81"/>
-      <c r="N21" s="79"/>
-      <c r="O21" s="80"/>
-      <c r="P21" s="80"/>
-      <c r="Q21" s="80"/>
-      <c r="R21" s="81"/>
+      <c r="B21" s="44"/>
+      <c r="C21" s="45"/>
+      <c r="D21" s="45"/>
+      <c r="E21" s="45"/>
+      <c r="F21" s="46"/>
+      <c r="H21" s="44"/>
+      <c r="I21" s="45"/>
+      <c r="J21" s="45"/>
+      <c r="K21" s="45"/>
+      <c r="L21" s="46"/>
+      <c r="N21" s="44"/>
+      <c r="O21" s="45"/>
+      <c r="P21" s="45"/>
+      <c r="Q21" s="45"/>
+      <c r="R21" s="46"/>
     </row>
     <row r="22" spans="2:18">
-      <c r="B22" s="79"/>
-      <c r="C22" s="80"/>
-      <c r="D22" s="80"/>
-      <c r="E22" s="80"/>
-      <c r="F22" s="81"/>
-      <c r="H22" s="79"/>
-      <c r="I22" s="80"/>
-      <c r="J22" s="80"/>
-      <c r="K22" s="80"/>
-      <c r="L22" s="81"/>
-      <c r="N22" s="79"/>
-      <c r="O22" s="80"/>
-      <c r="P22" s="80"/>
-      <c r="Q22" s="80"/>
-      <c r="R22" s="81"/>
+      <c r="B22" s="44"/>
+      <c r="C22" s="45"/>
+      <c r="D22" s="45"/>
+      <c r="E22" s="45"/>
+      <c r="F22" s="46"/>
+      <c r="H22" s="44"/>
+      <c r="I22" s="45"/>
+      <c r="J22" s="45"/>
+      <c r="K22" s="45"/>
+      <c r="L22" s="46"/>
+      <c r="N22" s="44"/>
+      <c r="O22" s="45"/>
+      <c r="P22" s="45"/>
+      <c r="Q22" s="45"/>
+      <c r="R22" s="46"/>
     </row>
     <row r="23" spans="2:18">
-      <c r="B23" s="82"/>
-      <c r="C23" s="83"/>
-      <c r="D23" s="83"/>
-      <c r="E23" s="83"/>
-      <c r="F23" s="84"/>
-      <c r="H23" s="82"/>
-      <c r="I23" s="83"/>
-      <c r="J23" s="83"/>
-      <c r="K23" s="83"/>
-      <c r="L23" s="84"/>
-      <c r="N23" s="82"/>
-      <c r="O23" s="83"/>
-      <c r="P23" s="83"/>
-      <c r="Q23" s="83"/>
-      <c r="R23" s="84"/>
+      <c r="B23" s="47"/>
+      <c r="C23" s="48"/>
+      <c r="D23" s="48"/>
+      <c r="E23" s="48"/>
+      <c r="F23" s="49"/>
+      <c r="H23" s="47"/>
+      <c r="I23" s="48"/>
+      <c r="J23" s="48"/>
+      <c r="K23" s="48"/>
+      <c r="L23" s="49"/>
+      <c r="N23" s="47"/>
+      <c r="O23" s="48"/>
+      <c r="P23" s="48"/>
+      <c r="Q23" s="48"/>
+      <c r="R23" s="49"/>
     </row>
     <row r="26" spans="2:18" ht="18.3">
       <c r="B26" s="6" t="s">
@@ -4066,341 +4068,341 @@
     </row>
     <row r="37" spans="2:18" ht="14.7" thickBot="1"/>
     <row r="38" spans="2:18">
-      <c r="B38" s="37" t="s">
+      <c r="B38" s="60" t="s">
         <v>117</v>
       </c>
-      <c r="C38" s="38"/>
-      <c r="D38" s="38"/>
-      <c r="E38" s="38"/>
-      <c r="F38" s="39"/>
-      <c r="H38" s="85" t="s">
+      <c r="C38" s="61"/>
+      <c r="D38" s="61"/>
+      <c r="E38" s="61"/>
+      <c r="F38" s="62"/>
+      <c r="H38" s="78" t="s">
         <v>118</v>
       </c>
-      <c r="I38" s="86"/>
-      <c r="J38" s="86"/>
-      <c r="K38" s="86"/>
-      <c r="L38" s="87"/>
-      <c r="N38" s="49" t="s">
+      <c r="I38" s="79"/>
+      <c r="J38" s="79"/>
+      <c r="K38" s="79"/>
+      <c r="L38" s="80"/>
+      <c r="N38" s="72" t="s">
         <v>119</v>
       </c>
-      <c r="O38" s="50"/>
-      <c r="P38" s="50"/>
-      <c r="Q38" s="50"/>
-      <c r="R38" s="51"/>
+      <c r="O38" s="73"/>
+      <c r="P38" s="73"/>
+      <c r="Q38" s="73"/>
+      <c r="R38" s="74"/>
     </row>
     <row r="39" spans="2:18" ht="14.7" thickBot="1">
-      <c r="B39" s="40"/>
-      <c r="C39" s="41"/>
-      <c r="D39" s="41"/>
-      <c r="E39" s="41"/>
-      <c r="F39" s="42"/>
-      <c r="H39" s="88"/>
-      <c r="I39" s="89"/>
-      <c r="J39" s="89"/>
-      <c r="K39" s="89"/>
-      <c r="L39" s="90"/>
-      <c r="N39" s="52"/>
-      <c r="O39" s="53"/>
-      <c r="P39" s="53"/>
-      <c r="Q39" s="53"/>
-      <c r="R39" s="54"/>
+      <c r="B39" s="63"/>
+      <c r="C39" s="64"/>
+      <c r="D39" s="64"/>
+      <c r="E39" s="64"/>
+      <c r="F39" s="65"/>
+      <c r="H39" s="81"/>
+      <c r="I39" s="82"/>
+      <c r="J39" s="82"/>
+      <c r="K39" s="82"/>
+      <c r="L39" s="83"/>
+      <c r="N39" s="75"/>
+      <c r="O39" s="76"/>
+      <c r="P39" s="76"/>
+      <c r="Q39" s="76"/>
+      <c r="R39" s="77"/>
     </row>
     <row r="40" spans="2:18">
-      <c r="B40" s="55" t="s">
+      <c r="B40" s="51" t="s">
         <v>120</v>
       </c>
-      <c r="C40" s="56"/>
-      <c r="D40" s="56"/>
-      <c r="E40" s="56"/>
-      <c r="F40" s="57"/>
-      <c r="H40" s="55" t="s">
+      <c r="C40" s="52"/>
+      <c r="D40" s="52"/>
+      <c r="E40" s="52"/>
+      <c r="F40" s="53"/>
+      <c r="H40" s="51" t="s">
         <v>121</v>
       </c>
-      <c r="I40" s="56"/>
-      <c r="J40" s="56"/>
-      <c r="K40" s="56"/>
-      <c r="L40" s="57"/>
-      <c r="N40" s="55" t="s">
+      <c r="I40" s="52"/>
+      <c r="J40" s="52"/>
+      <c r="K40" s="52"/>
+      <c r="L40" s="53"/>
+      <c r="N40" s="51" t="s">
         <v>122</v>
       </c>
-      <c r="O40" s="56"/>
-      <c r="P40" s="56"/>
-      <c r="Q40" s="56"/>
-      <c r="R40" s="57"/>
+      <c r="O40" s="52"/>
+      <c r="P40" s="52"/>
+      <c r="Q40" s="52"/>
+      <c r="R40" s="53"/>
     </row>
     <row r="41" spans="2:18">
-      <c r="B41" s="58"/>
-      <c r="C41" s="59"/>
-      <c r="D41" s="59"/>
-      <c r="E41" s="59"/>
-      <c r="F41" s="60"/>
-      <c r="H41" s="58"/>
-      <c r="I41" s="59"/>
-      <c r="J41" s="59"/>
-      <c r="K41" s="59"/>
-      <c r="L41" s="60"/>
-      <c r="N41" s="58"/>
-      <c r="O41" s="59"/>
-      <c r="P41" s="59"/>
-      <c r="Q41" s="59"/>
-      <c r="R41" s="60"/>
+      <c r="B41" s="54"/>
+      <c r="C41" s="55"/>
+      <c r="D41" s="55"/>
+      <c r="E41" s="55"/>
+      <c r="F41" s="56"/>
+      <c r="H41" s="54"/>
+      <c r="I41" s="55"/>
+      <c r="J41" s="55"/>
+      <c r="K41" s="55"/>
+      <c r="L41" s="56"/>
+      <c r="N41" s="54"/>
+      <c r="O41" s="55"/>
+      <c r="P41" s="55"/>
+      <c r="Q41" s="55"/>
+      <c r="R41" s="56"/>
     </row>
     <row r="42" spans="2:18">
-      <c r="B42" s="58"/>
-      <c r="C42" s="59"/>
-      <c r="D42" s="59"/>
-      <c r="E42" s="59"/>
-      <c r="F42" s="60"/>
-      <c r="H42" s="58"/>
-      <c r="I42" s="59"/>
-      <c r="J42" s="59"/>
-      <c r="K42" s="59"/>
-      <c r="L42" s="60"/>
-      <c r="N42" s="58"/>
-      <c r="O42" s="59"/>
-      <c r="P42" s="59"/>
-      <c r="Q42" s="59"/>
-      <c r="R42" s="60"/>
+      <c r="B42" s="54"/>
+      <c r="C42" s="55"/>
+      <c r="D42" s="55"/>
+      <c r="E42" s="55"/>
+      <c r="F42" s="56"/>
+      <c r="H42" s="54"/>
+      <c r="I42" s="55"/>
+      <c r="J42" s="55"/>
+      <c r="K42" s="55"/>
+      <c r="L42" s="56"/>
+      <c r="N42" s="54"/>
+      <c r="O42" s="55"/>
+      <c r="P42" s="55"/>
+      <c r="Q42" s="55"/>
+      <c r="R42" s="56"/>
     </row>
     <row r="43" spans="2:18">
-      <c r="B43" s="61"/>
-      <c r="C43" s="62"/>
-      <c r="D43" s="62"/>
-      <c r="E43" s="62"/>
-      <c r="F43" s="63"/>
-      <c r="H43" s="61"/>
-      <c r="I43" s="62"/>
-      <c r="J43" s="62"/>
-      <c r="K43" s="62"/>
-      <c r="L43" s="63"/>
-      <c r="N43" s="61"/>
-      <c r="O43" s="62"/>
-      <c r="P43" s="62"/>
-      <c r="Q43" s="62"/>
-      <c r="R43" s="63"/>
+      <c r="B43" s="57"/>
+      <c r="C43" s="58"/>
+      <c r="D43" s="58"/>
+      <c r="E43" s="58"/>
+      <c r="F43" s="59"/>
+      <c r="H43" s="57"/>
+      <c r="I43" s="58"/>
+      <c r="J43" s="58"/>
+      <c r="K43" s="58"/>
+      <c r="L43" s="59"/>
+      <c r="N43" s="57"/>
+      <c r="O43" s="58"/>
+      <c r="P43" s="58"/>
+      <c r="Q43" s="58"/>
+      <c r="R43" s="59"/>
     </row>
     <row r="45" spans="2:18" ht="14.7" thickBot="1"/>
     <row r="46" spans="2:18" ht="16" customHeight="1">
-      <c r="B46" s="37" t="s">
+      <c r="B46" s="60" t="s">
         <v>102</v>
       </c>
-      <c r="C46" s="38"/>
-      <c r="D46" s="38"/>
-      <c r="E46" s="38"/>
-      <c r="F46" s="39"/>
-      <c r="H46" s="91" t="s">
+      <c r="C46" s="61"/>
+      <c r="D46" s="61"/>
+      <c r="E46" s="61"/>
+      <c r="F46" s="62"/>
+      <c r="H46" s="66" t="s">
         <v>102</v>
       </c>
-      <c r="I46" s="92"/>
-      <c r="J46" s="92"/>
-      <c r="K46" s="92"/>
-      <c r="L46" s="93"/>
-      <c r="N46" s="49" t="s">
+      <c r="I46" s="67"/>
+      <c r="J46" s="67"/>
+      <c r="K46" s="67"/>
+      <c r="L46" s="68"/>
+      <c r="N46" s="72" t="s">
         <v>102</v>
       </c>
-      <c r="O46" s="50"/>
-      <c r="P46" s="50"/>
-      <c r="Q46" s="50"/>
-      <c r="R46" s="51"/>
+      <c r="O46" s="73"/>
+      <c r="P46" s="73"/>
+      <c r="Q46" s="73"/>
+      <c r="R46" s="74"/>
     </row>
     <row r="47" spans="2:18" ht="16" customHeight="1" thickBot="1">
-      <c r="B47" s="40"/>
-      <c r="C47" s="41"/>
-      <c r="D47" s="41"/>
-      <c r="E47" s="41"/>
-      <c r="F47" s="42"/>
-      <c r="H47" s="94"/>
-      <c r="I47" s="95"/>
-      <c r="J47" s="95"/>
-      <c r="K47" s="95"/>
-      <c r="L47" s="96"/>
-      <c r="N47" s="52"/>
-      <c r="O47" s="53"/>
-      <c r="P47" s="53"/>
-      <c r="Q47" s="53"/>
-      <c r="R47" s="54"/>
+      <c r="B47" s="63"/>
+      <c r="C47" s="64"/>
+      <c r="D47" s="64"/>
+      <c r="E47" s="64"/>
+      <c r="F47" s="65"/>
+      <c r="H47" s="69"/>
+      <c r="I47" s="70"/>
+      <c r="J47" s="70"/>
+      <c r="K47" s="70"/>
+      <c r="L47" s="71"/>
+      <c r="N47" s="75"/>
+      <c r="O47" s="76"/>
+      <c r="P47" s="76"/>
+      <c r="Q47" s="76"/>
+      <c r="R47" s="77"/>
     </row>
     <row r="48" spans="2:18">
-      <c r="B48" s="76" t="s">
+      <c r="B48" s="41" t="s">
         <v>123</v>
       </c>
-      <c r="C48" s="77"/>
-      <c r="D48" s="77"/>
-      <c r="E48" s="77"/>
-      <c r="F48" s="78"/>
-      <c r="H48" s="100" t="s">
+      <c r="C48" s="42"/>
+      <c r="D48" s="42"/>
+      <c r="E48" s="42"/>
+      <c r="F48" s="43"/>
+      <c r="H48" s="50" t="s">
         <v>124</v>
       </c>
-      <c r="I48" s="77"/>
-      <c r="J48" s="77"/>
-      <c r="K48" s="77"/>
-      <c r="L48" s="78"/>
-      <c r="N48" s="76" t="s">
+      <c r="I48" s="42"/>
+      <c r="J48" s="42"/>
+      <c r="K48" s="42"/>
+      <c r="L48" s="43"/>
+      <c r="N48" s="41" t="s">
         <v>125</v>
       </c>
-      <c r="O48" s="77"/>
-      <c r="P48" s="77"/>
-      <c r="Q48" s="77"/>
-      <c r="R48" s="78"/>
+      <c r="O48" s="42"/>
+      <c r="P48" s="42"/>
+      <c r="Q48" s="42"/>
+      <c r="R48" s="43"/>
     </row>
     <row r="49" spans="2:18">
-      <c r="B49" s="79"/>
-      <c r="C49" s="80"/>
-      <c r="D49" s="80"/>
-      <c r="E49" s="80"/>
-      <c r="F49" s="81"/>
-      <c r="H49" s="79"/>
-      <c r="I49" s="80"/>
-      <c r="J49" s="80"/>
-      <c r="K49" s="80"/>
-      <c r="L49" s="81"/>
-      <c r="N49" s="79"/>
-      <c r="O49" s="80"/>
-      <c r="P49" s="80"/>
-      <c r="Q49" s="80"/>
-      <c r="R49" s="81"/>
+      <c r="B49" s="44"/>
+      <c r="C49" s="45"/>
+      <c r="D49" s="45"/>
+      <c r="E49" s="45"/>
+      <c r="F49" s="46"/>
+      <c r="H49" s="44"/>
+      <c r="I49" s="45"/>
+      <c r="J49" s="45"/>
+      <c r="K49" s="45"/>
+      <c r="L49" s="46"/>
+      <c r="N49" s="44"/>
+      <c r="O49" s="45"/>
+      <c r="P49" s="45"/>
+      <c r="Q49" s="45"/>
+      <c r="R49" s="46"/>
     </row>
     <row r="50" spans="2:18">
-      <c r="B50" s="79"/>
-      <c r="C50" s="80"/>
-      <c r="D50" s="80"/>
-      <c r="E50" s="80"/>
-      <c r="F50" s="81"/>
-      <c r="H50" s="79"/>
-      <c r="I50" s="80"/>
-      <c r="J50" s="80"/>
-      <c r="K50" s="80"/>
-      <c r="L50" s="81"/>
-      <c r="N50" s="79"/>
-      <c r="O50" s="80"/>
-      <c r="P50" s="80"/>
-      <c r="Q50" s="80"/>
-      <c r="R50" s="81"/>
+      <c r="B50" s="44"/>
+      <c r="C50" s="45"/>
+      <c r="D50" s="45"/>
+      <c r="E50" s="45"/>
+      <c r="F50" s="46"/>
+      <c r="H50" s="44"/>
+      <c r="I50" s="45"/>
+      <c r="J50" s="45"/>
+      <c r="K50" s="45"/>
+      <c r="L50" s="46"/>
+      <c r="N50" s="44"/>
+      <c r="O50" s="45"/>
+      <c r="P50" s="45"/>
+      <c r="Q50" s="45"/>
+      <c r="R50" s="46"/>
     </row>
     <row r="51" spans="2:18">
-      <c r="B51" s="79"/>
-      <c r="C51" s="80"/>
-      <c r="D51" s="80"/>
-      <c r="E51" s="80"/>
-      <c r="F51" s="81"/>
-      <c r="H51" s="79"/>
-      <c r="I51" s="80"/>
-      <c r="J51" s="80"/>
-      <c r="K51" s="80"/>
-      <c r="L51" s="81"/>
-      <c r="N51" s="79"/>
-      <c r="O51" s="80"/>
-      <c r="P51" s="80"/>
-      <c r="Q51" s="80"/>
-      <c r="R51" s="81"/>
+      <c r="B51" s="44"/>
+      <c r="C51" s="45"/>
+      <c r="D51" s="45"/>
+      <c r="E51" s="45"/>
+      <c r="F51" s="46"/>
+      <c r="H51" s="44"/>
+      <c r="I51" s="45"/>
+      <c r="J51" s="45"/>
+      <c r="K51" s="45"/>
+      <c r="L51" s="46"/>
+      <c r="N51" s="44"/>
+      <c r="O51" s="45"/>
+      <c r="P51" s="45"/>
+      <c r="Q51" s="45"/>
+      <c r="R51" s="46"/>
     </row>
     <row r="52" spans="2:18">
-      <c r="B52" s="82"/>
-      <c r="C52" s="83"/>
-      <c r="D52" s="83"/>
-      <c r="E52" s="83"/>
-      <c r="F52" s="84"/>
-      <c r="H52" s="82"/>
-      <c r="I52" s="83"/>
-      <c r="J52" s="83"/>
-      <c r="K52" s="83"/>
-      <c r="L52" s="84"/>
-      <c r="N52" s="82"/>
-      <c r="O52" s="83"/>
-      <c r="P52" s="83"/>
-      <c r="Q52" s="83"/>
-      <c r="R52" s="84"/>
+      <c r="B52" s="47"/>
+      <c r="C52" s="48"/>
+      <c r="D52" s="48"/>
+      <c r="E52" s="48"/>
+      <c r="F52" s="49"/>
+      <c r="H52" s="47"/>
+      <c r="I52" s="48"/>
+      <c r="J52" s="48"/>
+      <c r="K52" s="48"/>
+      <c r="L52" s="49"/>
+      <c r="N52" s="47"/>
+      <c r="O52" s="48"/>
+      <c r="P52" s="48"/>
+      <c r="Q52" s="48"/>
+      <c r="R52" s="49"/>
     </row>
     <row r="53" spans="2:18">
-      <c r="B53" s="76" t="s">
+      <c r="B53" s="41" t="s">
         <v>126</v>
       </c>
-      <c r="C53" s="77"/>
-      <c r="D53" s="77"/>
-      <c r="E53" s="77"/>
-      <c r="F53" s="78"/>
-      <c r="H53" s="76" t="s">
+      <c r="C53" s="42"/>
+      <c r="D53" s="42"/>
+      <c r="E53" s="42"/>
+      <c r="F53" s="43"/>
+      <c r="H53" s="41" t="s">
         <v>127</v>
       </c>
-      <c r="I53" s="77"/>
-      <c r="J53" s="77"/>
-      <c r="K53" s="77"/>
-      <c r="L53" s="78"/>
-      <c r="N53" s="76" t="s">
+      <c r="I53" s="42"/>
+      <c r="J53" s="42"/>
+      <c r="K53" s="42"/>
+      <c r="L53" s="43"/>
+      <c r="N53" s="41" t="s">
         <v>128</v>
       </c>
-      <c r="O53" s="77"/>
-      <c r="P53" s="77"/>
-      <c r="Q53" s="77"/>
-      <c r="R53" s="78"/>
+      <c r="O53" s="42"/>
+      <c r="P53" s="42"/>
+      <c r="Q53" s="42"/>
+      <c r="R53" s="43"/>
     </row>
     <row r="54" spans="2:18">
-      <c r="B54" s="79"/>
-      <c r="C54" s="80"/>
-      <c r="D54" s="80"/>
-      <c r="E54" s="80"/>
-      <c r="F54" s="81"/>
-      <c r="H54" s="79"/>
-      <c r="I54" s="80"/>
-      <c r="J54" s="80"/>
-      <c r="K54" s="80"/>
-      <c r="L54" s="81"/>
-      <c r="N54" s="79"/>
-      <c r="O54" s="80"/>
-      <c r="P54" s="80"/>
-      <c r="Q54" s="80"/>
-      <c r="R54" s="81"/>
+      <c r="B54" s="44"/>
+      <c r="C54" s="45"/>
+      <c r="D54" s="45"/>
+      <c r="E54" s="45"/>
+      <c r="F54" s="46"/>
+      <c r="H54" s="44"/>
+      <c r="I54" s="45"/>
+      <c r="J54" s="45"/>
+      <c r="K54" s="45"/>
+      <c r="L54" s="46"/>
+      <c r="N54" s="44"/>
+      <c r="O54" s="45"/>
+      <c r="P54" s="45"/>
+      <c r="Q54" s="45"/>
+      <c r="R54" s="46"/>
     </row>
     <row r="55" spans="2:18">
-      <c r="B55" s="79"/>
-      <c r="C55" s="80"/>
-      <c r="D55" s="80"/>
-      <c r="E55" s="80"/>
-      <c r="F55" s="81"/>
-      <c r="H55" s="79"/>
-      <c r="I55" s="80"/>
-      <c r="J55" s="80"/>
-      <c r="K55" s="80"/>
-      <c r="L55" s="81"/>
-      <c r="N55" s="79"/>
-      <c r="O55" s="80"/>
-      <c r="P55" s="80"/>
-      <c r="Q55" s="80"/>
-      <c r="R55" s="81"/>
+      <c r="B55" s="44"/>
+      <c r="C55" s="45"/>
+      <c r="D55" s="45"/>
+      <c r="E55" s="45"/>
+      <c r="F55" s="46"/>
+      <c r="H55" s="44"/>
+      <c r="I55" s="45"/>
+      <c r="J55" s="45"/>
+      <c r="K55" s="45"/>
+      <c r="L55" s="46"/>
+      <c r="N55" s="44"/>
+      <c r="O55" s="45"/>
+      <c r="P55" s="45"/>
+      <c r="Q55" s="45"/>
+      <c r="R55" s="46"/>
     </row>
     <row r="56" spans="2:18">
-      <c r="B56" s="79"/>
-      <c r="C56" s="80"/>
-      <c r="D56" s="80"/>
-      <c r="E56" s="80"/>
-      <c r="F56" s="81"/>
-      <c r="H56" s="79"/>
-      <c r="I56" s="80"/>
-      <c r="J56" s="80"/>
-      <c r="K56" s="80"/>
-      <c r="L56" s="81"/>
-      <c r="N56" s="79"/>
-      <c r="O56" s="80"/>
-      <c r="P56" s="80"/>
-      <c r="Q56" s="80"/>
-      <c r="R56" s="81"/>
+      <c r="B56" s="44"/>
+      <c r="C56" s="45"/>
+      <c r="D56" s="45"/>
+      <c r="E56" s="45"/>
+      <c r="F56" s="46"/>
+      <c r="H56" s="44"/>
+      <c r="I56" s="45"/>
+      <c r="J56" s="45"/>
+      <c r="K56" s="45"/>
+      <c r="L56" s="46"/>
+      <c r="N56" s="44"/>
+      <c r="O56" s="45"/>
+      <c r="P56" s="45"/>
+      <c r="Q56" s="45"/>
+      <c r="R56" s="46"/>
     </row>
     <row r="57" spans="2:18">
-      <c r="B57" s="82"/>
-      <c r="C57" s="83"/>
-      <c r="D57" s="83"/>
-      <c r="E57" s="83"/>
-      <c r="F57" s="84"/>
-      <c r="H57" s="82"/>
-      <c r="I57" s="83"/>
-      <c r="J57" s="83"/>
-      <c r="K57" s="83"/>
-      <c r="L57" s="84"/>
-      <c r="N57" s="82"/>
-      <c r="O57" s="83"/>
-      <c r="P57" s="83"/>
-      <c r="Q57" s="83"/>
-      <c r="R57" s="84"/>
+      <c r="B57" s="47"/>
+      <c r="C57" s="48"/>
+      <c r="D57" s="48"/>
+      <c r="E57" s="48"/>
+      <c r="F57" s="49"/>
+      <c r="H57" s="47"/>
+      <c r="I57" s="48"/>
+      <c r="J57" s="48"/>
+      <c r="K57" s="48"/>
+      <c r="L57" s="49"/>
+      <c r="N57" s="47"/>
+      <c r="O57" s="48"/>
+      <c r="P57" s="48"/>
+      <c r="Q57" s="48"/>
+      <c r="R57" s="49"/>
     </row>
     <row r="60" spans="2:18" ht="18.3">
       <c r="B60" s="6" t="s">
@@ -4573,13 +4575,13 @@
       <c r="R67" s="27"/>
     </row>
     <row r="70" spans="2:18" ht="15.6">
-      <c r="N70" s="97" t="s">
+      <c r="N70" s="38" t="s">
         <v>143</v>
       </c>
-      <c r="O70" s="98"/>
-      <c r="P70" s="98"/>
-      <c r="Q70" s="98"/>
-      <c r="R70" s="99"/>
+      <c r="O70" s="39"/>
+      <c r="P70" s="39"/>
+      <c r="Q70" s="39"/>
+      <c r="R70" s="40"/>
     </row>
     <row r="71" spans="2:18" ht="32.1" customHeight="1">
       <c r="N71" s="28"/>
@@ -4654,6 +4656,30 @@
     </row>
   </sheetData>
   <mergeCells count="31">
+    <mergeCell ref="B4:F5"/>
+    <mergeCell ref="H4:L5"/>
+    <mergeCell ref="N4:R5"/>
+    <mergeCell ref="B6:F9"/>
+    <mergeCell ref="H6:L9"/>
+    <mergeCell ref="N6:R9"/>
+    <mergeCell ref="B12:F13"/>
+    <mergeCell ref="H12:L13"/>
+    <mergeCell ref="N12:R13"/>
+    <mergeCell ref="B14:F18"/>
+    <mergeCell ref="H14:L18"/>
+    <mergeCell ref="N14:R18"/>
+    <mergeCell ref="B19:F23"/>
+    <mergeCell ref="H19:L23"/>
+    <mergeCell ref="N19:R23"/>
+    <mergeCell ref="B38:F39"/>
+    <mergeCell ref="H38:L39"/>
+    <mergeCell ref="N38:R39"/>
+    <mergeCell ref="B40:F43"/>
+    <mergeCell ref="H40:L43"/>
+    <mergeCell ref="N40:R43"/>
+    <mergeCell ref="B46:F47"/>
+    <mergeCell ref="H46:L47"/>
+    <mergeCell ref="N46:R47"/>
     <mergeCell ref="N70:R70"/>
     <mergeCell ref="B48:F52"/>
     <mergeCell ref="H48:L52"/>
@@ -4661,30 +4687,6 @@
     <mergeCell ref="B53:F57"/>
     <mergeCell ref="H53:L57"/>
     <mergeCell ref="N53:R57"/>
-    <mergeCell ref="B40:F43"/>
-    <mergeCell ref="H40:L43"/>
-    <mergeCell ref="N40:R43"/>
-    <mergeCell ref="B46:F47"/>
-    <mergeCell ref="H46:L47"/>
-    <mergeCell ref="N46:R47"/>
-    <mergeCell ref="B19:F23"/>
-    <mergeCell ref="H19:L23"/>
-    <mergeCell ref="N19:R23"/>
-    <mergeCell ref="B38:F39"/>
-    <mergeCell ref="H38:L39"/>
-    <mergeCell ref="N38:R39"/>
-    <mergeCell ref="B12:F13"/>
-    <mergeCell ref="H12:L13"/>
-    <mergeCell ref="N12:R13"/>
-    <mergeCell ref="B14:F18"/>
-    <mergeCell ref="H14:L18"/>
-    <mergeCell ref="N14:R18"/>
-    <mergeCell ref="B4:F5"/>
-    <mergeCell ref="H4:L5"/>
-    <mergeCell ref="N4:R5"/>
-    <mergeCell ref="B6:F9"/>
-    <mergeCell ref="H6:L9"/>
-    <mergeCell ref="N6:R9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>

</xml_diff>

<commit_message>
adding overnight rates-IL-out iwmo
</commit_message>
<xml_diff>
--- a/input/multiassets.xlsx
+++ b/input/multiassets.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/935cc860ba0efd68/GitHub/myportfolio/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="81" documentId="13_ncr:1_{B10D7187-5546-4483-8DEF-63838578FBF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8697EC8E-8124-448D-80A6-1090337D679B}"/>
+  <xr:revisionPtr revIDLastSave="149" documentId="13_ncr:1_{B10D7187-5546-4483-8DEF-63838578FBF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{23B53F54-8431-4271-AE87-42DA6408CEF4}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,7 +18,8 @@
     <sheet name="altri" sheetId="4" r:id="rId3"/>
     <sheet name="ticker" sheetId="3" r:id="rId4"/>
     <sheet name="ISIN" sheetId="2" r:id="rId5"/>
-    <sheet name="bond" sheetId="5" r:id="rId6"/>
+    <sheet name="bonds" sheetId="7" r:id="rId6"/>
+    <sheet name="bond" sheetId="5" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -302,7 +303,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="390" uniqueCount="212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="469" uniqueCount="226">
   <si>
     <t>iShares Core MSCI World UCITS ETF USD</t>
   </si>
@@ -1112,15 +1113,9 @@
     <t>US Short Treasury</t>
   </si>
   <si>
-    <t>iShares USD TIPS 0-5 UCITS ETF USD (Dist) | SXRH | IE00BDQYWQ65</t>
-  </si>
-  <si>
     <t>dist</t>
   </si>
   <si>
-    <t>IE00BDQYWQ65</t>
-  </si>
-  <si>
     <t>IBGM.AS</t>
   </si>
   <si>
@@ -1154,15 +1149,6 @@
     <t>Invesco Physical Gold A | SGLD | IE00B579F325</t>
   </si>
   <si>
-    <t>iShares $ TIPS 0-5 UCITS ETF USD (Dist)</t>
-  </si>
-  <si>
-    <t>TIP5.L</t>
-  </si>
-  <si>
-    <t>US TIPS 0-5y</t>
-  </si>
-  <si>
     <t>IE00BF4RFH31</t>
   </si>
   <si>
@@ -1233,6 +1219,63 @@
   </si>
   <si>
     <t>IE0032523478</t>
+  </si>
+  <si>
+    <t>LEONIA.MI</t>
+  </si>
+  <si>
+    <t>Amundi EUR Overnight Return UCITS ETF Acc (LEONIA.MI) Stock Price, News, Quote &amp; History - Yahoo Finance</t>
+  </si>
+  <si>
+    <t>Amundi EUR Overnight Return UCITS ETF Acc</t>
+  </si>
+  <si>
+    <t>EU Overnight</t>
+  </si>
+  <si>
+    <t>FR0010510800</t>
+  </si>
+  <si>
+    <t>unfunded swap</t>
+  </si>
+  <si>
+    <t>quota cash</t>
+  </si>
+  <si>
+    <t>IE00B0M62X26</t>
+  </si>
+  <si>
+    <t>IBCI.AS</t>
+  </si>
+  <si>
+    <t>EU Inflation-Linked</t>
+  </si>
+  <si>
+    <t>iShares Euro Inflation Linked Government Bond UCITS ETF | IBCI | IE00B0M62X26</t>
+  </si>
+  <si>
+    <t>LU1390062245</t>
+  </si>
+  <si>
+    <t>iShares € Inflation Linked Govt Bond UCITS ETF EUR (Acc)</t>
+  </si>
+  <si>
+    <t>Amundi Euro Inflation Expectations 2-10Y UCITS ETF Acc | INFL | LU1390062245</t>
+  </si>
+  <si>
+    <t>EU Break-Even 2-10y</t>
+  </si>
+  <si>
+    <t>Amundi Euro Inflation Expectations 2-10Y UCITS ETF Acc</t>
+  </si>
+  <si>
+    <t>INFL.PA</t>
+  </si>
+  <si>
+    <t>swap</t>
+  </si>
+  <si>
+    <t>iShares Core MSCI World UCITS ETF USD (Acc) | SWDA | IE00B4L5Y983</t>
   </si>
 </sst>
 </file>
@@ -1725,6 +1768,186 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="8" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1734,188 +1957,8 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1935,6 +1978,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2200,11 +2247,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B015881-81C4-40D2-9396-65046E56EE7C}">
-  <dimension ref="A1:L9"/>
+  <dimension ref="A1:L10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
@@ -2212,7 +2257,8 @@
     <col min="2" max="2" width="52.7890625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="52.1015625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.41796875" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="7.9453125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.26171875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.9453125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15.1015625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="13.26171875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="5.5234375" bestFit="1" customWidth="1"/>
@@ -2261,34 +2307,34 @@
     </row>
     <row r="2" spans="1:12">
       <c r="A2" s="36" t="s">
-        <v>165</v>
+        <v>225</v>
       </c>
       <c r="B2" t="s">
-        <v>201</v>
+        <v>14</v>
       </c>
       <c r="C2" t="s">
-        <v>154</v>
+        <v>0</v>
       </c>
       <c r="D2" t="s">
-        <v>155</v>
+        <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>161</v>
+        <v>59</v>
       </c>
       <c r="F2" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="G2" t="s">
         <v>7</v>
       </c>
       <c r="H2" t="s">
-        <v>180</v>
+        <v>32</v>
       </c>
       <c r="I2" s="1">
-        <v>2.5000000000000001E-3</v>
+        <v>2E-3</v>
       </c>
       <c r="J2" t="s">
-        <v>54</v>
+        <v>34</v>
       </c>
       <c r="K2" t="s">
         <v>151</v>
@@ -2299,19 +2345,19 @@
     </row>
     <row r="3" spans="1:12">
       <c r="A3" s="36" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="B3" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="C3" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="D3" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="E3" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="F3" t="s">
         <v>11</v>
@@ -2331,19 +2377,19 @@
     </row>
     <row r="4" spans="1:12">
       <c r="A4" s="36" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="B4" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="C4" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="D4" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="E4" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="F4" t="s">
         <v>11</v>
@@ -2369,13 +2415,13 @@
         <v>169</v>
       </c>
       <c r="C5" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="D5" t="s">
         <v>168</v>
       </c>
       <c r="E5" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="F5" t="s">
         <v>17</v>
@@ -2384,7 +2430,7 @@
         <v>7</v>
       </c>
       <c r="H5" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="I5" s="1">
         <v>1.5E-3</v>
@@ -2401,19 +2447,19 @@
     </row>
     <row r="6" spans="1:12">
       <c r="A6" s="36" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="B6" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="C6" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="D6" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="E6" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="F6" t="s">
         <v>17</v>
@@ -2422,10 +2468,10 @@
         <v>7</v>
       </c>
       <c r="H6" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="J6" t="s">
         <v>34</v>
@@ -2433,125 +2479,155 @@
     </row>
     <row r="7" spans="1:12">
       <c r="A7" s="36" t="s">
-        <v>171</v>
+        <v>217</v>
       </c>
       <c r="B7" t="s">
-        <v>187</v>
+        <v>216</v>
       </c>
       <c r="C7" t="s">
-        <v>185</v>
+        <v>219</v>
       </c>
       <c r="D7" t="s">
-        <v>173</v>
+        <v>214</v>
       </c>
       <c r="E7" t="s">
-        <v>186</v>
+        <v>215</v>
       </c>
       <c r="F7" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="G7" t="s">
         <v>7</v>
       </c>
       <c r="H7" t="s">
-        <v>172</v>
+        <v>178</v>
       </c>
       <c r="I7" s="1">
-        <v>1E-3</v>
+        <v>8.9999999999999998E-4</v>
       </c>
       <c r="J7" t="s">
         <v>34</v>
       </c>
-      <c r="K7" t="s">
-        <v>86</v>
-      </c>
-      <c r="L7" t="s">
-        <v>87</v>
-      </c>
     </row>
     <row r="8" spans="1:12">
       <c r="A8" s="36" t="s">
-        <v>176</v>
+        <v>208</v>
       </c>
       <c r="B8" t="s">
-        <v>170</v>
+        <v>210</v>
       </c>
       <c r="C8" t="s">
-        <v>177</v>
+        <v>209</v>
       </c>
       <c r="D8" t="s">
-        <v>178</v>
+        <v>211</v>
       </c>
       <c r="E8" t="s">
-        <v>179</v>
+        <v>207</v>
       </c>
       <c r="F8" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="G8" t="s">
         <v>7</v>
       </c>
       <c r="H8" t="s">
-        <v>172</v>
+        <v>178</v>
       </c>
       <c r="I8" s="1">
-        <v>6.9999999999999999E-4</v>
+        <v>1E-3</v>
       </c>
       <c r="J8" t="s">
-        <v>34</v>
+        <v>212</v>
       </c>
       <c r="K8" t="s">
-        <v>85</v>
+        <v>213</v>
       </c>
     </row>
     <row r="9" spans="1:12">
       <c r="A9" s="36" t="s">
-        <v>184</v>
+        <v>174</v>
       </c>
       <c r="B9" t="s">
-        <v>75</v>
+        <v>170</v>
       </c>
       <c r="C9" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
       <c r="D9" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="E9" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
       <c r="F9" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="G9" t="s">
         <v>7</v>
       </c>
       <c r="H9" t="s">
+        <v>171</v>
+      </c>
+      <c r="I9" s="1">
+        <v>6.9999999999999999E-4</v>
+      </c>
+      <c r="J9" t="s">
+        <v>34</v>
+      </c>
+      <c r="K9" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12">
+      <c r="A10" s="36" t="s">
+        <v>182</v>
+      </c>
+      <c r="B10" t="s">
+        <v>75</v>
+      </c>
+      <c r="C10" t="s">
         <v>180</v>
       </c>
-      <c r="I9" s="1">
+      <c r="D10" t="s">
+        <v>179</v>
+      </c>
+      <c r="E10" t="s">
+        <v>181</v>
+      </c>
+      <c r="F10" t="s">
+        <v>17</v>
+      </c>
+      <c r="G10" t="s">
+        <v>7</v>
+      </c>
+      <c r="H10" t="s">
+        <v>178</v>
+      </c>
+      <c r="I10" s="1">
         <v>1.1999999999999999E-3</v>
       </c>
-      <c r="J9" t="s">
+      <c r="J10" t="s">
         <v>54</v>
       </c>
-      <c r="K9" t="s">
+      <c r="K10" t="s">
         <v>86</v>
       </c>
-      <c r="L9" t="s">
+      <c r="L10" t="s">
         <v>82</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://www.justetf.com/it/etf-profile.html?isin=IE00BP3QZ825" xr:uid="{5E561C16-8B8B-483B-AA10-D0DDAD2EE0FF}"/>
-    <hyperlink ref="A5" r:id="rId2" display="https://www.justetf.com/it/etf-profile.html?isin=IE00B3VTN290" xr:uid="{6AB80B8F-0CAF-4297-B9BB-D72ED9AFBF01}"/>
-    <hyperlink ref="A8" r:id="rId3" display="https://www.justetf.com/it/etf-profile.html?isin=IE00BGR7L912" xr:uid="{69029A56-B54E-49FD-A0F5-77171229A26E}"/>
-    <hyperlink ref="A9" r:id="rId4" display="https://www.justetf.com/it/etf-profile.html?isin=IE00B579F325" xr:uid="{42CB0A67-6EA5-4F8A-A191-29BAAE4A4956}"/>
-    <hyperlink ref="A7" r:id="rId5" display="https://www.justetf.com/it/etf-profile.html?isin=IE00BDQYWQ65" xr:uid="{6C04B138-97D3-42C8-B6E1-00870CCBE0B4}"/>
-    <hyperlink ref="A3" r:id="rId6" display="https://www.justetf.com/it/etf-profile.html?isin=IE00BD1F4L37" xr:uid="{DF84D7C7-B8F6-477A-8C9A-D4997B54C865}"/>
-    <hyperlink ref="A4" r:id="rId7" display="https://www.justetf.com/it/etf-profile.html?isin=IE00B8FHGS14" xr:uid="{47A684AB-EAC0-4609-B6F5-2C135D16A87D}"/>
-    <hyperlink ref="A6" r:id="rId8" display="https://www.justetf.com/it/etf-profile.html?isin=IE0032523478" xr:uid="{20C7AF50-87F2-4FC4-B8A4-93B98529FB55}"/>
+    <hyperlink ref="A5" r:id="rId1" display="https://www.justetf.com/it/etf-profile.html?isin=IE00B3VTN290" xr:uid="{6AB80B8F-0CAF-4297-B9BB-D72ED9AFBF01}"/>
+    <hyperlink ref="A9" r:id="rId2" display="https://www.justetf.com/it/etf-profile.html?isin=IE00BGR7L912" xr:uid="{69029A56-B54E-49FD-A0F5-77171229A26E}"/>
+    <hyperlink ref="A10" r:id="rId3" display="https://www.justetf.com/it/etf-profile.html?isin=IE00B579F325" xr:uid="{42CB0A67-6EA5-4F8A-A191-29BAAE4A4956}"/>
+    <hyperlink ref="A3" r:id="rId4" display="https://www.justetf.com/it/etf-profile.html?isin=IE00BD1F4L37" xr:uid="{DF84D7C7-B8F6-477A-8C9A-D4997B54C865}"/>
+    <hyperlink ref="A4" r:id="rId5" display="https://www.justetf.com/it/etf-profile.html?isin=IE00B8FHGS14" xr:uid="{47A684AB-EAC0-4609-B6F5-2C135D16A87D}"/>
+    <hyperlink ref="A6" r:id="rId6" display="https://www.justetf.com/it/etf-profile.html?isin=IE0032523478" xr:uid="{20C7AF50-87F2-4FC4-B8A4-93B98529FB55}"/>
+    <hyperlink ref="A8" r:id="rId7" display="https://finance.yahoo.com/quote/LEONIA.MI/" xr:uid="{C03B49D3-5D8D-4719-818C-85A9CCE78BAE}"/>
+    <hyperlink ref="A7" r:id="rId8" display="https://www.justetf.com/it/etf-profile.html?isin=IE00B0M62X26" xr:uid="{80E603FC-0B0D-4EAD-9D73-152F6C249FED}"/>
+    <hyperlink ref="A2" r:id="rId9" display="https://www.justetf.com/it/etf-profile.html?isin=IE00B4L5Y983" xr:uid="{07C799E5-4B70-419F-8A83-D91DFAD88307}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2559,10 +2635,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K11"/>
+  <dimension ref="A1:L12"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A1:K10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -2578,354 +2654,398 @@
     <col min="10" max="10" width="21.7890625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:12">
       <c r="A1" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
-      <c r="A2" t="s">
+    <row r="2" spans="1:12">
+      <c r="A2" s="36" t="s">
+        <v>165</v>
+      </c>
+      <c r="B2" t="s">
+        <v>196</v>
+      </c>
+      <c r="C2" t="s">
+        <v>154</v>
+      </c>
+      <c r="D2" t="s">
+        <v>155</v>
+      </c>
+      <c r="E2" t="s">
+        <v>161</v>
+      </c>
+      <c r="F2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H2" t="s">
+        <v>178</v>
+      </c>
+      <c r="I2" s="1">
+        <v>2.5000000000000001E-3</v>
+      </c>
+      <c r="J2" t="s">
+        <v>54</v>
+      </c>
+      <c r="K2" t="s">
+        <v>151</v>
+      </c>
+      <c r="L2" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12">
+      <c r="B3" t="s">
         <v>78</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C3" t="s">
         <v>81</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D3" t="s">
         <v>79</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E3" t="s">
         <v>80</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F3" t="s">
         <v>17</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G3" t="s">
         <v>7</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H3" t="s">
         <v>32</v>
       </c>
-      <c r="H2" s="1">
+      <c r="I3" s="1">
         <v>1.5E-3</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J3" t="s">
         <v>35</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K3" t="s">
         <v>151</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L3" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
-      <c r="A3" t="s">
+    <row r="4" spans="1:12">
+      <c r="B4" t="s">
         <v>14</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C4" t="s">
         <v>0</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D4" t="s">
         <v>1</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E4" t="s">
         <v>59</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F4" t="s">
         <v>11</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G4" t="s">
         <v>7</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H4" t="s">
         <v>32</v>
       </c>
-      <c r="H3" s="1">
+      <c r="I4" s="1">
         <v>2E-3</v>
       </c>
-      <c r="I3" t="s">
+      <c r="J4" t="s">
         <v>34</v>
       </c>
-      <c r="J3" t="s">
+      <c r="K4" t="s">
         <v>151</v>
       </c>
-      <c r="K3" t="s">
+      <c r="L4" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="4" spans="1:11">
-      <c r="A4" t="s">
+    <row r="5" spans="1:12">
+      <c r="B5" t="s">
         <v>13</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C5" t="s">
         <v>9</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D5" t="s">
         <v>12</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E5" t="s">
         <v>60</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F5" t="s">
         <v>11</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G5" t="s">
         <v>7</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H5" t="s">
         <v>32</v>
       </c>
-      <c r="H4" s="1">
+      <c r="I5" s="1">
         <v>2E-3</v>
       </c>
-      <c r="I4" t="s">
+      <c r="J5" t="s">
         <v>35</v>
       </c>
-      <c r="J4" t="s">
+      <c r="K5" t="s">
         <v>151</v>
       </c>
-      <c r="K4" t="s">
+      <c r="L5" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="5" spans="1:11">
-      <c r="A5" t="s">
+    <row r="6" spans="1:12">
+      <c r="B6" t="s">
         <v>18</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C6" t="s">
         <v>15</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D6" t="s">
         <v>16</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E6" t="s">
         <v>57</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F6" t="s">
         <v>17</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G6" t="s">
         <v>7</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H6" t="s">
         <v>32</v>
       </c>
-      <c r="H5" s="1">
+      <c r="I6" s="1">
         <v>1.5E-3</v>
       </c>
-      <c r="I5" t="s">
+      <c r="J6" t="s">
         <v>34</v>
       </c>
-      <c r="J5" t="s">
+      <c r="K6" t="s">
         <v>84</v>
       </c>
-      <c r="K5" t="s">
+      <c r="L6" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="6" spans="1:11">
-      <c r="A6" t="s">
+    <row r="7" spans="1:12">
+      <c r="B7" t="s">
         <v>21</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C7" t="s">
         <v>23</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D7" t="s">
         <v>22</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E7" t="s">
         <v>63</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F7" t="s">
         <v>17</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G7" t="s">
         <v>31</v>
       </c>
-      <c r="G6" t="s">
+      <c r="H7" t="s">
         <v>32</v>
       </c>
-      <c r="H6" s="1">
+      <c r="I7" s="1">
         <v>1E-3</v>
       </c>
-      <c r="I6" t="s">
+      <c r="J7" t="s">
         <v>34</v>
       </c>
-      <c r="J6" t="s">
+      <c r="K7" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="7" spans="1:11">
-      <c r="A7" t="s">
+    <row r="8" spans="1:12">
+      <c r="B8" t="s">
         <v>50</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C8" t="s">
         <v>49</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D8" t="s">
         <v>51</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E8" t="s">
         <v>58</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F8" t="s">
         <v>17</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G8" t="s">
         <v>7</v>
       </c>
-      <c r="G7" t="s">
+      <c r="H8" t="s">
         <v>32</v>
       </c>
-      <c r="H7" s="1">
+      <c r="I8" s="1">
         <v>8.9999999999999998E-4</v>
       </c>
-      <c r="I7" t="s">
+      <c r="J8" t="s">
         <v>34</v>
       </c>
-      <c r="J7" t="s">
+      <c r="K8" t="s">
         <v>86</v>
       </c>
-      <c r="K7" t="s">
+      <c r="L8" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="8" spans="1:11">
-      <c r="A8" t="s">
+    <row r="9" spans="1:12">
+      <c r="B9" t="s">
         <v>53</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C9" t="s">
         <v>71</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D9" t="s">
         <v>69</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E9" t="s">
         <v>70</v>
       </c>
-      <c r="E8" t="s">
+      <c r="F9" t="s">
         <v>11</v>
       </c>
-      <c r="F8" t="s">
+      <c r="G9" t="s">
         <v>7</v>
       </c>
-      <c r="G8" t="s">
+      <c r="H9" t="s">
         <v>32</v>
       </c>
-      <c r="H8" s="1">
+      <c r="I9" s="1">
         <v>6.9999999999999999E-4</v>
       </c>
-      <c r="I8" t="s">
+      <c r="J9" t="s">
         <v>34</v>
       </c>
-      <c r="J8" t="s">
+      <c r="K9" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="9" spans="1:11">
-      <c r="A9" t="s">
+    <row r="10" spans="1:12">
+      <c r="B10" t="s">
         <v>91</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C10" t="s">
         <v>90</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D10" t="s">
         <v>92</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E10" t="s">
         <v>94</v>
       </c>
-      <c r="E9" t="s">
+      <c r="F10" t="s">
         <v>17</v>
       </c>
-      <c r="F9" t="s">
+      <c r="G10" t="s">
         <v>7</v>
       </c>
-      <c r="G9" t="s">
+      <c r="H10" t="s">
         <v>32</v>
       </c>
-      <c r="H9" s="1">
+      <c r="I10" s="1">
         <v>1.5E-3</v>
       </c>
-      <c r="I9" t="s">
+      <c r="J10" t="s">
         <v>34</v>
       </c>
-      <c r="J9" t="s">
+      <c r="K10" t="s">
         <v>85</v>
       </c>
-      <c r="K9" t="s">
+      <c r="L10" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="10" spans="1:11">
-      <c r="A10" t="s">
+    <row r="11" spans="1:12">
+      <c r="B11" t="s">
         <v>75</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C11" t="s">
         <v>77</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D11" t="s">
         <v>93</v>
       </c>
-      <c r="D10" t="s">
+      <c r="E11" t="s">
         <v>76</v>
       </c>
-      <c r="E10" t="s">
+      <c r="F11" t="s">
         <v>11</v>
       </c>
-      <c r="F10" t="s">
+      <c r="G11" t="s">
         <v>7</v>
       </c>
-      <c r="G10" t="s">
+      <c r="H11" t="s">
         <v>32</v>
       </c>
-      <c r="H10" s="1">
+      <c r="I11" s="1">
         <v>1.1999999999999999E-3</v>
       </c>
-      <c r="I10" t="s">
+      <c r="J11" t="s">
         <v>54</v>
       </c>
-      <c r="J10" t="s">
+      <c r="K11" t="s">
         <v>86</v>
       </c>
-      <c r="K10" t="s">
+      <c r="L11" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="11" spans="1:11">
-      <c r="B11" s="3"/>
+    <row r="12" spans="1:12">
+      <c r="B12" s="3"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" display="https://www.justetf.com/it/etf-profile.html?isin=IE00BP3QZ825" xr:uid="{5E561C16-8B8B-483B-AA10-D0DDAD2EE0FF}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -3225,16 +3345,16 @@
     </row>
     <row r="10" spans="1:12">
       <c r="B10" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="C10" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="D10" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="E10" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="F10" t="s">
         <v>11</v>
@@ -3254,16 +3374,16 @@
     </row>
     <row r="11" spans="1:12" ht="14.7" customHeight="1">
       <c r="B11" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="C11" s="37" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="D11" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="E11" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="F11" t="s">
         <v>11</v>
@@ -3283,16 +3403,16 @@
     </row>
     <row r="12" spans="1:12">
       <c r="B12" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="C12" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="D12" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="E12" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="F12" t="s">
         <v>11</v>
@@ -3333,7 +3453,7 @@
         <v>7</v>
       </c>
       <c r="H13" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="I13" s="1">
         <v>2.5000000000000001E-3</v>
@@ -3353,7 +3473,7 @@
         <v>156</v>
       </c>
       <c r="D14" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="E14" t="s">
         <v>157</v>
@@ -3365,7 +3485,7 @@
         <v>7</v>
       </c>
       <c r="H14" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="I14" s="1">
         <v>3.5000000000000001E-3</v>
@@ -3385,7 +3505,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{939D994C-0E7B-435F-BB4C-7162BD8072E3}">
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3393,20 +3513,20 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="str" cm="1">
-        <f t="array" ref="A1:A9">overview!E1:E9</f>
+        <f t="array" ref="A1:A10">overview!E1:E10</f>
         <v>Ticker</v>
       </c>
       <c r="B1" t="str" cm="1">
-        <f t="array" ref="B1:B9">overview!B1:B9</f>
+        <f t="array" ref="B1:B10">overview!B1:B10</f>
         <v>Index</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="str">
-        <v>IWMO.L</v>
+        <v>IWDA.L</v>
       </c>
       <c r="B2" t="str">
-        <v>World Momentum</v>
+        <v>MSCI World</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -3443,25 +3563,33 @@
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="str">
-        <v>TIP5.L</v>
+        <v>IBCI.AS</v>
       </c>
       <c r="B7" t="str">
-        <v>US TIPS 0-5y</v>
+        <v>EU Inflation-Linked</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="str">
-        <v>IBTU.L</v>
+        <v>LEONIA.MI</v>
       </c>
       <c r="B8" t="str">
-        <v>US Short Treasury</v>
+        <v>EU Overnight</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="str">
+        <v>IBTU.L</v>
+      </c>
+      <c r="B9" t="str">
+        <v>US Short Treasury</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" t="str">
         <v>SGLD.AS</v>
       </c>
-      <c r="B9" t="str">
+      <c r="B10" t="str">
         <v>ETC GOLD</v>
       </c>
     </row>
@@ -3472,7 +3600,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA57C457-A80C-477F-8A3E-0F8DB96F6511}">
-  <dimension ref="A1:A9"/>
+  <dimension ref="A1:A10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -3482,13 +3610,13 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="str" cm="1">
-        <f t="array" ref="A1:A9">overview!C1:C9</f>
+        <f t="array" ref="A1:A10">overview!C1:C10</f>
         <v>Name</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="str">
-        <v>iShares Edge MSCI World Momentum Factor UCITS ETF</v>
+        <v>iShares Core MSCI World UCITS ETF USD</v>
       </c>
     </row>
     <row r="3" spans="1:1">
@@ -3513,16 +3641,21 @@
     </row>
     <row r="7" spans="1:1">
       <c r="A7" t="str">
-        <v>iShares $ TIPS 0-5 UCITS ETF USD (Dist)</v>
+        <v>iShares € Inflation Linked Govt Bond UCITS ETF EUR (Acc)</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8" t="str">
-        <v>iShares USD Treasury Bond 0-1yr UCITS ETF (Dist)</v>
+        <v>Amundi EUR Overnight Return UCITS ETF Acc</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9" t="str">
+        <v>iShares USD Treasury Bond 0-1yr UCITS ETF (Dist)</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1">
+      <c r="A10" t="str">
         <v>Invesco Physical Gold ETC</v>
       </c>
     </row>
@@ -3532,6 +3665,237 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A35CB12-9DE7-49FA-8FB3-31069683DE1C}">
+  <dimension ref="A1:L6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="87.83984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12">
+      <c r="A1" s="36" t="s">
+        <v>167</v>
+      </c>
+      <c r="B1" t="s">
+        <v>169</v>
+      </c>
+      <c r="C1" t="s">
+        <v>173</v>
+      </c>
+      <c r="D1" t="s">
+        <v>168</v>
+      </c>
+      <c r="E1" t="s">
+        <v>172</v>
+      </c>
+      <c r="F1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" t="s">
+        <v>171</v>
+      </c>
+      <c r="I1" s="1">
+        <v>1.5E-3</v>
+      </c>
+      <c r="J1" t="s">
+        <v>34</v>
+      </c>
+      <c r="K1" t="s">
+        <v>84</v>
+      </c>
+      <c r="L1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12">
+      <c r="A2" s="36" t="s">
+        <v>203</v>
+      </c>
+      <c r="B2" t="s">
+        <v>205</v>
+      </c>
+      <c r="C2" t="s">
+        <v>204</v>
+      </c>
+      <c r="D2" t="s">
+        <v>206</v>
+      </c>
+      <c r="E2" t="s">
+        <v>201</v>
+      </c>
+      <c r="F2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H2" t="s">
+        <v>171</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="J2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12">
+      <c r="A3" s="36" t="s">
+        <v>217</v>
+      </c>
+      <c r="B3" t="s">
+        <v>216</v>
+      </c>
+      <c r="C3" t="s">
+        <v>219</v>
+      </c>
+      <c r="D3" t="s">
+        <v>214</v>
+      </c>
+      <c r="E3" t="s">
+        <v>215</v>
+      </c>
+      <c r="F3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G3" t="s">
+        <v>7</v>
+      </c>
+      <c r="H3" t="s">
+        <v>178</v>
+      </c>
+      <c r="I3" s="1">
+        <v>8.9999999999999998E-4</v>
+      </c>
+      <c r="J3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12">
+      <c r="A4" s="36" t="s">
+        <v>220</v>
+      </c>
+      <c r="B4" t="s">
+        <v>221</v>
+      </c>
+      <c r="C4" t="s">
+        <v>222</v>
+      </c>
+      <c r="D4" t="s">
+        <v>218</v>
+      </c>
+      <c r="E4" t="s">
+        <v>223</v>
+      </c>
+      <c r="F4" t="s">
+        <v>17</v>
+      </c>
+      <c r="G4" t="s">
+        <v>7</v>
+      </c>
+      <c r="H4" t="s">
+        <v>178</v>
+      </c>
+      <c r="I4" s="1">
+        <v>2.5000000000000001E-3</v>
+      </c>
+      <c r="J4" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12">
+      <c r="A5" s="36" t="s">
+        <v>208</v>
+      </c>
+      <c r="B5" t="s">
+        <v>210</v>
+      </c>
+      <c r="C5" t="s">
+        <v>209</v>
+      </c>
+      <c r="D5" t="s">
+        <v>211</v>
+      </c>
+      <c r="E5" t="s">
+        <v>207</v>
+      </c>
+      <c r="F5" t="s">
+        <v>17</v>
+      </c>
+      <c r="G5" t="s">
+        <v>7</v>
+      </c>
+      <c r="H5" t="s">
+        <v>178</v>
+      </c>
+      <c r="I5" s="1">
+        <v>1E-3</v>
+      </c>
+      <c r="J5" t="s">
+        <v>212</v>
+      </c>
+      <c r="K5" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12">
+      <c r="A6" s="36" t="s">
+        <v>174</v>
+      </c>
+      <c r="B6" t="s">
+        <v>170</v>
+      </c>
+      <c r="C6" t="s">
+        <v>175</v>
+      </c>
+      <c r="D6" t="s">
+        <v>176</v>
+      </c>
+      <c r="E6" t="s">
+        <v>177</v>
+      </c>
+      <c r="F6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G6" t="s">
+        <v>7</v>
+      </c>
+      <c r="H6" t="s">
+        <v>171</v>
+      </c>
+      <c r="I6" s="1">
+        <v>6.9999999999999999E-4</v>
+      </c>
+      <c r="J6" t="s">
+        <v>34</v>
+      </c>
+      <c r="K6" t="s">
+        <v>85</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A1" r:id="rId1" display="https://www.justetf.com/it/etf-profile.html?isin=IE00B3VTN290" xr:uid="{790B6689-2F70-4816-8F52-314A7D6D5ECB}"/>
+    <hyperlink ref="A6" r:id="rId2" display="https://www.justetf.com/it/etf-profile.html?isin=IE00BGR7L912" xr:uid="{4D3B5B99-D20D-43F5-B928-C07184C7BA74}"/>
+    <hyperlink ref="A2" r:id="rId3" display="https://www.justetf.com/it/etf-profile.html?isin=IE0032523478" xr:uid="{B0F54AEA-02CB-422A-938E-08F48CB58AF5}"/>
+    <hyperlink ref="A5" r:id="rId4" display="https://finance.yahoo.com/quote/LEONIA.MI/" xr:uid="{A3204164-FC69-48CC-A00D-A1BB7637CC40}"/>
+    <hyperlink ref="A3" r:id="rId5" display="https://www.justetf.com/it/etf-profile.html?isin=IE00B0M62X26" xr:uid="{C0362A1C-8363-4809-8005-2D5D78844FAD}"/>
+    <hyperlink ref="A4" r:id="rId6" display="https://www.justetf.com/it/etf-profile.html?isin=LU1390062245" xr:uid="{EDFC20A4-1859-4E34-AA2C-099765263EBC}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F1305C8-BDCE-4FC8-A22D-01D299B339FB}">
   <dimension ref="A1:R75"/>
   <sheetViews>
@@ -3551,118 +3915,118 @@
     </row>
     <row r="3" spans="1:18" ht="14.7" thickBot="1"/>
     <row r="4" spans="1:18" ht="16" customHeight="1">
-      <c r="B4" s="60" t="s">
+      <c r="B4" s="38" t="s">
         <v>97</v>
       </c>
-      <c r="C4" s="61"/>
-      <c r="D4" s="61"/>
-      <c r="E4" s="61"/>
-      <c r="F4" s="62"/>
-      <c r="H4" s="96" t="s">
+      <c r="C4" s="39"/>
+      <c r="D4" s="39"/>
+      <c r="E4" s="39"/>
+      <c r="F4" s="40"/>
+      <c r="H4" s="44" t="s">
         <v>98</v>
       </c>
-      <c r="I4" s="97"/>
-      <c r="J4" s="97"/>
-      <c r="K4" s="97"/>
-      <c r="L4" s="98"/>
-      <c r="N4" s="72" t="s">
+      <c r="I4" s="45"/>
+      <c r="J4" s="45"/>
+      <c r="K4" s="45"/>
+      <c r="L4" s="46"/>
+      <c r="N4" s="50" t="s">
         <v>99</v>
       </c>
-      <c r="O4" s="73"/>
-      <c r="P4" s="73"/>
-      <c r="Q4" s="73"/>
-      <c r="R4" s="74"/>
+      <c r="O4" s="51"/>
+      <c r="P4" s="51"/>
+      <c r="Q4" s="51"/>
+      <c r="R4" s="52"/>
     </row>
     <row r="5" spans="1:18" ht="17.100000000000001" customHeight="1" thickBot="1">
-      <c r="B5" s="63"/>
-      <c r="C5" s="64"/>
-      <c r="D5" s="64"/>
-      <c r="E5" s="64"/>
-      <c r="F5" s="65"/>
-      <c r="H5" s="99"/>
-      <c r="I5" s="100"/>
-      <c r="J5" s="100"/>
-      <c r="K5" s="100"/>
-      <c r="L5" s="101"/>
-      <c r="N5" s="75"/>
-      <c r="O5" s="76"/>
-      <c r="P5" s="76"/>
-      <c r="Q5" s="76"/>
-      <c r="R5" s="77"/>
+      <c r="B5" s="41"/>
+      <c r="C5" s="42"/>
+      <c r="D5" s="42"/>
+      <c r="E5" s="42"/>
+      <c r="F5" s="43"/>
+      <c r="H5" s="47"/>
+      <c r="I5" s="48"/>
+      <c r="J5" s="48"/>
+      <c r="K5" s="48"/>
+      <c r="L5" s="49"/>
+      <c r="N5" s="53"/>
+      <c r="O5" s="54"/>
+      <c r="P5" s="54"/>
+      <c r="Q5" s="54"/>
+      <c r="R5" s="55"/>
     </row>
     <row r="6" spans="1:18">
-      <c r="B6" s="51" t="s">
+      <c r="B6" s="56" t="s">
         <v>100</v>
       </c>
-      <c r="C6" s="52"/>
-      <c r="D6" s="52"/>
-      <c r="E6" s="52"/>
-      <c r="F6" s="53"/>
-      <c r="H6" s="51" t="s">
+      <c r="C6" s="57"/>
+      <c r="D6" s="57"/>
+      <c r="E6" s="57"/>
+      <c r="F6" s="58"/>
+      <c r="H6" s="56" t="s">
         <v>101</v>
       </c>
-      <c r="I6" s="52"/>
-      <c r="J6" s="52"/>
-      <c r="K6" s="52"/>
-      <c r="L6" s="53"/>
-      <c r="N6" s="51" t="s">
+      <c r="I6" s="57"/>
+      <c r="J6" s="57"/>
+      <c r="K6" s="57"/>
+      <c r="L6" s="58"/>
+      <c r="N6" s="56" t="s">
         <v>101</v>
       </c>
-      <c r="O6" s="52"/>
-      <c r="P6" s="52"/>
-      <c r="Q6" s="52"/>
-      <c r="R6" s="53"/>
+      <c r="O6" s="57"/>
+      <c r="P6" s="57"/>
+      <c r="Q6" s="57"/>
+      <c r="R6" s="58"/>
     </row>
     <row r="7" spans="1:18">
-      <c r="B7" s="54"/>
-      <c r="C7" s="55"/>
-      <c r="D7" s="55"/>
-      <c r="E7" s="55"/>
-      <c r="F7" s="56"/>
-      <c r="H7" s="54"/>
-      <c r="I7" s="55"/>
-      <c r="J7" s="55"/>
-      <c r="K7" s="55"/>
-      <c r="L7" s="56"/>
-      <c r="N7" s="54"/>
-      <c r="O7" s="55"/>
-      <c r="P7" s="55"/>
-      <c r="Q7" s="55"/>
-      <c r="R7" s="56"/>
+      <c r="B7" s="59"/>
+      <c r="C7" s="60"/>
+      <c r="D7" s="60"/>
+      <c r="E7" s="60"/>
+      <c r="F7" s="61"/>
+      <c r="H7" s="59"/>
+      <c r="I7" s="60"/>
+      <c r="J7" s="60"/>
+      <c r="K7" s="60"/>
+      <c r="L7" s="61"/>
+      <c r="N7" s="59"/>
+      <c r="O7" s="60"/>
+      <c r="P7" s="60"/>
+      <c r="Q7" s="60"/>
+      <c r="R7" s="61"/>
     </row>
     <row r="8" spans="1:18">
-      <c r="B8" s="54"/>
-      <c r="C8" s="55"/>
-      <c r="D8" s="55"/>
-      <c r="E8" s="55"/>
-      <c r="F8" s="56"/>
-      <c r="H8" s="54"/>
-      <c r="I8" s="55"/>
-      <c r="J8" s="55"/>
-      <c r="K8" s="55"/>
-      <c r="L8" s="56"/>
-      <c r="N8" s="54"/>
-      <c r="O8" s="55"/>
-      <c r="P8" s="55"/>
-      <c r="Q8" s="55"/>
-      <c r="R8" s="56"/>
+      <c r="B8" s="59"/>
+      <c r="C8" s="60"/>
+      <c r="D8" s="60"/>
+      <c r="E8" s="60"/>
+      <c r="F8" s="61"/>
+      <c r="H8" s="59"/>
+      <c r="I8" s="60"/>
+      <c r="J8" s="60"/>
+      <c r="K8" s="60"/>
+      <c r="L8" s="61"/>
+      <c r="N8" s="59"/>
+      <c r="O8" s="60"/>
+      <c r="P8" s="60"/>
+      <c r="Q8" s="60"/>
+      <c r="R8" s="61"/>
     </row>
     <row r="9" spans="1:18">
-      <c r="B9" s="57"/>
-      <c r="C9" s="58"/>
-      <c r="D9" s="58"/>
-      <c r="E9" s="58"/>
-      <c r="F9" s="59"/>
-      <c r="H9" s="57"/>
-      <c r="I9" s="58"/>
-      <c r="J9" s="58"/>
-      <c r="K9" s="58"/>
-      <c r="L9" s="59"/>
-      <c r="N9" s="57"/>
-      <c r="O9" s="58"/>
-      <c r="P9" s="58"/>
-      <c r="Q9" s="58"/>
-      <c r="R9" s="59"/>
+      <c r="B9" s="62"/>
+      <c r="C9" s="63"/>
+      <c r="D9" s="63"/>
+      <c r="E9" s="63"/>
+      <c r="F9" s="64"/>
+      <c r="H9" s="62"/>
+      <c r="I9" s="63"/>
+      <c r="J9" s="63"/>
+      <c r="K9" s="63"/>
+      <c r="L9" s="64"/>
+      <c r="N9" s="62"/>
+      <c r="O9" s="63"/>
+      <c r="P9" s="63"/>
+      <c r="Q9" s="63"/>
+      <c r="R9" s="64"/>
     </row>
     <row r="10" spans="1:18">
       <c r="B10" s="5"/>
@@ -3683,226 +4047,226 @@
     </row>
     <row r="11" spans="1:18" ht="14.7" thickBot="1"/>
     <row r="12" spans="1:18" ht="16" customHeight="1">
-      <c r="B12" s="60" t="s">
+      <c r="B12" s="38" t="s">
         <v>102</v>
       </c>
-      <c r="C12" s="61"/>
-      <c r="D12" s="61"/>
-      <c r="E12" s="61"/>
-      <c r="F12" s="62"/>
-      <c r="H12" s="84" t="s">
+      <c r="C12" s="39"/>
+      <c r="D12" s="39"/>
+      <c r="E12" s="39"/>
+      <c r="F12" s="40"/>
+      <c r="H12" s="65" t="s">
         <v>102</v>
       </c>
-      <c r="I12" s="85"/>
-      <c r="J12" s="85"/>
-      <c r="K12" s="85"/>
-      <c r="L12" s="86"/>
-      <c r="N12" s="90" t="s">
+      <c r="I12" s="66"/>
+      <c r="J12" s="66"/>
+      <c r="K12" s="66"/>
+      <c r="L12" s="67"/>
+      <c r="N12" s="71" t="s">
         <v>102</v>
       </c>
-      <c r="O12" s="91"/>
-      <c r="P12" s="91"/>
-      <c r="Q12" s="91"/>
-      <c r="R12" s="92"/>
+      <c r="O12" s="72"/>
+      <c r="P12" s="72"/>
+      <c r="Q12" s="72"/>
+      <c r="R12" s="73"/>
     </row>
     <row r="13" spans="1:18" ht="16" customHeight="1">
-      <c r="B13" s="63"/>
-      <c r="C13" s="64"/>
-      <c r="D13" s="64"/>
-      <c r="E13" s="64"/>
-      <c r="F13" s="65"/>
-      <c r="H13" s="87"/>
-      <c r="I13" s="88"/>
-      <c r="J13" s="88"/>
-      <c r="K13" s="88"/>
-      <c r="L13" s="89"/>
-      <c r="N13" s="93"/>
-      <c r="O13" s="94"/>
-      <c r="P13" s="94"/>
-      <c r="Q13" s="94"/>
-      <c r="R13" s="95"/>
+      <c r="B13" s="41"/>
+      <c r="C13" s="42"/>
+      <c r="D13" s="42"/>
+      <c r="E13" s="42"/>
+      <c r="F13" s="43"/>
+      <c r="H13" s="68"/>
+      <c r="I13" s="69"/>
+      <c r="J13" s="69"/>
+      <c r="K13" s="69"/>
+      <c r="L13" s="70"/>
+      <c r="N13" s="74"/>
+      <c r="O13" s="75"/>
+      <c r="P13" s="75"/>
+      <c r="Q13" s="75"/>
+      <c r="R13" s="76"/>
     </row>
     <row r="14" spans="1:18" ht="16" customHeight="1">
-      <c r="B14" s="41" t="s">
+      <c r="B14" s="77" t="s">
         <v>103</v>
       </c>
-      <c r="C14" s="42"/>
-      <c r="D14" s="42"/>
-      <c r="E14" s="42"/>
-      <c r="F14" s="43"/>
-      <c r="H14" s="41" t="s">
+      <c r="C14" s="78"/>
+      <c r="D14" s="78"/>
+      <c r="E14" s="78"/>
+      <c r="F14" s="79"/>
+      <c r="H14" s="77" t="s">
         <v>104</v>
       </c>
-      <c r="I14" s="42"/>
-      <c r="J14" s="42"/>
-      <c r="K14" s="42"/>
-      <c r="L14" s="43"/>
-      <c r="N14" s="41" t="s">
+      <c r="I14" s="78"/>
+      <c r="J14" s="78"/>
+      <c r="K14" s="78"/>
+      <c r="L14" s="79"/>
+      <c r="N14" s="77" t="s">
         <v>105</v>
       </c>
-      <c r="O14" s="42"/>
-      <c r="P14" s="42"/>
-      <c r="Q14" s="42"/>
-      <c r="R14" s="43"/>
+      <c r="O14" s="78"/>
+      <c r="P14" s="78"/>
+      <c r="Q14" s="78"/>
+      <c r="R14" s="79"/>
     </row>
     <row r="15" spans="1:18">
-      <c r="B15" s="44"/>
-      <c r="C15" s="45"/>
-      <c r="D15" s="45"/>
-      <c r="E15" s="45"/>
-      <c r="F15" s="46"/>
-      <c r="H15" s="44"/>
-      <c r="I15" s="45"/>
-      <c r="J15" s="45"/>
-      <c r="K15" s="45"/>
-      <c r="L15" s="46"/>
-      <c r="N15" s="44"/>
-      <c r="O15" s="45"/>
-      <c r="P15" s="45"/>
-      <c r="Q15" s="45"/>
-      <c r="R15" s="46"/>
+      <c r="B15" s="80"/>
+      <c r="C15" s="81"/>
+      <c r="D15" s="81"/>
+      <c r="E15" s="81"/>
+      <c r="F15" s="82"/>
+      <c r="H15" s="80"/>
+      <c r="I15" s="81"/>
+      <c r="J15" s="81"/>
+      <c r="K15" s="81"/>
+      <c r="L15" s="82"/>
+      <c r="N15" s="80"/>
+      <c r="O15" s="81"/>
+      <c r="P15" s="81"/>
+      <c r="Q15" s="81"/>
+      <c r="R15" s="82"/>
     </row>
     <row r="16" spans="1:18">
-      <c r="B16" s="44"/>
-      <c r="C16" s="45"/>
-      <c r="D16" s="45"/>
-      <c r="E16" s="45"/>
-      <c r="F16" s="46"/>
-      <c r="H16" s="44"/>
-      <c r="I16" s="45"/>
-      <c r="J16" s="45"/>
-      <c r="K16" s="45"/>
-      <c r="L16" s="46"/>
-      <c r="N16" s="44"/>
-      <c r="O16" s="45"/>
-      <c r="P16" s="45"/>
-      <c r="Q16" s="45"/>
-      <c r="R16" s="46"/>
+      <c r="B16" s="80"/>
+      <c r="C16" s="81"/>
+      <c r="D16" s="81"/>
+      <c r="E16" s="81"/>
+      <c r="F16" s="82"/>
+      <c r="H16" s="80"/>
+      <c r="I16" s="81"/>
+      <c r="J16" s="81"/>
+      <c r="K16" s="81"/>
+      <c r="L16" s="82"/>
+      <c r="N16" s="80"/>
+      <c r="O16" s="81"/>
+      <c r="P16" s="81"/>
+      <c r="Q16" s="81"/>
+      <c r="R16" s="82"/>
     </row>
     <row r="17" spans="2:18">
-      <c r="B17" s="44"/>
-      <c r="C17" s="45"/>
-      <c r="D17" s="45"/>
-      <c r="E17" s="45"/>
-      <c r="F17" s="46"/>
-      <c r="H17" s="44"/>
-      <c r="I17" s="45"/>
-      <c r="J17" s="45"/>
-      <c r="K17" s="45"/>
-      <c r="L17" s="46"/>
-      <c r="N17" s="44"/>
-      <c r="O17" s="45"/>
-      <c r="P17" s="45"/>
-      <c r="Q17" s="45"/>
-      <c r="R17" s="46"/>
+      <c r="B17" s="80"/>
+      <c r="C17" s="81"/>
+      <c r="D17" s="81"/>
+      <c r="E17" s="81"/>
+      <c r="F17" s="82"/>
+      <c r="H17" s="80"/>
+      <c r="I17" s="81"/>
+      <c r="J17" s="81"/>
+      <c r="K17" s="81"/>
+      <c r="L17" s="82"/>
+      <c r="N17" s="80"/>
+      <c r="O17" s="81"/>
+      <c r="P17" s="81"/>
+      <c r="Q17" s="81"/>
+      <c r="R17" s="82"/>
     </row>
     <row r="18" spans="2:18">
-      <c r="B18" s="47"/>
-      <c r="C18" s="48"/>
-      <c r="D18" s="48"/>
-      <c r="E18" s="48"/>
-      <c r="F18" s="49"/>
-      <c r="H18" s="47"/>
-      <c r="I18" s="48"/>
-      <c r="J18" s="48"/>
-      <c r="K18" s="48"/>
-      <c r="L18" s="49"/>
-      <c r="N18" s="47"/>
-      <c r="O18" s="48"/>
-      <c r="P18" s="48"/>
-      <c r="Q18" s="48"/>
-      <c r="R18" s="49"/>
+      <c r="B18" s="83"/>
+      <c r="C18" s="84"/>
+      <c r="D18" s="84"/>
+      <c r="E18" s="84"/>
+      <c r="F18" s="85"/>
+      <c r="H18" s="83"/>
+      <c r="I18" s="84"/>
+      <c r="J18" s="84"/>
+      <c r="K18" s="84"/>
+      <c r="L18" s="85"/>
+      <c r="N18" s="83"/>
+      <c r="O18" s="84"/>
+      <c r="P18" s="84"/>
+      <c r="Q18" s="84"/>
+      <c r="R18" s="85"/>
     </row>
     <row r="19" spans="2:18" ht="16" customHeight="1">
-      <c r="B19" s="41" t="s">
+      <c r="B19" s="77" t="s">
         <v>106</v>
       </c>
-      <c r="C19" s="42"/>
-      <c r="D19" s="42"/>
-      <c r="E19" s="42"/>
-      <c r="F19" s="43"/>
-      <c r="H19" s="41" t="s">
+      <c r="C19" s="78"/>
+      <c r="D19" s="78"/>
+      <c r="E19" s="78"/>
+      <c r="F19" s="79"/>
+      <c r="H19" s="77" t="s">
         <v>106</v>
       </c>
-      <c r="I19" s="42"/>
-      <c r="J19" s="42"/>
-      <c r="K19" s="42"/>
-      <c r="L19" s="43"/>
-      <c r="N19" s="41" t="s">
+      <c r="I19" s="78"/>
+      <c r="J19" s="78"/>
+      <c r="K19" s="78"/>
+      <c r="L19" s="79"/>
+      <c r="N19" s="77" t="s">
         <v>107</v>
       </c>
-      <c r="O19" s="42"/>
-      <c r="P19" s="42"/>
-      <c r="Q19" s="42"/>
-      <c r="R19" s="43"/>
+      <c r="O19" s="78"/>
+      <c r="P19" s="78"/>
+      <c r="Q19" s="78"/>
+      <c r="R19" s="79"/>
     </row>
     <row r="20" spans="2:18">
-      <c r="B20" s="44"/>
-      <c r="C20" s="45"/>
-      <c r="D20" s="45"/>
-      <c r="E20" s="45"/>
-      <c r="F20" s="46"/>
-      <c r="H20" s="44"/>
-      <c r="I20" s="45"/>
-      <c r="J20" s="45"/>
-      <c r="K20" s="45"/>
-      <c r="L20" s="46"/>
-      <c r="N20" s="44"/>
-      <c r="O20" s="45"/>
-      <c r="P20" s="45"/>
-      <c r="Q20" s="45"/>
-      <c r="R20" s="46"/>
+      <c r="B20" s="80"/>
+      <c r="C20" s="81"/>
+      <c r="D20" s="81"/>
+      <c r="E20" s="81"/>
+      <c r="F20" s="82"/>
+      <c r="H20" s="80"/>
+      <c r="I20" s="81"/>
+      <c r="J20" s="81"/>
+      <c r="K20" s="81"/>
+      <c r="L20" s="82"/>
+      <c r="N20" s="80"/>
+      <c r="O20" s="81"/>
+      <c r="P20" s="81"/>
+      <c r="Q20" s="81"/>
+      <c r="R20" s="82"/>
     </row>
     <row r="21" spans="2:18">
-      <c r="B21" s="44"/>
-      <c r="C21" s="45"/>
-      <c r="D21" s="45"/>
-      <c r="E21" s="45"/>
-      <c r="F21" s="46"/>
-      <c r="H21" s="44"/>
-      <c r="I21" s="45"/>
-      <c r="J21" s="45"/>
-      <c r="K21" s="45"/>
-      <c r="L21" s="46"/>
-      <c r="N21" s="44"/>
-      <c r="O21" s="45"/>
-      <c r="P21" s="45"/>
-      <c r="Q21" s="45"/>
-      <c r="R21" s="46"/>
+      <c r="B21" s="80"/>
+      <c r="C21" s="81"/>
+      <c r="D21" s="81"/>
+      <c r="E21" s="81"/>
+      <c r="F21" s="82"/>
+      <c r="H21" s="80"/>
+      <c r="I21" s="81"/>
+      <c r="J21" s="81"/>
+      <c r="K21" s="81"/>
+      <c r="L21" s="82"/>
+      <c r="N21" s="80"/>
+      <c r="O21" s="81"/>
+      <c r="P21" s="81"/>
+      <c r="Q21" s="81"/>
+      <c r="R21" s="82"/>
     </row>
     <row r="22" spans="2:18">
-      <c r="B22" s="44"/>
-      <c r="C22" s="45"/>
-      <c r="D22" s="45"/>
-      <c r="E22" s="45"/>
-      <c r="F22" s="46"/>
-      <c r="H22" s="44"/>
-      <c r="I22" s="45"/>
-      <c r="J22" s="45"/>
-      <c r="K22" s="45"/>
-      <c r="L22" s="46"/>
-      <c r="N22" s="44"/>
-      <c r="O22" s="45"/>
-      <c r="P22" s="45"/>
-      <c r="Q22" s="45"/>
-      <c r="R22" s="46"/>
+      <c r="B22" s="80"/>
+      <c r="C22" s="81"/>
+      <c r="D22" s="81"/>
+      <c r="E22" s="81"/>
+      <c r="F22" s="82"/>
+      <c r="H22" s="80"/>
+      <c r="I22" s="81"/>
+      <c r="J22" s="81"/>
+      <c r="K22" s="81"/>
+      <c r="L22" s="82"/>
+      <c r="N22" s="80"/>
+      <c r="O22" s="81"/>
+      <c r="P22" s="81"/>
+      <c r="Q22" s="81"/>
+      <c r="R22" s="82"/>
     </row>
     <row r="23" spans="2:18">
-      <c r="B23" s="47"/>
-      <c r="C23" s="48"/>
-      <c r="D23" s="48"/>
-      <c r="E23" s="48"/>
-      <c r="F23" s="49"/>
-      <c r="H23" s="47"/>
-      <c r="I23" s="48"/>
-      <c r="J23" s="48"/>
-      <c r="K23" s="48"/>
-      <c r="L23" s="49"/>
-      <c r="N23" s="47"/>
-      <c r="O23" s="48"/>
-      <c r="P23" s="48"/>
-      <c r="Q23" s="48"/>
-      <c r="R23" s="49"/>
+      <c r="B23" s="83"/>
+      <c r="C23" s="84"/>
+      <c r="D23" s="84"/>
+      <c r="E23" s="84"/>
+      <c r="F23" s="85"/>
+      <c r="H23" s="83"/>
+      <c r="I23" s="84"/>
+      <c r="J23" s="84"/>
+      <c r="K23" s="84"/>
+      <c r="L23" s="85"/>
+      <c r="N23" s="83"/>
+      <c r="O23" s="84"/>
+      <c r="P23" s="84"/>
+      <c r="Q23" s="84"/>
+      <c r="R23" s="85"/>
     </row>
     <row r="26" spans="2:18" ht="18.3">
       <c r="B26" s="6" t="s">
@@ -4068,341 +4432,341 @@
     </row>
     <row r="37" spans="2:18" ht="14.7" thickBot="1"/>
     <row r="38" spans="2:18">
-      <c r="B38" s="60" t="s">
+      <c r="B38" s="38" t="s">
         <v>117</v>
       </c>
-      <c r="C38" s="61"/>
-      <c r="D38" s="61"/>
-      <c r="E38" s="61"/>
-      <c r="F38" s="62"/>
-      <c r="H38" s="78" t="s">
+      <c r="C38" s="39"/>
+      <c r="D38" s="39"/>
+      <c r="E38" s="39"/>
+      <c r="F38" s="40"/>
+      <c r="H38" s="86" t="s">
         <v>118</v>
       </c>
-      <c r="I38" s="79"/>
-      <c r="J38" s="79"/>
-      <c r="K38" s="79"/>
-      <c r="L38" s="80"/>
-      <c r="N38" s="72" t="s">
+      <c r="I38" s="87"/>
+      <c r="J38" s="87"/>
+      <c r="K38" s="87"/>
+      <c r="L38" s="88"/>
+      <c r="N38" s="50" t="s">
         <v>119</v>
       </c>
-      <c r="O38" s="73"/>
-      <c r="P38" s="73"/>
-      <c r="Q38" s="73"/>
-      <c r="R38" s="74"/>
+      <c r="O38" s="51"/>
+      <c r="P38" s="51"/>
+      <c r="Q38" s="51"/>
+      <c r="R38" s="52"/>
     </row>
     <row r="39" spans="2:18" ht="14.7" thickBot="1">
-      <c r="B39" s="63"/>
-      <c r="C39" s="64"/>
-      <c r="D39" s="64"/>
-      <c r="E39" s="64"/>
-      <c r="F39" s="65"/>
-      <c r="H39" s="81"/>
-      <c r="I39" s="82"/>
-      <c r="J39" s="82"/>
-      <c r="K39" s="82"/>
-      <c r="L39" s="83"/>
-      <c r="N39" s="75"/>
-      <c r="O39" s="76"/>
-      <c r="P39" s="76"/>
-      <c r="Q39" s="76"/>
-      <c r="R39" s="77"/>
+      <c r="B39" s="41"/>
+      <c r="C39" s="42"/>
+      <c r="D39" s="42"/>
+      <c r="E39" s="42"/>
+      <c r="F39" s="43"/>
+      <c r="H39" s="89"/>
+      <c r="I39" s="90"/>
+      <c r="J39" s="90"/>
+      <c r="K39" s="90"/>
+      <c r="L39" s="91"/>
+      <c r="N39" s="53"/>
+      <c r="O39" s="54"/>
+      <c r="P39" s="54"/>
+      <c r="Q39" s="54"/>
+      <c r="R39" s="55"/>
     </row>
     <row r="40" spans="2:18">
-      <c r="B40" s="51" t="s">
+      <c r="B40" s="56" t="s">
         <v>120</v>
       </c>
-      <c r="C40" s="52"/>
-      <c r="D40" s="52"/>
-      <c r="E40" s="52"/>
-      <c r="F40" s="53"/>
-      <c r="H40" s="51" t="s">
+      <c r="C40" s="57"/>
+      <c r="D40" s="57"/>
+      <c r="E40" s="57"/>
+      <c r="F40" s="58"/>
+      <c r="H40" s="56" t="s">
         <v>121</v>
       </c>
-      <c r="I40" s="52"/>
-      <c r="J40" s="52"/>
-      <c r="K40" s="52"/>
-      <c r="L40" s="53"/>
-      <c r="N40" s="51" t="s">
+      <c r="I40" s="57"/>
+      <c r="J40" s="57"/>
+      <c r="K40" s="57"/>
+      <c r="L40" s="58"/>
+      <c r="N40" s="56" t="s">
         <v>122</v>
       </c>
-      <c r="O40" s="52"/>
-      <c r="P40" s="52"/>
-      <c r="Q40" s="52"/>
-      <c r="R40" s="53"/>
+      <c r="O40" s="57"/>
+      <c r="P40" s="57"/>
+      <c r="Q40" s="57"/>
+      <c r="R40" s="58"/>
     </row>
     <row r="41" spans="2:18">
-      <c r="B41" s="54"/>
-      <c r="C41" s="55"/>
-      <c r="D41" s="55"/>
-      <c r="E41" s="55"/>
-      <c r="F41" s="56"/>
-      <c r="H41" s="54"/>
-      <c r="I41" s="55"/>
-      <c r="J41" s="55"/>
-      <c r="K41" s="55"/>
-      <c r="L41" s="56"/>
-      <c r="N41" s="54"/>
-      <c r="O41" s="55"/>
-      <c r="P41" s="55"/>
-      <c r="Q41" s="55"/>
-      <c r="R41" s="56"/>
+      <c r="B41" s="59"/>
+      <c r="C41" s="60"/>
+      <c r="D41" s="60"/>
+      <c r="E41" s="60"/>
+      <c r="F41" s="61"/>
+      <c r="H41" s="59"/>
+      <c r="I41" s="60"/>
+      <c r="J41" s="60"/>
+      <c r="K41" s="60"/>
+      <c r="L41" s="61"/>
+      <c r="N41" s="59"/>
+      <c r="O41" s="60"/>
+      <c r="P41" s="60"/>
+      <c r="Q41" s="60"/>
+      <c r="R41" s="61"/>
     </row>
     <row r="42" spans="2:18">
-      <c r="B42" s="54"/>
-      <c r="C42" s="55"/>
-      <c r="D42" s="55"/>
-      <c r="E42" s="55"/>
-      <c r="F42" s="56"/>
-      <c r="H42" s="54"/>
-      <c r="I42" s="55"/>
-      <c r="J42" s="55"/>
-      <c r="K42" s="55"/>
-      <c r="L42" s="56"/>
-      <c r="N42" s="54"/>
-      <c r="O42" s="55"/>
-      <c r="P42" s="55"/>
-      <c r="Q42" s="55"/>
-      <c r="R42" s="56"/>
+      <c r="B42" s="59"/>
+      <c r="C42" s="60"/>
+      <c r="D42" s="60"/>
+      <c r="E42" s="60"/>
+      <c r="F42" s="61"/>
+      <c r="H42" s="59"/>
+      <c r="I42" s="60"/>
+      <c r="J42" s="60"/>
+      <c r="K42" s="60"/>
+      <c r="L42" s="61"/>
+      <c r="N42" s="59"/>
+      <c r="O42" s="60"/>
+      <c r="P42" s="60"/>
+      <c r="Q42" s="60"/>
+      <c r="R42" s="61"/>
     </row>
     <row r="43" spans="2:18">
-      <c r="B43" s="57"/>
-      <c r="C43" s="58"/>
-      <c r="D43" s="58"/>
-      <c r="E43" s="58"/>
-      <c r="F43" s="59"/>
-      <c r="H43" s="57"/>
-      <c r="I43" s="58"/>
-      <c r="J43" s="58"/>
-      <c r="K43" s="58"/>
-      <c r="L43" s="59"/>
-      <c r="N43" s="57"/>
-      <c r="O43" s="58"/>
-      <c r="P43" s="58"/>
-      <c r="Q43" s="58"/>
-      <c r="R43" s="59"/>
+      <c r="B43" s="62"/>
+      <c r="C43" s="63"/>
+      <c r="D43" s="63"/>
+      <c r="E43" s="63"/>
+      <c r="F43" s="64"/>
+      <c r="H43" s="62"/>
+      <c r="I43" s="63"/>
+      <c r="J43" s="63"/>
+      <c r="K43" s="63"/>
+      <c r="L43" s="64"/>
+      <c r="N43" s="62"/>
+      <c r="O43" s="63"/>
+      <c r="P43" s="63"/>
+      <c r="Q43" s="63"/>
+      <c r="R43" s="64"/>
     </row>
     <row r="45" spans="2:18" ht="14.7" thickBot="1"/>
     <row r="46" spans="2:18" ht="16" customHeight="1">
-      <c r="B46" s="60" t="s">
+      <c r="B46" s="38" t="s">
         <v>102</v>
       </c>
-      <c r="C46" s="61"/>
-      <c r="D46" s="61"/>
-      <c r="E46" s="61"/>
-      <c r="F46" s="62"/>
-      <c r="H46" s="66" t="s">
+      <c r="C46" s="39"/>
+      <c r="D46" s="39"/>
+      <c r="E46" s="39"/>
+      <c r="F46" s="40"/>
+      <c r="H46" s="92" t="s">
         <v>102</v>
       </c>
-      <c r="I46" s="67"/>
-      <c r="J46" s="67"/>
-      <c r="K46" s="67"/>
-      <c r="L46" s="68"/>
-      <c r="N46" s="72" t="s">
+      <c r="I46" s="93"/>
+      <c r="J46" s="93"/>
+      <c r="K46" s="93"/>
+      <c r="L46" s="94"/>
+      <c r="N46" s="50" t="s">
         <v>102</v>
       </c>
-      <c r="O46" s="73"/>
-      <c r="P46" s="73"/>
-      <c r="Q46" s="73"/>
-      <c r="R46" s="74"/>
+      <c r="O46" s="51"/>
+      <c r="P46" s="51"/>
+      <c r="Q46" s="51"/>
+      <c r="R46" s="52"/>
     </row>
     <row r="47" spans="2:18" ht="16" customHeight="1" thickBot="1">
-      <c r="B47" s="63"/>
-      <c r="C47" s="64"/>
-      <c r="D47" s="64"/>
-      <c r="E47" s="64"/>
-      <c r="F47" s="65"/>
-      <c r="H47" s="69"/>
-      <c r="I47" s="70"/>
-      <c r="J47" s="70"/>
-      <c r="K47" s="70"/>
-      <c r="L47" s="71"/>
-      <c r="N47" s="75"/>
-      <c r="O47" s="76"/>
-      <c r="P47" s="76"/>
-      <c r="Q47" s="76"/>
-      <c r="R47" s="77"/>
+      <c r="B47" s="41"/>
+      <c r="C47" s="42"/>
+      <c r="D47" s="42"/>
+      <c r="E47" s="42"/>
+      <c r="F47" s="43"/>
+      <c r="H47" s="95"/>
+      <c r="I47" s="96"/>
+      <c r="J47" s="96"/>
+      <c r="K47" s="96"/>
+      <c r="L47" s="97"/>
+      <c r="N47" s="53"/>
+      <c r="O47" s="54"/>
+      <c r="P47" s="54"/>
+      <c r="Q47" s="54"/>
+      <c r="R47" s="55"/>
     </row>
     <row r="48" spans="2:18">
-      <c r="B48" s="41" t="s">
+      <c r="B48" s="77" t="s">
         <v>123</v>
       </c>
-      <c r="C48" s="42"/>
-      <c r="D48" s="42"/>
-      <c r="E48" s="42"/>
-      <c r="F48" s="43"/>
-      <c r="H48" s="50" t="s">
+      <c r="C48" s="78"/>
+      <c r="D48" s="78"/>
+      <c r="E48" s="78"/>
+      <c r="F48" s="79"/>
+      <c r="H48" s="101" t="s">
         <v>124</v>
       </c>
-      <c r="I48" s="42"/>
-      <c r="J48" s="42"/>
-      <c r="K48" s="42"/>
-      <c r="L48" s="43"/>
-      <c r="N48" s="41" t="s">
+      <c r="I48" s="78"/>
+      <c r="J48" s="78"/>
+      <c r="K48" s="78"/>
+      <c r="L48" s="79"/>
+      <c r="N48" s="77" t="s">
         <v>125</v>
       </c>
-      <c r="O48" s="42"/>
-      <c r="P48" s="42"/>
-      <c r="Q48" s="42"/>
-      <c r="R48" s="43"/>
+      <c r="O48" s="78"/>
+      <c r="P48" s="78"/>
+      <c r="Q48" s="78"/>
+      <c r="R48" s="79"/>
     </row>
     <row r="49" spans="2:18">
-      <c r="B49" s="44"/>
-      <c r="C49" s="45"/>
-      <c r="D49" s="45"/>
-      <c r="E49" s="45"/>
-      <c r="F49" s="46"/>
-      <c r="H49" s="44"/>
-      <c r="I49" s="45"/>
-      <c r="J49" s="45"/>
-      <c r="K49" s="45"/>
-      <c r="L49" s="46"/>
-      <c r="N49" s="44"/>
-      <c r="O49" s="45"/>
-      <c r="P49" s="45"/>
-      <c r="Q49" s="45"/>
-      <c r="R49" s="46"/>
+      <c r="B49" s="80"/>
+      <c r="C49" s="81"/>
+      <c r="D49" s="81"/>
+      <c r="E49" s="81"/>
+      <c r="F49" s="82"/>
+      <c r="H49" s="80"/>
+      <c r="I49" s="81"/>
+      <c r="J49" s="81"/>
+      <c r="K49" s="81"/>
+      <c r="L49" s="82"/>
+      <c r="N49" s="80"/>
+      <c r="O49" s="81"/>
+      <c r="P49" s="81"/>
+      <c r="Q49" s="81"/>
+      <c r="R49" s="82"/>
     </row>
     <row r="50" spans="2:18">
-      <c r="B50" s="44"/>
-      <c r="C50" s="45"/>
-      <c r="D50" s="45"/>
-      <c r="E50" s="45"/>
-      <c r="F50" s="46"/>
-      <c r="H50" s="44"/>
-      <c r="I50" s="45"/>
-      <c r="J50" s="45"/>
-      <c r="K50" s="45"/>
-      <c r="L50" s="46"/>
-      <c r="N50" s="44"/>
-      <c r="O50" s="45"/>
-      <c r="P50" s="45"/>
-      <c r="Q50" s="45"/>
-      <c r="R50" s="46"/>
+      <c r="B50" s="80"/>
+      <c r="C50" s="81"/>
+      <c r="D50" s="81"/>
+      <c r="E50" s="81"/>
+      <c r="F50" s="82"/>
+      <c r="H50" s="80"/>
+      <c r="I50" s="81"/>
+      <c r="J50" s="81"/>
+      <c r="K50" s="81"/>
+      <c r="L50" s="82"/>
+      <c r="N50" s="80"/>
+      <c r="O50" s="81"/>
+      <c r="P50" s="81"/>
+      <c r="Q50" s="81"/>
+      <c r="R50" s="82"/>
     </row>
     <row r="51" spans="2:18">
-      <c r="B51" s="44"/>
-      <c r="C51" s="45"/>
-      <c r="D51" s="45"/>
-      <c r="E51" s="45"/>
-      <c r="F51" s="46"/>
-      <c r="H51" s="44"/>
-      <c r="I51" s="45"/>
-      <c r="J51" s="45"/>
-      <c r="K51" s="45"/>
-      <c r="L51" s="46"/>
-      <c r="N51" s="44"/>
-      <c r="O51" s="45"/>
-      <c r="P51" s="45"/>
-      <c r="Q51" s="45"/>
-      <c r="R51" s="46"/>
+      <c r="B51" s="80"/>
+      <c r="C51" s="81"/>
+      <c r="D51" s="81"/>
+      <c r="E51" s="81"/>
+      <c r="F51" s="82"/>
+      <c r="H51" s="80"/>
+      <c r="I51" s="81"/>
+      <c r="J51" s="81"/>
+      <c r="K51" s="81"/>
+      <c r="L51" s="82"/>
+      <c r="N51" s="80"/>
+      <c r="O51" s="81"/>
+      <c r="P51" s="81"/>
+      <c r="Q51" s="81"/>
+      <c r="R51" s="82"/>
     </row>
     <row r="52" spans="2:18">
-      <c r="B52" s="47"/>
-      <c r="C52" s="48"/>
-      <c r="D52" s="48"/>
-      <c r="E52" s="48"/>
-      <c r="F52" s="49"/>
-      <c r="H52" s="47"/>
-      <c r="I52" s="48"/>
-      <c r="J52" s="48"/>
-      <c r="K52" s="48"/>
-      <c r="L52" s="49"/>
-      <c r="N52" s="47"/>
-      <c r="O52" s="48"/>
-      <c r="P52" s="48"/>
-      <c r="Q52" s="48"/>
-      <c r="R52" s="49"/>
+      <c r="B52" s="83"/>
+      <c r="C52" s="84"/>
+      <c r="D52" s="84"/>
+      <c r="E52" s="84"/>
+      <c r="F52" s="85"/>
+      <c r="H52" s="83"/>
+      <c r="I52" s="84"/>
+      <c r="J52" s="84"/>
+      <c r="K52" s="84"/>
+      <c r="L52" s="85"/>
+      <c r="N52" s="83"/>
+      <c r="O52" s="84"/>
+      <c r="P52" s="84"/>
+      <c r="Q52" s="84"/>
+      <c r="R52" s="85"/>
     </row>
     <row r="53" spans="2:18">
-      <c r="B53" s="41" t="s">
+      <c r="B53" s="77" t="s">
         <v>126</v>
       </c>
-      <c r="C53" s="42"/>
-      <c r="D53" s="42"/>
-      <c r="E53" s="42"/>
-      <c r="F53" s="43"/>
-      <c r="H53" s="41" t="s">
+      <c r="C53" s="78"/>
+      <c r="D53" s="78"/>
+      <c r="E53" s="78"/>
+      <c r="F53" s="79"/>
+      <c r="H53" s="77" t="s">
         <v>127</v>
       </c>
-      <c r="I53" s="42"/>
-      <c r="J53" s="42"/>
-      <c r="K53" s="42"/>
-      <c r="L53" s="43"/>
-      <c r="N53" s="41" t="s">
+      <c r="I53" s="78"/>
+      <c r="J53" s="78"/>
+      <c r="K53" s="78"/>
+      <c r="L53" s="79"/>
+      <c r="N53" s="77" t="s">
         <v>128</v>
       </c>
-      <c r="O53" s="42"/>
-      <c r="P53" s="42"/>
-      <c r="Q53" s="42"/>
-      <c r="R53" s="43"/>
+      <c r="O53" s="78"/>
+      <c r="P53" s="78"/>
+      <c r="Q53" s="78"/>
+      <c r="R53" s="79"/>
     </row>
     <row r="54" spans="2:18">
-      <c r="B54" s="44"/>
-      <c r="C54" s="45"/>
-      <c r="D54" s="45"/>
-      <c r="E54" s="45"/>
-      <c r="F54" s="46"/>
-      <c r="H54" s="44"/>
-      <c r="I54" s="45"/>
-      <c r="J54" s="45"/>
-      <c r="K54" s="45"/>
-      <c r="L54" s="46"/>
-      <c r="N54" s="44"/>
-      <c r="O54" s="45"/>
-      <c r="P54" s="45"/>
-      <c r="Q54" s="45"/>
-      <c r="R54" s="46"/>
+      <c r="B54" s="80"/>
+      <c r="C54" s="81"/>
+      <c r="D54" s="81"/>
+      <c r="E54" s="81"/>
+      <c r="F54" s="82"/>
+      <c r="H54" s="80"/>
+      <c r="I54" s="81"/>
+      <c r="J54" s="81"/>
+      <c r="K54" s="81"/>
+      <c r="L54" s="82"/>
+      <c r="N54" s="80"/>
+      <c r="O54" s="81"/>
+      <c r="P54" s="81"/>
+      <c r="Q54" s="81"/>
+      <c r="R54" s="82"/>
     </row>
     <row r="55" spans="2:18">
-      <c r="B55" s="44"/>
-      <c r="C55" s="45"/>
-      <c r="D55" s="45"/>
-      <c r="E55" s="45"/>
-      <c r="F55" s="46"/>
-      <c r="H55" s="44"/>
-      <c r="I55" s="45"/>
-      <c r="J55" s="45"/>
-      <c r="K55" s="45"/>
-      <c r="L55" s="46"/>
-      <c r="N55" s="44"/>
-      <c r="O55" s="45"/>
-      <c r="P55" s="45"/>
-      <c r="Q55" s="45"/>
-      <c r="R55" s="46"/>
+      <c r="B55" s="80"/>
+      <c r="C55" s="81"/>
+      <c r="D55" s="81"/>
+      <c r="E55" s="81"/>
+      <c r="F55" s="82"/>
+      <c r="H55" s="80"/>
+      <c r="I55" s="81"/>
+      <c r="J55" s="81"/>
+      <c r="K55" s="81"/>
+      <c r="L55" s="82"/>
+      <c r="N55" s="80"/>
+      <c r="O55" s="81"/>
+      <c r="P55" s="81"/>
+      <c r="Q55" s="81"/>
+      <c r="R55" s="82"/>
     </row>
     <row r="56" spans="2:18">
-      <c r="B56" s="44"/>
-      <c r="C56" s="45"/>
-      <c r="D56" s="45"/>
-      <c r="E56" s="45"/>
-      <c r="F56" s="46"/>
-      <c r="H56" s="44"/>
-      <c r="I56" s="45"/>
-      <c r="J56" s="45"/>
-      <c r="K56" s="45"/>
-      <c r="L56" s="46"/>
-      <c r="N56" s="44"/>
-      <c r="O56" s="45"/>
-      <c r="P56" s="45"/>
-      <c r="Q56" s="45"/>
-      <c r="R56" s="46"/>
+      <c r="B56" s="80"/>
+      <c r="C56" s="81"/>
+      <c r="D56" s="81"/>
+      <c r="E56" s="81"/>
+      <c r="F56" s="82"/>
+      <c r="H56" s="80"/>
+      <c r="I56" s="81"/>
+      <c r="J56" s="81"/>
+      <c r="K56" s="81"/>
+      <c r="L56" s="82"/>
+      <c r="N56" s="80"/>
+      <c r="O56" s="81"/>
+      <c r="P56" s="81"/>
+      <c r="Q56" s="81"/>
+      <c r="R56" s="82"/>
     </row>
     <row r="57" spans="2:18">
-      <c r="B57" s="47"/>
-      <c r="C57" s="48"/>
-      <c r="D57" s="48"/>
-      <c r="E57" s="48"/>
-      <c r="F57" s="49"/>
-      <c r="H57" s="47"/>
-      <c r="I57" s="48"/>
-      <c r="J57" s="48"/>
-      <c r="K57" s="48"/>
-      <c r="L57" s="49"/>
-      <c r="N57" s="47"/>
-      <c r="O57" s="48"/>
-      <c r="P57" s="48"/>
-      <c r="Q57" s="48"/>
-      <c r="R57" s="49"/>
+      <c r="B57" s="83"/>
+      <c r="C57" s="84"/>
+      <c r="D57" s="84"/>
+      <c r="E57" s="84"/>
+      <c r="F57" s="85"/>
+      <c r="H57" s="83"/>
+      <c r="I57" s="84"/>
+      <c r="J57" s="84"/>
+      <c r="K57" s="84"/>
+      <c r="L57" s="85"/>
+      <c r="N57" s="83"/>
+      <c r="O57" s="84"/>
+      <c r="P57" s="84"/>
+      <c r="Q57" s="84"/>
+      <c r="R57" s="85"/>
     </row>
     <row r="60" spans="2:18" ht="18.3">
       <c r="B60" s="6" t="s">
@@ -4575,13 +4939,13 @@
       <c r="R67" s="27"/>
     </row>
     <row r="70" spans="2:18" ht="15.6">
-      <c r="N70" s="38" t="s">
+      <c r="N70" s="98" t="s">
         <v>143</v>
       </c>
-      <c r="O70" s="39"/>
-      <c r="P70" s="39"/>
-      <c r="Q70" s="39"/>
-      <c r="R70" s="40"/>
+      <c r="O70" s="99"/>
+      <c r="P70" s="99"/>
+      <c r="Q70" s="99"/>
+      <c r="R70" s="100"/>
     </row>
     <row r="71" spans="2:18" ht="32.1" customHeight="1">
       <c r="N71" s="28"/>
@@ -4656,30 +5020,6 @@
     </row>
   </sheetData>
   <mergeCells count="31">
-    <mergeCell ref="B4:F5"/>
-    <mergeCell ref="H4:L5"/>
-    <mergeCell ref="N4:R5"/>
-    <mergeCell ref="B6:F9"/>
-    <mergeCell ref="H6:L9"/>
-    <mergeCell ref="N6:R9"/>
-    <mergeCell ref="B12:F13"/>
-    <mergeCell ref="H12:L13"/>
-    <mergeCell ref="N12:R13"/>
-    <mergeCell ref="B14:F18"/>
-    <mergeCell ref="H14:L18"/>
-    <mergeCell ref="N14:R18"/>
-    <mergeCell ref="B19:F23"/>
-    <mergeCell ref="H19:L23"/>
-    <mergeCell ref="N19:R23"/>
-    <mergeCell ref="B38:F39"/>
-    <mergeCell ref="H38:L39"/>
-    <mergeCell ref="N38:R39"/>
-    <mergeCell ref="B40:F43"/>
-    <mergeCell ref="H40:L43"/>
-    <mergeCell ref="N40:R43"/>
-    <mergeCell ref="B46:F47"/>
-    <mergeCell ref="H46:L47"/>
-    <mergeCell ref="N46:R47"/>
     <mergeCell ref="N70:R70"/>
     <mergeCell ref="B48:F52"/>
     <mergeCell ref="H48:L52"/>
@@ -4687,6 +5027,30 @@
     <mergeCell ref="B53:F57"/>
     <mergeCell ref="H53:L57"/>
     <mergeCell ref="N53:R57"/>
+    <mergeCell ref="B40:F43"/>
+    <mergeCell ref="H40:L43"/>
+    <mergeCell ref="N40:R43"/>
+    <mergeCell ref="B46:F47"/>
+    <mergeCell ref="H46:L47"/>
+    <mergeCell ref="N46:R47"/>
+    <mergeCell ref="B19:F23"/>
+    <mergeCell ref="H19:L23"/>
+    <mergeCell ref="N19:R23"/>
+    <mergeCell ref="B38:F39"/>
+    <mergeCell ref="H38:L39"/>
+    <mergeCell ref="N38:R39"/>
+    <mergeCell ref="B12:F13"/>
+    <mergeCell ref="H12:L13"/>
+    <mergeCell ref="N12:R13"/>
+    <mergeCell ref="B14:F18"/>
+    <mergeCell ref="H14:L18"/>
+    <mergeCell ref="N14:R18"/>
+    <mergeCell ref="B4:F5"/>
+    <mergeCell ref="H4:L5"/>
+    <mergeCell ref="N4:R5"/>
+    <mergeCell ref="B6:F9"/>
+    <mergeCell ref="H6:L9"/>
+    <mergeCell ref="N6:R9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>

</xml_diff>

<commit_message>
cambio quote + doc
</commit_message>
<xml_diff>
--- a/input/multiassets.xlsx
+++ b/input/multiassets.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/935cc860ba0efd68/GitHub/myportfolio/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="149" documentId="13_ncr:1_{B10D7187-5546-4483-8DEF-63838578FBF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{23B53F54-8431-4271-AE87-42DA6408CEF4}"/>
+  <xr:revisionPtr revIDLastSave="151" documentId="13_ncr:1_{B10D7187-5546-4483-8DEF-63838578FBF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0A13D085-46C6-46F1-9E9A-545B3413B1A2}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1768,122 +1768,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -1912,53 +1804,161 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -2247,9 +2247,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B015881-81C4-40D2-9396-65046E56EE7C}">
-  <dimension ref="A1:L10"/>
+  <dimension ref="A1:L9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
@@ -2447,19 +2449,19 @@
     </row>
     <row r="6" spans="1:12">
       <c r="A6" s="36" t="s">
-        <v>203</v>
+        <v>217</v>
       </c>
       <c r="B6" t="s">
-        <v>205</v>
+        <v>216</v>
       </c>
       <c r="C6" t="s">
-        <v>204</v>
+        <v>219</v>
       </c>
       <c r="D6" t="s">
-        <v>206</v>
+        <v>214</v>
       </c>
       <c r="E6" t="s">
-        <v>201</v>
+        <v>215</v>
       </c>
       <c r="F6" t="s">
         <v>17</v>
@@ -2468,10 +2470,10 @@
         <v>7</v>
       </c>
       <c r="H6" t="s">
-        <v>171</v>
-      </c>
-      <c r="I6" s="1" t="s">
-        <v>202</v>
+        <v>178</v>
+      </c>
+      <c r="I6" s="1">
+        <v>8.9999999999999998E-4</v>
       </c>
       <c r="J6" t="s">
         <v>34</v>
@@ -2479,19 +2481,19 @@
     </row>
     <row r="7" spans="1:12">
       <c r="A7" s="36" t="s">
-        <v>217</v>
+        <v>208</v>
       </c>
       <c r="B7" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
       <c r="C7" t="s">
-        <v>219</v>
+        <v>209</v>
       </c>
       <c r="D7" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="E7" t="s">
-        <v>215</v>
+        <v>207</v>
       </c>
       <c r="F7" t="s">
         <v>17</v>
@@ -2503,131 +2505,98 @@
         <v>178</v>
       </c>
       <c r="I7" s="1">
-        <v>8.9999999999999998E-4</v>
+        <v>1E-3</v>
       </c>
       <c r="J7" t="s">
-        <v>34</v>
+        <v>212</v>
+      </c>
+      <c r="K7" t="s">
+        <v>213</v>
       </c>
     </row>
     <row r="8" spans="1:12">
       <c r="A8" s="36" t="s">
-        <v>208</v>
+        <v>174</v>
       </c>
       <c r="B8" t="s">
-        <v>210</v>
+        <v>170</v>
       </c>
       <c r="C8" t="s">
-        <v>209</v>
+        <v>175</v>
       </c>
       <c r="D8" t="s">
-        <v>211</v>
+        <v>176</v>
       </c>
       <c r="E8" t="s">
-        <v>207</v>
+        <v>177</v>
       </c>
       <c r="F8" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="G8" t="s">
         <v>7</v>
       </c>
       <c r="H8" t="s">
-        <v>178</v>
+        <v>171</v>
       </c>
       <c r="I8" s="1">
-        <v>1E-3</v>
+        <v>6.9999999999999999E-4</v>
       </c>
       <c r="J8" t="s">
-        <v>212</v>
+        <v>34</v>
       </c>
       <c r="K8" t="s">
-        <v>213</v>
+        <v>85</v>
       </c>
     </row>
     <row r="9" spans="1:12">
       <c r="A9" s="36" t="s">
-        <v>174</v>
+        <v>182</v>
       </c>
       <c r="B9" t="s">
-        <v>170</v>
+        <v>75</v>
       </c>
       <c r="C9" t="s">
-        <v>175</v>
+        <v>180</v>
       </c>
       <c r="D9" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="E9" t="s">
-        <v>177</v>
+        <v>181</v>
       </c>
       <c r="F9" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="G9" t="s">
         <v>7</v>
       </c>
       <c r="H9" t="s">
-        <v>171</v>
+        <v>178</v>
       </c>
       <c r="I9" s="1">
-        <v>6.9999999999999999E-4</v>
+        <v>1.1999999999999999E-3</v>
       </c>
       <c r="J9" t="s">
-        <v>34</v>
+        <v>54</v>
       </c>
       <c r="K9" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12">
-      <c r="A10" s="36" t="s">
-        <v>182</v>
-      </c>
-      <c r="B10" t="s">
-        <v>75</v>
-      </c>
-      <c r="C10" t="s">
-        <v>180</v>
-      </c>
-      <c r="D10" t="s">
-        <v>179</v>
-      </c>
-      <c r="E10" t="s">
-        <v>181</v>
-      </c>
-      <c r="F10" t="s">
-        <v>17</v>
-      </c>
-      <c r="G10" t="s">
-        <v>7</v>
-      </c>
-      <c r="H10" t="s">
-        <v>178</v>
-      </c>
-      <c r="I10" s="1">
-        <v>1.1999999999999999E-3</v>
-      </c>
-      <c r="J10" t="s">
-        <v>54</v>
-      </c>
-      <c r="K10" t="s">
         <v>86</v>
       </c>
-      <c r="L10" t="s">
+      <c r="L9" t="s">
         <v>82</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A5" r:id="rId1" display="https://www.justetf.com/it/etf-profile.html?isin=IE00B3VTN290" xr:uid="{6AB80B8F-0CAF-4297-B9BB-D72ED9AFBF01}"/>
-    <hyperlink ref="A9" r:id="rId2" display="https://www.justetf.com/it/etf-profile.html?isin=IE00BGR7L912" xr:uid="{69029A56-B54E-49FD-A0F5-77171229A26E}"/>
-    <hyperlink ref="A10" r:id="rId3" display="https://www.justetf.com/it/etf-profile.html?isin=IE00B579F325" xr:uid="{42CB0A67-6EA5-4F8A-A191-29BAAE4A4956}"/>
+    <hyperlink ref="A8" r:id="rId2" display="https://www.justetf.com/it/etf-profile.html?isin=IE00BGR7L912" xr:uid="{69029A56-B54E-49FD-A0F5-77171229A26E}"/>
+    <hyperlink ref="A9" r:id="rId3" display="https://www.justetf.com/it/etf-profile.html?isin=IE00B579F325" xr:uid="{42CB0A67-6EA5-4F8A-A191-29BAAE4A4956}"/>
     <hyperlink ref="A3" r:id="rId4" display="https://www.justetf.com/it/etf-profile.html?isin=IE00BD1F4L37" xr:uid="{DF84D7C7-B8F6-477A-8C9A-D4997B54C865}"/>
     <hyperlink ref="A4" r:id="rId5" display="https://www.justetf.com/it/etf-profile.html?isin=IE00B8FHGS14" xr:uid="{47A684AB-EAC0-4609-B6F5-2C135D16A87D}"/>
-    <hyperlink ref="A6" r:id="rId6" display="https://www.justetf.com/it/etf-profile.html?isin=IE0032523478" xr:uid="{20C7AF50-87F2-4FC4-B8A4-93B98529FB55}"/>
-    <hyperlink ref="A8" r:id="rId7" display="https://finance.yahoo.com/quote/LEONIA.MI/" xr:uid="{C03B49D3-5D8D-4719-818C-85A9CCE78BAE}"/>
-    <hyperlink ref="A7" r:id="rId8" display="https://www.justetf.com/it/etf-profile.html?isin=IE00B0M62X26" xr:uid="{80E603FC-0B0D-4EAD-9D73-152F6C249FED}"/>
-    <hyperlink ref="A2" r:id="rId9" display="https://www.justetf.com/it/etf-profile.html?isin=IE00B4L5Y983" xr:uid="{07C799E5-4B70-419F-8A83-D91DFAD88307}"/>
+    <hyperlink ref="A7" r:id="rId6" display="https://finance.yahoo.com/quote/LEONIA.MI/" xr:uid="{C03B49D3-5D8D-4719-818C-85A9CCE78BAE}"/>
+    <hyperlink ref="A6" r:id="rId7" display="https://www.justetf.com/it/etf-profile.html?isin=IE00B0M62X26" xr:uid="{80E603FC-0B0D-4EAD-9D73-152F6C249FED}"/>
+    <hyperlink ref="A2" r:id="rId8" display="https://www.justetf.com/it/etf-profile.html?isin=IE00B4L5Y983" xr:uid="{07C799E5-4B70-419F-8A83-D91DFAD88307}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3052,10 +3021,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{222E099E-8C0E-4FA4-8471-33732A50ACAC}">
-  <dimension ref="A1:L14"/>
+  <dimension ref="A1:L15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -3494,10 +3463,43 @@
         <v>34</v>
       </c>
     </row>
+    <row r="15" spans="1:12">
+      <c r="A15" s="36" t="s">
+        <v>203</v>
+      </c>
+      <c r="B15" t="s">
+        <v>205</v>
+      </c>
+      <c r="C15" t="s">
+        <v>204</v>
+      </c>
+      <c r="D15" t="s">
+        <v>206</v>
+      </c>
+      <c r="E15" t="s">
+        <v>201</v>
+      </c>
+      <c r="F15" t="s">
+        <v>17</v>
+      </c>
+      <c r="G15" t="s">
+        <v>7</v>
+      </c>
+      <c r="H15" t="s">
+        <v>171</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="J15" t="s">
+        <v>34</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A13" r:id="rId1" display="https://www.justetf.com/it/etf-profile.html?isin=IE00BM67HN09" xr:uid="{910EFAF6-3CEE-4CB8-8783-0CCFA8F4D835}"/>
     <hyperlink ref="A14" r:id="rId2" display="https://www.justetf.com/it/etf-profile.html?isin=IE00BF4RFH31" xr:uid="{684559CE-9181-4573-92B0-6AF7C01E84D0}"/>
+    <hyperlink ref="A15" r:id="rId3" display="https://www.justetf.com/it/etf-profile.html?isin=IE0032523478" xr:uid="{20C7AF50-87F2-4FC4-B8A4-93B98529FB55}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3505,7 +3507,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{939D994C-0E7B-435F-BB4C-7162BD8072E3}">
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3513,11 +3515,11 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="str" cm="1">
-        <f t="array" ref="A1:A10">overview!E1:E10</f>
+        <f t="array" ref="A1:A9">overview!E1:E9</f>
         <v>Ticker</v>
       </c>
       <c r="B1" t="str" cm="1">
-        <f t="array" ref="B1:B10">overview!B1:B10</f>
+        <f t="array" ref="B1:B9">overview!B1:B9</f>
         <v>Index</v>
       </c>
     </row>
@@ -3555,41 +3557,33 @@
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="str">
-        <v>IBCX.AS</v>
+        <v>IBCI.AS</v>
       </c>
       <c r="B6" t="str">
-        <v>EU Corp Large Cap bonds</v>
+        <v>EU Inflation-Linked</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="str">
-        <v>IBCI.AS</v>
+        <v>LEONIA.MI</v>
       </c>
       <c r="B7" t="str">
-        <v>EU Inflation-Linked</v>
+        <v>EU Overnight</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="str">
-        <v>LEONIA.MI</v>
+        <v>IBTU.L</v>
       </c>
       <c r="B8" t="str">
-        <v>EU Overnight</v>
+        <v>US Short Treasury</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="str">
-        <v>IBTU.L</v>
+        <v>SGLD.AS</v>
       </c>
       <c r="B9" t="str">
-        <v>US Short Treasury</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2">
-      <c r="A10" t="str">
-        <v>SGLD.AS</v>
-      </c>
-      <c r="B10" t="str">
         <v>ETC GOLD</v>
       </c>
     </row>
@@ -3600,7 +3594,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA57C457-A80C-477F-8A3E-0F8DB96F6511}">
-  <dimension ref="A1:A10"/>
+  <dimension ref="A1:A9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -3610,7 +3604,7 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="str" cm="1">
-        <f t="array" ref="A1:A10">overview!C1:C10</f>
+        <f t="array" ref="A1:A9">overview!C1:C9</f>
         <v>Name</v>
       </c>
     </row>
@@ -3636,26 +3630,21 @@
     </row>
     <row r="6" spans="1:1">
       <c r="A6" t="str">
-        <v>iShares Euro Corporate Bond Large Cap UCITS ETF</v>
+        <v>iShares € Inflation Linked Govt Bond UCITS ETF EUR (Acc)</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" t="str">
-        <v>iShares € Inflation Linked Govt Bond UCITS ETF EUR (Acc)</v>
+        <v>Amundi EUR Overnight Return UCITS ETF Acc</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8" t="str">
-        <v>Amundi EUR Overnight Return UCITS ETF Acc</v>
+        <v>iShares USD Treasury Bond 0-1yr UCITS ETF (Dist)</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9" t="str">
-        <v>iShares USD Treasury Bond 0-1yr UCITS ETF (Dist)</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1">
-      <c r="A10" t="str">
         <v>Invesco Physical Gold ETC</v>
       </c>
     </row>
@@ -3915,118 +3904,118 @@
     </row>
     <row r="3" spans="1:18" ht="14.7" thickBot="1"/>
     <row r="4" spans="1:18" ht="16" customHeight="1">
-      <c r="B4" s="38" t="s">
+      <c r="B4" s="60" t="s">
         <v>97</v>
       </c>
-      <c r="C4" s="39"/>
-      <c r="D4" s="39"/>
-      <c r="E4" s="39"/>
-      <c r="F4" s="40"/>
-      <c r="H4" s="44" t="s">
+      <c r="C4" s="61"/>
+      <c r="D4" s="61"/>
+      <c r="E4" s="61"/>
+      <c r="F4" s="62"/>
+      <c r="H4" s="96" t="s">
         <v>98</v>
       </c>
-      <c r="I4" s="45"/>
-      <c r="J4" s="45"/>
-      <c r="K4" s="45"/>
-      <c r="L4" s="46"/>
-      <c r="N4" s="50" t="s">
+      <c r="I4" s="97"/>
+      <c r="J4" s="97"/>
+      <c r="K4" s="97"/>
+      <c r="L4" s="98"/>
+      <c r="N4" s="72" t="s">
         <v>99</v>
       </c>
-      <c r="O4" s="51"/>
-      <c r="P4" s="51"/>
-      <c r="Q4" s="51"/>
-      <c r="R4" s="52"/>
+      <c r="O4" s="73"/>
+      <c r="P4" s="73"/>
+      <c r="Q4" s="73"/>
+      <c r="R4" s="74"/>
     </row>
     <row r="5" spans="1:18" ht="17.100000000000001" customHeight="1" thickBot="1">
-      <c r="B5" s="41"/>
-      <c r="C5" s="42"/>
-      <c r="D5" s="42"/>
-      <c r="E5" s="42"/>
-      <c r="F5" s="43"/>
-      <c r="H5" s="47"/>
-      <c r="I5" s="48"/>
-      <c r="J5" s="48"/>
-      <c r="K5" s="48"/>
-      <c r="L5" s="49"/>
-      <c r="N5" s="53"/>
-      <c r="O5" s="54"/>
-      <c r="P5" s="54"/>
-      <c r="Q5" s="54"/>
-      <c r="R5" s="55"/>
+      <c r="B5" s="63"/>
+      <c r="C5" s="64"/>
+      <c r="D5" s="64"/>
+      <c r="E5" s="64"/>
+      <c r="F5" s="65"/>
+      <c r="H5" s="99"/>
+      <c r="I5" s="100"/>
+      <c r="J5" s="100"/>
+      <c r="K5" s="100"/>
+      <c r="L5" s="101"/>
+      <c r="N5" s="75"/>
+      <c r="O5" s="76"/>
+      <c r="P5" s="76"/>
+      <c r="Q5" s="76"/>
+      <c r="R5" s="77"/>
     </row>
     <row r="6" spans="1:18">
-      <c r="B6" s="56" t="s">
+      <c r="B6" s="51" t="s">
         <v>100</v>
       </c>
-      <c r="C6" s="57"/>
-      <c r="D6" s="57"/>
-      <c r="E6" s="57"/>
-      <c r="F6" s="58"/>
-      <c r="H6" s="56" t="s">
+      <c r="C6" s="52"/>
+      <c r="D6" s="52"/>
+      <c r="E6" s="52"/>
+      <c r="F6" s="53"/>
+      <c r="H6" s="51" t="s">
         <v>101</v>
       </c>
-      <c r="I6" s="57"/>
-      <c r="J6" s="57"/>
-      <c r="K6" s="57"/>
-      <c r="L6" s="58"/>
-      <c r="N6" s="56" t="s">
+      <c r="I6" s="52"/>
+      <c r="J6" s="52"/>
+      <c r="K6" s="52"/>
+      <c r="L6" s="53"/>
+      <c r="N6" s="51" t="s">
         <v>101</v>
       </c>
-      <c r="O6" s="57"/>
-      <c r="P6" s="57"/>
-      <c r="Q6" s="57"/>
-      <c r="R6" s="58"/>
+      <c r="O6" s="52"/>
+      <c r="P6" s="52"/>
+      <c r="Q6" s="52"/>
+      <c r="R6" s="53"/>
     </row>
     <row r="7" spans="1:18">
-      <c r="B7" s="59"/>
-      <c r="C7" s="60"/>
-      <c r="D7" s="60"/>
-      <c r="E7" s="60"/>
-      <c r="F7" s="61"/>
-      <c r="H7" s="59"/>
-      <c r="I7" s="60"/>
-      <c r="J7" s="60"/>
-      <c r="K7" s="60"/>
-      <c r="L7" s="61"/>
-      <c r="N7" s="59"/>
-      <c r="O7" s="60"/>
-      <c r="P7" s="60"/>
-      <c r="Q7" s="60"/>
-      <c r="R7" s="61"/>
+      <c r="B7" s="54"/>
+      <c r="C7" s="55"/>
+      <c r="D7" s="55"/>
+      <c r="E7" s="55"/>
+      <c r="F7" s="56"/>
+      <c r="H7" s="54"/>
+      <c r="I7" s="55"/>
+      <c r="J7" s="55"/>
+      <c r="K7" s="55"/>
+      <c r="L7" s="56"/>
+      <c r="N7" s="54"/>
+      <c r="O7" s="55"/>
+      <c r="P7" s="55"/>
+      <c r="Q7" s="55"/>
+      <c r="R7" s="56"/>
     </row>
     <row r="8" spans="1:18">
-      <c r="B8" s="59"/>
-      <c r="C8" s="60"/>
-      <c r="D8" s="60"/>
-      <c r="E8" s="60"/>
-      <c r="F8" s="61"/>
-      <c r="H8" s="59"/>
-      <c r="I8" s="60"/>
-      <c r="J8" s="60"/>
-      <c r="K8" s="60"/>
-      <c r="L8" s="61"/>
-      <c r="N8" s="59"/>
-      <c r="O8" s="60"/>
-      <c r="P8" s="60"/>
-      <c r="Q8" s="60"/>
-      <c r="R8" s="61"/>
+      <c r="B8" s="54"/>
+      <c r="C8" s="55"/>
+      <c r="D8" s="55"/>
+      <c r="E8" s="55"/>
+      <c r="F8" s="56"/>
+      <c r="H8" s="54"/>
+      <c r="I8" s="55"/>
+      <c r="J8" s="55"/>
+      <c r="K8" s="55"/>
+      <c r="L8" s="56"/>
+      <c r="N8" s="54"/>
+      <c r="O8" s="55"/>
+      <c r="P8" s="55"/>
+      <c r="Q8" s="55"/>
+      <c r="R8" s="56"/>
     </row>
     <row r="9" spans="1:18">
-      <c r="B9" s="62"/>
-      <c r="C9" s="63"/>
-      <c r="D9" s="63"/>
-      <c r="E9" s="63"/>
-      <c r="F9" s="64"/>
-      <c r="H9" s="62"/>
-      <c r="I9" s="63"/>
-      <c r="J9" s="63"/>
-      <c r="K9" s="63"/>
-      <c r="L9" s="64"/>
-      <c r="N9" s="62"/>
-      <c r="O9" s="63"/>
-      <c r="P9" s="63"/>
-      <c r="Q9" s="63"/>
-      <c r="R9" s="64"/>
+      <c r="B9" s="57"/>
+      <c r="C9" s="58"/>
+      <c r="D9" s="58"/>
+      <c r="E9" s="58"/>
+      <c r="F9" s="59"/>
+      <c r="H9" s="57"/>
+      <c r="I9" s="58"/>
+      <c r="J9" s="58"/>
+      <c r="K9" s="58"/>
+      <c r="L9" s="59"/>
+      <c r="N9" s="57"/>
+      <c r="O9" s="58"/>
+      <c r="P9" s="58"/>
+      <c r="Q9" s="58"/>
+      <c r="R9" s="59"/>
     </row>
     <row r="10" spans="1:18">
       <c r="B10" s="5"/>
@@ -4047,226 +4036,226 @@
     </row>
     <row r="11" spans="1:18" ht="14.7" thickBot="1"/>
     <row r="12" spans="1:18" ht="16" customHeight="1">
-      <c r="B12" s="38" t="s">
+      <c r="B12" s="60" t="s">
         <v>102</v>
       </c>
-      <c r="C12" s="39"/>
-      <c r="D12" s="39"/>
-      <c r="E12" s="39"/>
-      <c r="F12" s="40"/>
-      <c r="H12" s="65" t="s">
+      <c r="C12" s="61"/>
+      <c r="D12" s="61"/>
+      <c r="E12" s="61"/>
+      <c r="F12" s="62"/>
+      <c r="H12" s="84" t="s">
         <v>102</v>
       </c>
-      <c r="I12" s="66"/>
-      <c r="J12" s="66"/>
-      <c r="K12" s="66"/>
-      <c r="L12" s="67"/>
-      <c r="N12" s="71" t="s">
+      <c r="I12" s="85"/>
+      <c r="J12" s="85"/>
+      <c r="K12" s="85"/>
+      <c r="L12" s="86"/>
+      <c r="N12" s="90" t="s">
         <v>102</v>
       </c>
-      <c r="O12" s="72"/>
-      <c r="P12" s="72"/>
-      <c r="Q12" s="72"/>
-      <c r="R12" s="73"/>
+      <c r="O12" s="91"/>
+      <c r="P12" s="91"/>
+      <c r="Q12" s="91"/>
+      <c r="R12" s="92"/>
     </row>
     <row r="13" spans="1:18" ht="16" customHeight="1">
-      <c r="B13" s="41"/>
-      <c r="C13" s="42"/>
-      <c r="D13" s="42"/>
-      <c r="E13" s="42"/>
-      <c r="F13" s="43"/>
-      <c r="H13" s="68"/>
-      <c r="I13" s="69"/>
-      <c r="J13" s="69"/>
-      <c r="K13" s="69"/>
-      <c r="L13" s="70"/>
-      <c r="N13" s="74"/>
-      <c r="O13" s="75"/>
-      <c r="P13" s="75"/>
-      <c r="Q13" s="75"/>
-      <c r="R13" s="76"/>
+      <c r="B13" s="63"/>
+      <c r="C13" s="64"/>
+      <c r="D13" s="64"/>
+      <c r="E13" s="64"/>
+      <c r="F13" s="65"/>
+      <c r="H13" s="87"/>
+      <c r="I13" s="88"/>
+      <c r="J13" s="88"/>
+      <c r="K13" s="88"/>
+      <c r="L13" s="89"/>
+      <c r="N13" s="93"/>
+      <c r="O13" s="94"/>
+      <c r="P13" s="94"/>
+      <c r="Q13" s="94"/>
+      <c r="R13" s="95"/>
     </row>
     <row r="14" spans="1:18" ht="16" customHeight="1">
-      <c r="B14" s="77" t="s">
+      <c r="B14" s="41" t="s">
         <v>103</v>
       </c>
-      <c r="C14" s="78"/>
-      <c r="D14" s="78"/>
-      <c r="E14" s="78"/>
-      <c r="F14" s="79"/>
-      <c r="H14" s="77" t="s">
+      <c r="C14" s="42"/>
+      <c r="D14" s="42"/>
+      <c r="E14" s="42"/>
+      <c r="F14" s="43"/>
+      <c r="H14" s="41" t="s">
         <v>104</v>
       </c>
-      <c r="I14" s="78"/>
-      <c r="J14" s="78"/>
-      <c r="K14" s="78"/>
-      <c r="L14" s="79"/>
-      <c r="N14" s="77" t="s">
+      <c r="I14" s="42"/>
+      <c r="J14" s="42"/>
+      <c r="K14" s="42"/>
+      <c r="L14" s="43"/>
+      <c r="N14" s="41" t="s">
         <v>105</v>
       </c>
-      <c r="O14" s="78"/>
-      <c r="P14" s="78"/>
-      <c r="Q14" s="78"/>
-      <c r="R14" s="79"/>
+      <c r="O14" s="42"/>
+      <c r="P14" s="42"/>
+      <c r="Q14" s="42"/>
+      <c r="R14" s="43"/>
     </row>
     <row r="15" spans="1:18">
-      <c r="B15" s="80"/>
-      <c r="C15" s="81"/>
-      <c r="D15" s="81"/>
-      <c r="E15" s="81"/>
-      <c r="F15" s="82"/>
-      <c r="H15" s="80"/>
-      <c r="I15" s="81"/>
-      <c r="J15" s="81"/>
-      <c r="K15" s="81"/>
-      <c r="L15" s="82"/>
-      <c r="N15" s="80"/>
-      <c r="O15" s="81"/>
-      <c r="P15" s="81"/>
-      <c r="Q15" s="81"/>
-      <c r="R15" s="82"/>
+      <c r="B15" s="44"/>
+      <c r="C15" s="45"/>
+      <c r="D15" s="45"/>
+      <c r="E15" s="45"/>
+      <c r="F15" s="46"/>
+      <c r="H15" s="44"/>
+      <c r="I15" s="45"/>
+      <c r="J15" s="45"/>
+      <c r="K15" s="45"/>
+      <c r="L15" s="46"/>
+      <c r="N15" s="44"/>
+      <c r="O15" s="45"/>
+      <c r="P15" s="45"/>
+      <c r="Q15" s="45"/>
+      <c r="R15" s="46"/>
     </row>
     <row r="16" spans="1:18">
-      <c r="B16" s="80"/>
-      <c r="C16" s="81"/>
-      <c r="D16" s="81"/>
-      <c r="E16" s="81"/>
-      <c r="F16" s="82"/>
-      <c r="H16" s="80"/>
-      <c r="I16" s="81"/>
-      <c r="J16" s="81"/>
-      <c r="K16" s="81"/>
-      <c r="L16" s="82"/>
-      <c r="N16" s="80"/>
-      <c r="O16" s="81"/>
-      <c r="P16" s="81"/>
-      <c r="Q16" s="81"/>
-      <c r="R16" s="82"/>
+      <c r="B16" s="44"/>
+      <c r="C16" s="45"/>
+      <c r="D16" s="45"/>
+      <c r="E16" s="45"/>
+      <c r="F16" s="46"/>
+      <c r="H16" s="44"/>
+      <c r="I16" s="45"/>
+      <c r="J16" s="45"/>
+      <c r="K16" s="45"/>
+      <c r="L16" s="46"/>
+      <c r="N16" s="44"/>
+      <c r="O16" s="45"/>
+      <c r="P16" s="45"/>
+      <c r="Q16" s="45"/>
+      <c r="R16" s="46"/>
     </row>
     <row r="17" spans="2:18">
-      <c r="B17" s="80"/>
-      <c r="C17" s="81"/>
-      <c r="D17" s="81"/>
-      <c r="E17" s="81"/>
-      <c r="F17" s="82"/>
-      <c r="H17" s="80"/>
-      <c r="I17" s="81"/>
-      <c r="J17" s="81"/>
-      <c r="K17" s="81"/>
-      <c r="L17" s="82"/>
-      <c r="N17" s="80"/>
-      <c r="O17" s="81"/>
-      <c r="P17" s="81"/>
-      <c r="Q17" s="81"/>
-      <c r="R17" s="82"/>
+      <c r="B17" s="44"/>
+      <c r="C17" s="45"/>
+      <c r="D17" s="45"/>
+      <c r="E17" s="45"/>
+      <c r="F17" s="46"/>
+      <c r="H17" s="44"/>
+      <c r="I17" s="45"/>
+      <c r="J17" s="45"/>
+      <c r="K17" s="45"/>
+      <c r="L17" s="46"/>
+      <c r="N17" s="44"/>
+      <c r="O17" s="45"/>
+      <c r="P17" s="45"/>
+      <c r="Q17" s="45"/>
+      <c r="R17" s="46"/>
     </row>
     <row r="18" spans="2:18">
-      <c r="B18" s="83"/>
-      <c r="C18" s="84"/>
-      <c r="D18" s="84"/>
-      <c r="E18" s="84"/>
-      <c r="F18" s="85"/>
-      <c r="H18" s="83"/>
-      <c r="I18" s="84"/>
-      <c r="J18" s="84"/>
-      <c r="K18" s="84"/>
-      <c r="L18" s="85"/>
-      <c r="N18" s="83"/>
-      <c r="O18" s="84"/>
-      <c r="P18" s="84"/>
-      <c r="Q18" s="84"/>
-      <c r="R18" s="85"/>
+      <c r="B18" s="47"/>
+      <c r="C18" s="48"/>
+      <c r="D18" s="48"/>
+      <c r="E18" s="48"/>
+      <c r="F18" s="49"/>
+      <c r="H18" s="47"/>
+      <c r="I18" s="48"/>
+      <c r="J18" s="48"/>
+      <c r="K18" s="48"/>
+      <c r="L18" s="49"/>
+      <c r="N18" s="47"/>
+      <c r="O18" s="48"/>
+      <c r="P18" s="48"/>
+      <c r="Q18" s="48"/>
+      <c r="R18" s="49"/>
     </row>
     <row r="19" spans="2:18" ht="16" customHeight="1">
-      <c r="B19" s="77" t="s">
+      <c r="B19" s="41" t="s">
         <v>106</v>
       </c>
-      <c r="C19" s="78"/>
-      <c r="D19" s="78"/>
-      <c r="E19" s="78"/>
-      <c r="F19" s="79"/>
-      <c r="H19" s="77" t="s">
+      <c r="C19" s="42"/>
+      <c r="D19" s="42"/>
+      <c r="E19" s="42"/>
+      <c r="F19" s="43"/>
+      <c r="H19" s="41" t="s">
         <v>106</v>
       </c>
-      <c r="I19" s="78"/>
-      <c r="J19" s="78"/>
-      <c r="K19" s="78"/>
-      <c r="L19" s="79"/>
-      <c r="N19" s="77" t="s">
+      <c r="I19" s="42"/>
+      <c r="J19" s="42"/>
+      <c r="K19" s="42"/>
+      <c r="L19" s="43"/>
+      <c r="N19" s="41" t="s">
         <v>107</v>
       </c>
-      <c r="O19" s="78"/>
-      <c r="P19" s="78"/>
-      <c r="Q19" s="78"/>
-      <c r="R19" s="79"/>
+      <c r="O19" s="42"/>
+      <c r="P19" s="42"/>
+      <c r="Q19" s="42"/>
+      <c r="R19" s="43"/>
     </row>
     <row r="20" spans="2:18">
-      <c r="B20" s="80"/>
-      <c r="C20" s="81"/>
-      <c r="D20" s="81"/>
-      <c r="E20" s="81"/>
-      <c r="F20" s="82"/>
-      <c r="H20" s="80"/>
-      <c r="I20" s="81"/>
-      <c r="J20" s="81"/>
-      <c r="K20" s="81"/>
-      <c r="L20" s="82"/>
-      <c r="N20" s="80"/>
-      <c r="O20" s="81"/>
-      <c r="P20" s="81"/>
-      <c r="Q20" s="81"/>
-      <c r="R20" s="82"/>
+      <c r="B20" s="44"/>
+      <c r="C20" s="45"/>
+      <c r="D20" s="45"/>
+      <c r="E20" s="45"/>
+      <c r="F20" s="46"/>
+      <c r="H20" s="44"/>
+      <c r="I20" s="45"/>
+      <c r="J20" s="45"/>
+      <c r="K20" s="45"/>
+      <c r="L20" s="46"/>
+      <c r="N20" s="44"/>
+      <c r="O20" s="45"/>
+      <c r="P20" s="45"/>
+      <c r="Q20" s="45"/>
+      <c r="R20" s="46"/>
     </row>
     <row r="21" spans="2:18">
-      <c r="B21" s="80"/>
-      <c r="C21" s="81"/>
-      <c r="D21" s="81"/>
-      <c r="E21" s="81"/>
-      <c r="F21" s="82"/>
-      <c r="H21" s="80"/>
-      <c r="I21" s="81"/>
-      <c r="J21" s="81"/>
-      <c r="K21" s="81"/>
-      <c r="L21" s="82"/>
-      <c r="N21" s="80"/>
-      <c r="O21" s="81"/>
-      <c r="P21" s="81"/>
-      <c r="Q21" s="81"/>
-      <c r="R21" s="82"/>
+      <c r="B21" s="44"/>
+      <c r="C21" s="45"/>
+      <c r="D21" s="45"/>
+      <c r="E21" s="45"/>
+      <c r="F21" s="46"/>
+      <c r="H21" s="44"/>
+      <c r="I21" s="45"/>
+      <c r="J21" s="45"/>
+      <c r="K21" s="45"/>
+      <c r="L21" s="46"/>
+      <c r="N21" s="44"/>
+      <c r="O21" s="45"/>
+      <c r="P21" s="45"/>
+      <c r="Q21" s="45"/>
+      <c r="R21" s="46"/>
     </row>
     <row r="22" spans="2:18">
-      <c r="B22" s="80"/>
-      <c r="C22" s="81"/>
-      <c r="D22" s="81"/>
-      <c r="E22" s="81"/>
-      <c r="F22" s="82"/>
-      <c r="H22" s="80"/>
-      <c r="I22" s="81"/>
-      <c r="J22" s="81"/>
-      <c r="K22" s="81"/>
-      <c r="L22" s="82"/>
-      <c r="N22" s="80"/>
-      <c r="O22" s="81"/>
-      <c r="P22" s="81"/>
-      <c r="Q22" s="81"/>
-      <c r="R22" s="82"/>
+      <c r="B22" s="44"/>
+      <c r="C22" s="45"/>
+      <c r="D22" s="45"/>
+      <c r="E22" s="45"/>
+      <c r="F22" s="46"/>
+      <c r="H22" s="44"/>
+      <c r="I22" s="45"/>
+      <c r="J22" s="45"/>
+      <c r="K22" s="45"/>
+      <c r="L22" s="46"/>
+      <c r="N22" s="44"/>
+      <c r="O22" s="45"/>
+      <c r="P22" s="45"/>
+      <c r="Q22" s="45"/>
+      <c r="R22" s="46"/>
     </row>
     <row r="23" spans="2:18">
-      <c r="B23" s="83"/>
-      <c r="C23" s="84"/>
-      <c r="D23" s="84"/>
-      <c r="E23" s="84"/>
-      <c r="F23" s="85"/>
-      <c r="H23" s="83"/>
-      <c r="I23" s="84"/>
-      <c r="J23" s="84"/>
-      <c r="K23" s="84"/>
-      <c r="L23" s="85"/>
-      <c r="N23" s="83"/>
-      <c r="O23" s="84"/>
-      <c r="P23" s="84"/>
-      <c r="Q23" s="84"/>
-      <c r="R23" s="85"/>
+      <c r="B23" s="47"/>
+      <c r="C23" s="48"/>
+      <c r="D23" s="48"/>
+      <c r="E23" s="48"/>
+      <c r="F23" s="49"/>
+      <c r="H23" s="47"/>
+      <c r="I23" s="48"/>
+      <c r="J23" s="48"/>
+      <c r="K23" s="48"/>
+      <c r="L23" s="49"/>
+      <c r="N23" s="47"/>
+      <c r="O23" s="48"/>
+      <c r="P23" s="48"/>
+      <c r="Q23" s="48"/>
+      <c r="R23" s="49"/>
     </row>
     <row r="26" spans="2:18" ht="18.3">
       <c r="B26" s="6" t="s">
@@ -4432,341 +4421,341 @@
     </row>
     <row r="37" spans="2:18" ht="14.7" thickBot="1"/>
     <row r="38" spans="2:18">
-      <c r="B38" s="38" t="s">
+      <c r="B38" s="60" t="s">
         <v>117</v>
       </c>
-      <c r="C38" s="39"/>
-      <c r="D38" s="39"/>
-      <c r="E38" s="39"/>
-      <c r="F38" s="40"/>
-      <c r="H38" s="86" t="s">
+      <c r="C38" s="61"/>
+      <c r="D38" s="61"/>
+      <c r="E38" s="61"/>
+      <c r="F38" s="62"/>
+      <c r="H38" s="78" t="s">
         <v>118</v>
       </c>
-      <c r="I38" s="87"/>
-      <c r="J38" s="87"/>
-      <c r="K38" s="87"/>
-      <c r="L38" s="88"/>
-      <c r="N38" s="50" t="s">
+      <c r="I38" s="79"/>
+      <c r="J38" s="79"/>
+      <c r="K38" s="79"/>
+      <c r="L38" s="80"/>
+      <c r="N38" s="72" t="s">
         <v>119</v>
       </c>
-      <c r="O38" s="51"/>
-      <c r="P38" s="51"/>
-      <c r="Q38" s="51"/>
-      <c r="R38" s="52"/>
+      <c r="O38" s="73"/>
+      <c r="P38" s="73"/>
+      <c r="Q38" s="73"/>
+      <c r="R38" s="74"/>
     </row>
     <row r="39" spans="2:18" ht="14.7" thickBot="1">
-      <c r="B39" s="41"/>
-      <c r="C39" s="42"/>
-      <c r="D39" s="42"/>
-      <c r="E39" s="42"/>
-      <c r="F39" s="43"/>
-      <c r="H39" s="89"/>
-      <c r="I39" s="90"/>
-      <c r="J39" s="90"/>
-      <c r="K39" s="90"/>
-      <c r="L39" s="91"/>
-      <c r="N39" s="53"/>
-      <c r="O39" s="54"/>
-      <c r="P39" s="54"/>
-      <c r="Q39" s="54"/>
-      <c r="R39" s="55"/>
+      <c r="B39" s="63"/>
+      <c r="C39" s="64"/>
+      <c r="D39" s="64"/>
+      <c r="E39" s="64"/>
+      <c r="F39" s="65"/>
+      <c r="H39" s="81"/>
+      <c r="I39" s="82"/>
+      <c r="J39" s="82"/>
+      <c r="K39" s="82"/>
+      <c r="L39" s="83"/>
+      <c r="N39" s="75"/>
+      <c r="O39" s="76"/>
+      <c r="P39" s="76"/>
+      <c r="Q39" s="76"/>
+      <c r="R39" s="77"/>
     </row>
     <row r="40" spans="2:18">
-      <c r="B40" s="56" t="s">
+      <c r="B40" s="51" t="s">
         <v>120</v>
       </c>
-      <c r="C40" s="57"/>
-      <c r="D40" s="57"/>
-      <c r="E40" s="57"/>
-      <c r="F40" s="58"/>
-      <c r="H40" s="56" t="s">
+      <c r="C40" s="52"/>
+      <c r="D40" s="52"/>
+      <c r="E40" s="52"/>
+      <c r="F40" s="53"/>
+      <c r="H40" s="51" t="s">
         <v>121</v>
       </c>
-      <c r="I40" s="57"/>
-      <c r="J40" s="57"/>
-      <c r="K40" s="57"/>
-      <c r="L40" s="58"/>
-      <c r="N40" s="56" t="s">
+      <c r="I40" s="52"/>
+      <c r="J40" s="52"/>
+      <c r="K40" s="52"/>
+      <c r="L40" s="53"/>
+      <c r="N40" s="51" t="s">
         <v>122</v>
       </c>
-      <c r="O40" s="57"/>
-      <c r="P40" s="57"/>
-      <c r="Q40" s="57"/>
-      <c r="R40" s="58"/>
+      <c r="O40" s="52"/>
+      <c r="P40" s="52"/>
+      <c r="Q40" s="52"/>
+      <c r="R40" s="53"/>
     </row>
     <row r="41" spans="2:18">
-      <c r="B41" s="59"/>
-      <c r="C41" s="60"/>
-      <c r="D41" s="60"/>
-      <c r="E41" s="60"/>
-      <c r="F41" s="61"/>
-      <c r="H41" s="59"/>
-      <c r="I41" s="60"/>
-      <c r="J41" s="60"/>
-      <c r="K41" s="60"/>
-      <c r="L41" s="61"/>
-      <c r="N41" s="59"/>
-      <c r="O41" s="60"/>
-      <c r="P41" s="60"/>
-      <c r="Q41" s="60"/>
-      <c r="R41" s="61"/>
+      <c r="B41" s="54"/>
+      <c r="C41" s="55"/>
+      <c r="D41" s="55"/>
+      <c r="E41" s="55"/>
+      <c r="F41" s="56"/>
+      <c r="H41" s="54"/>
+      <c r="I41" s="55"/>
+      <c r="J41" s="55"/>
+      <c r="K41" s="55"/>
+      <c r="L41" s="56"/>
+      <c r="N41" s="54"/>
+      <c r="O41" s="55"/>
+      <c r="P41" s="55"/>
+      <c r="Q41" s="55"/>
+      <c r="R41" s="56"/>
     </row>
     <row r="42" spans="2:18">
-      <c r="B42" s="59"/>
-      <c r="C42" s="60"/>
-      <c r="D42" s="60"/>
-      <c r="E42" s="60"/>
-      <c r="F42" s="61"/>
-      <c r="H42" s="59"/>
-      <c r="I42" s="60"/>
-      <c r="J42" s="60"/>
-      <c r="K42" s="60"/>
-      <c r="L42" s="61"/>
-      <c r="N42" s="59"/>
-      <c r="O42" s="60"/>
-      <c r="P42" s="60"/>
-      <c r="Q42" s="60"/>
-      <c r="R42" s="61"/>
+      <c r="B42" s="54"/>
+      <c r="C42" s="55"/>
+      <c r="D42" s="55"/>
+      <c r="E42" s="55"/>
+      <c r="F42" s="56"/>
+      <c r="H42" s="54"/>
+      <c r="I42" s="55"/>
+      <c r="J42" s="55"/>
+      <c r="K42" s="55"/>
+      <c r="L42" s="56"/>
+      <c r="N42" s="54"/>
+      <c r="O42" s="55"/>
+      <c r="P42" s="55"/>
+      <c r="Q42" s="55"/>
+      <c r="R42" s="56"/>
     </row>
     <row r="43" spans="2:18">
-      <c r="B43" s="62"/>
-      <c r="C43" s="63"/>
-      <c r="D43" s="63"/>
-      <c r="E43" s="63"/>
-      <c r="F43" s="64"/>
-      <c r="H43" s="62"/>
-      <c r="I43" s="63"/>
-      <c r="J43" s="63"/>
-      <c r="K43" s="63"/>
-      <c r="L43" s="64"/>
-      <c r="N43" s="62"/>
-      <c r="O43" s="63"/>
-      <c r="P43" s="63"/>
-      <c r="Q43" s="63"/>
-      <c r="R43" s="64"/>
+      <c r="B43" s="57"/>
+      <c r="C43" s="58"/>
+      <c r="D43" s="58"/>
+      <c r="E43" s="58"/>
+      <c r="F43" s="59"/>
+      <c r="H43" s="57"/>
+      <c r="I43" s="58"/>
+      <c r="J43" s="58"/>
+      <c r="K43" s="58"/>
+      <c r="L43" s="59"/>
+      <c r="N43" s="57"/>
+      <c r="O43" s="58"/>
+      <c r="P43" s="58"/>
+      <c r="Q43" s="58"/>
+      <c r="R43" s="59"/>
     </row>
     <row r="45" spans="2:18" ht="14.7" thickBot="1"/>
     <row r="46" spans="2:18" ht="16" customHeight="1">
-      <c r="B46" s="38" t="s">
+      <c r="B46" s="60" t="s">
         <v>102</v>
       </c>
-      <c r="C46" s="39"/>
-      <c r="D46" s="39"/>
-      <c r="E46" s="39"/>
-      <c r="F46" s="40"/>
-      <c r="H46" s="92" t="s">
+      <c r="C46" s="61"/>
+      <c r="D46" s="61"/>
+      <c r="E46" s="61"/>
+      <c r="F46" s="62"/>
+      <c r="H46" s="66" t="s">
         <v>102</v>
       </c>
-      <c r="I46" s="93"/>
-      <c r="J46" s="93"/>
-      <c r="K46" s="93"/>
-      <c r="L46" s="94"/>
-      <c r="N46" s="50" t="s">
+      <c r="I46" s="67"/>
+      <c r="J46" s="67"/>
+      <c r="K46" s="67"/>
+      <c r="L46" s="68"/>
+      <c r="N46" s="72" t="s">
         <v>102</v>
       </c>
-      <c r="O46" s="51"/>
-      <c r="P46" s="51"/>
-      <c r="Q46" s="51"/>
-      <c r="R46" s="52"/>
+      <c r="O46" s="73"/>
+      <c r="P46" s="73"/>
+      <c r="Q46" s="73"/>
+      <c r="R46" s="74"/>
     </row>
     <row r="47" spans="2:18" ht="16" customHeight="1" thickBot="1">
-      <c r="B47" s="41"/>
-      <c r="C47" s="42"/>
-      <c r="D47" s="42"/>
-      <c r="E47" s="42"/>
-      <c r="F47" s="43"/>
-      <c r="H47" s="95"/>
-      <c r="I47" s="96"/>
-      <c r="J47" s="96"/>
-      <c r="K47" s="96"/>
-      <c r="L47" s="97"/>
-      <c r="N47" s="53"/>
-      <c r="O47" s="54"/>
-      <c r="P47" s="54"/>
-      <c r="Q47" s="54"/>
-      <c r="R47" s="55"/>
+      <c r="B47" s="63"/>
+      <c r="C47" s="64"/>
+      <c r="D47" s="64"/>
+      <c r="E47" s="64"/>
+      <c r="F47" s="65"/>
+      <c r="H47" s="69"/>
+      <c r="I47" s="70"/>
+      <c r="J47" s="70"/>
+      <c r="K47" s="70"/>
+      <c r="L47" s="71"/>
+      <c r="N47" s="75"/>
+      <c r="O47" s="76"/>
+      <c r="P47" s="76"/>
+      <c r="Q47" s="76"/>
+      <c r="R47" s="77"/>
     </row>
     <row r="48" spans="2:18">
-      <c r="B48" s="77" t="s">
+      <c r="B48" s="41" t="s">
         <v>123</v>
       </c>
-      <c r="C48" s="78"/>
-      <c r="D48" s="78"/>
-      <c r="E48" s="78"/>
-      <c r="F48" s="79"/>
-      <c r="H48" s="101" t="s">
+      <c r="C48" s="42"/>
+      <c r="D48" s="42"/>
+      <c r="E48" s="42"/>
+      <c r="F48" s="43"/>
+      <c r="H48" s="50" t="s">
         <v>124</v>
       </c>
-      <c r="I48" s="78"/>
-      <c r="J48" s="78"/>
-      <c r="K48" s="78"/>
-      <c r="L48" s="79"/>
-      <c r="N48" s="77" t="s">
+      <c r="I48" s="42"/>
+      <c r="J48" s="42"/>
+      <c r="K48" s="42"/>
+      <c r="L48" s="43"/>
+      <c r="N48" s="41" t="s">
         <v>125</v>
       </c>
-      <c r="O48" s="78"/>
-      <c r="P48" s="78"/>
-      <c r="Q48" s="78"/>
-      <c r="R48" s="79"/>
+      <c r="O48" s="42"/>
+      <c r="P48" s="42"/>
+      <c r="Q48" s="42"/>
+      <c r="R48" s="43"/>
     </row>
     <row r="49" spans="2:18">
-      <c r="B49" s="80"/>
-      <c r="C49" s="81"/>
-      <c r="D49" s="81"/>
-      <c r="E49" s="81"/>
-      <c r="F49" s="82"/>
-      <c r="H49" s="80"/>
-      <c r="I49" s="81"/>
-      <c r="J49" s="81"/>
-      <c r="K49" s="81"/>
-      <c r="L49" s="82"/>
-      <c r="N49" s="80"/>
-      <c r="O49" s="81"/>
-      <c r="P49" s="81"/>
-      <c r="Q49" s="81"/>
-      <c r="R49" s="82"/>
+      <c r="B49" s="44"/>
+      <c r="C49" s="45"/>
+      <c r="D49" s="45"/>
+      <c r="E49" s="45"/>
+      <c r="F49" s="46"/>
+      <c r="H49" s="44"/>
+      <c r="I49" s="45"/>
+      <c r="J49" s="45"/>
+      <c r="K49" s="45"/>
+      <c r="L49" s="46"/>
+      <c r="N49" s="44"/>
+      <c r="O49" s="45"/>
+      <c r="P49" s="45"/>
+      <c r="Q49" s="45"/>
+      <c r="R49" s="46"/>
     </row>
     <row r="50" spans="2:18">
-      <c r="B50" s="80"/>
-      <c r="C50" s="81"/>
-      <c r="D50" s="81"/>
-      <c r="E50" s="81"/>
-      <c r="F50" s="82"/>
-      <c r="H50" s="80"/>
-      <c r="I50" s="81"/>
-      <c r="J50" s="81"/>
-      <c r="K50" s="81"/>
-      <c r="L50" s="82"/>
-      <c r="N50" s="80"/>
-      <c r="O50" s="81"/>
-      <c r="P50" s="81"/>
-      <c r="Q50" s="81"/>
-      <c r="R50" s="82"/>
+      <c r="B50" s="44"/>
+      <c r="C50" s="45"/>
+      <c r="D50" s="45"/>
+      <c r="E50" s="45"/>
+      <c r="F50" s="46"/>
+      <c r="H50" s="44"/>
+      <c r="I50" s="45"/>
+      <c r="J50" s="45"/>
+      <c r="K50" s="45"/>
+      <c r="L50" s="46"/>
+      <c r="N50" s="44"/>
+      <c r="O50" s="45"/>
+      <c r="P50" s="45"/>
+      <c r="Q50" s="45"/>
+      <c r="R50" s="46"/>
     </row>
     <row r="51" spans="2:18">
-      <c r="B51" s="80"/>
-      <c r="C51" s="81"/>
-      <c r="D51" s="81"/>
-      <c r="E51" s="81"/>
-      <c r="F51" s="82"/>
-      <c r="H51" s="80"/>
-      <c r="I51" s="81"/>
-      <c r="J51" s="81"/>
-      <c r="K51" s="81"/>
-      <c r="L51" s="82"/>
-      <c r="N51" s="80"/>
-      <c r="O51" s="81"/>
-      <c r="P51" s="81"/>
-      <c r="Q51" s="81"/>
-      <c r="R51" s="82"/>
+      <c r="B51" s="44"/>
+      <c r="C51" s="45"/>
+      <c r="D51" s="45"/>
+      <c r="E51" s="45"/>
+      <c r="F51" s="46"/>
+      <c r="H51" s="44"/>
+      <c r="I51" s="45"/>
+      <c r="J51" s="45"/>
+      <c r="K51" s="45"/>
+      <c r="L51" s="46"/>
+      <c r="N51" s="44"/>
+      <c r="O51" s="45"/>
+      <c r="P51" s="45"/>
+      <c r="Q51" s="45"/>
+      <c r="R51" s="46"/>
     </row>
     <row r="52" spans="2:18">
-      <c r="B52" s="83"/>
-      <c r="C52" s="84"/>
-      <c r="D52" s="84"/>
-      <c r="E52" s="84"/>
-      <c r="F52" s="85"/>
-      <c r="H52" s="83"/>
-      <c r="I52" s="84"/>
-      <c r="J52" s="84"/>
-      <c r="K52" s="84"/>
-      <c r="L52" s="85"/>
-      <c r="N52" s="83"/>
-      <c r="O52" s="84"/>
-      <c r="P52" s="84"/>
-      <c r="Q52" s="84"/>
-      <c r="R52" s="85"/>
+      <c r="B52" s="47"/>
+      <c r="C52" s="48"/>
+      <c r="D52" s="48"/>
+      <c r="E52" s="48"/>
+      <c r="F52" s="49"/>
+      <c r="H52" s="47"/>
+      <c r="I52" s="48"/>
+      <c r="J52" s="48"/>
+      <c r="K52" s="48"/>
+      <c r="L52" s="49"/>
+      <c r="N52" s="47"/>
+      <c r="O52" s="48"/>
+      <c r="P52" s="48"/>
+      <c r="Q52" s="48"/>
+      <c r="R52" s="49"/>
     </row>
     <row r="53" spans="2:18">
-      <c r="B53" s="77" t="s">
+      <c r="B53" s="41" t="s">
         <v>126</v>
       </c>
-      <c r="C53" s="78"/>
-      <c r="D53" s="78"/>
-      <c r="E53" s="78"/>
-      <c r="F53" s="79"/>
-      <c r="H53" s="77" t="s">
+      <c r="C53" s="42"/>
+      <c r="D53" s="42"/>
+      <c r="E53" s="42"/>
+      <c r="F53" s="43"/>
+      <c r="H53" s="41" t="s">
         <v>127</v>
       </c>
-      <c r="I53" s="78"/>
-      <c r="J53" s="78"/>
-      <c r="K53" s="78"/>
-      <c r="L53" s="79"/>
-      <c r="N53" s="77" t="s">
+      <c r="I53" s="42"/>
+      <c r="J53" s="42"/>
+      <c r="K53" s="42"/>
+      <c r="L53" s="43"/>
+      <c r="N53" s="41" t="s">
         <v>128</v>
       </c>
-      <c r="O53" s="78"/>
-      <c r="P53" s="78"/>
-      <c r="Q53" s="78"/>
-      <c r="R53" s="79"/>
+      <c r="O53" s="42"/>
+      <c r="P53" s="42"/>
+      <c r="Q53" s="42"/>
+      <c r="R53" s="43"/>
     </row>
     <row r="54" spans="2:18">
-      <c r="B54" s="80"/>
-      <c r="C54" s="81"/>
-      <c r="D54" s="81"/>
-      <c r="E54" s="81"/>
-      <c r="F54" s="82"/>
-      <c r="H54" s="80"/>
-      <c r="I54" s="81"/>
-      <c r="J54" s="81"/>
-      <c r="K54" s="81"/>
-      <c r="L54" s="82"/>
-      <c r="N54" s="80"/>
-      <c r="O54" s="81"/>
-      <c r="P54" s="81"/>
-      <c r="Q54" s="81"/>
-      <c r="R54" s="82"/>
+      <c r="B54" s="44"/>
+      <c r="C54" s="45"/>
+      <c r="D54" s="45"/>
+      <c r="E54" s="45"/>
+      <c r="F54" s="46"/>
+      <c r="H54" s="44"/>
+      <c r="I54" s="45"/>
+      <c r="J54" s="45"/>
+      <c r="K54" s="45"/>
+      <c r="L54" s="46"/>
+      <c r="N54" s="44"/>
+      <c r="O54" s="45"/>
+      <c r="P54" s="45"/>
+      <c r="Q54" s="45"/>
+      <c r="R54" s="46"/>
     </row>
     <row r="55" spans="2:18">
-      <c r="B55" s="80"/>
-      <c r="C55" s="81"/>
-      <c r="D55" s="81"/>
-      <c r="E55" s="81"/>
-      <c r="F55" s="82"/>
-      <c r="H55" s="80"/>
-      <c r="I55" s="81"/>
-      <c r="J55" s="81"/>
-      <c r="K55" s="81"/>
-      <c r="L55" s="82"/>
-      <c r="N55" s="80"/>
-      <c r="O55" s="81"/>
-      <c r="P55" s="81"/>
-      <c r="Q55" s="81"/>
-      <c r="R55" s="82"/>
+      <c r="B55" s="44"/>
+      <c r="C55" s="45"/>
+      <c r="D55" s="45"/>
+      <c r="E55" s="45"/>
+      <c r="F55" s="46"/>
+      <c r="H55" s="44"/>
+      <c r="I55" s="45"/>
+      <c r="J55" s="45"/>
+      <c r="K55" s="45"/>
+      <c r="L55" s="46"/>
+      <c r="N55" s="44"/>
+      <c r="O55" s="45"/>
+      <c r="P55" s="45"/>
+      <c r="Q55" s="45"/>
+      <c r="R55" s="46"/>
     </row>
     <row r="56" spans="2:18">
-      <c r="B56" s="80"/>
-      <c r="C56" s="81"/>
-      <c r="D56" s="81"/>
-      <c r="E56" s="81"/>
-      <c r="F56" s="82"/>
-      <c r="H56" s="80"/>
-      <c r="I56" s="81"/>
-      <c r="J56" s="81"/>
-      <c r="K56" s="81"/>
-      <c r="L56" s="82"/>
-      <c r="N56" s="80"/>
-      <c r="O56" s="81"/>
-      <c r="P56" s="81"/>
-      <c r="Q56" s="81"/>
-      <c r="R56" s="82"/>
+      <c r="B56" s="44"/>
+      <c r="C56" s="45"/>
+      <c r="D56" s="45"/>
+      <c r="E56" s="45"/>
+      <c r="F56" s="46"/>
+      <c r="H56" s="44"/>
+      <c r="I56" s="45"/>
+      <c r="J56" s="45"/>
+      <c r="K56" s="45"/>
+      <c r="L56" s="46"/>
+      <c r="N56" s="44"/>
+      <c r="O56" s="45"/>
+      <c r="P56" s="45"/>
+      <c r="Q56" s="45"/>
+      <c r="R56" s="46"/>
     </row>
     <row r="57" spans="2:18">
-      <c r="B57" s="83"/>
-      <c r="C57" s="84"/>
-      <c r="D57" s="84"/>
-      <c r="E57" s="84"/>
-      <c r="F57" s="85"/>
-      <c r="H57" s="83"/>
-      <c r="I57" s="84"/>
-      <c r="J57" s="84"/>
-      <c r="K57" s="84"/>
-      <c r="L57" s="85"/>
-      <c r="N57" s="83"/>
-      <c r="O57" s="84"/>
-      <c r="P57" s="84"/>
-      <c r="Q57" s="84"/>
-      <c r="R57" s="85"/>
+      <c r="B57" s="47"/>
+      <c r="C57" s="48"/>
+      <c r="D57" s="48"/>
+      <c r="E57" s="48"/>
+      <c r="F57" s="49"/>
+      <c r="H57" s="47"/>
+      <c r="I57" s="48"/>
+      <c r="J57" s="48"/>
+      <c r="K57" s="48"/>
+      <c r="L57" s="49"/>
+      <c r="N57" s="47"/>
+      <c r="O57" s="48"/>
+      <c r="P57" s="48"/>
+      <c r="Q57" s="48"/>
+      <c r="R57" s="49"/>
     </row>
     <row r="60" spans="2:18" ht="18.3">
       <c r="B60" s="6" t="s">
@@ -4939,13 +4928,13 @@
       <c r="R67" s="27"/>
     </row>
     <row r="70" spans="2:18" ht="15.6">
-      <c r="N70" s="98" t="s">
+      <c r="N70" s="38" t="s">
         <v>143</v>
       </c>
-      <c r="O70" s="99"/>
-      <c r="P70" s="99"/>
-      <c r="Q70" s="99"/>
-      <c r="R70" s="100"/>
+      <c r="O70" s="39"/>
+      <c r="P70" s="39"/>
+      <c r="Q70" s="39"/>
+      <c r="R70" s="40"/>
     </row>
     <row r="71" spans="2:18" ht="32.1" customHeight="1">
       <c r="N71" s="28"/>
@@ -5020,6 +5009,30 @@
     </row>
   </sheetData>
   <mergeCells count="31">
+    <mergeCell ref="B4:F5"/>
+    <mergeCell ref="H4:L5"/>
+    <mergeCell ref="N4:R5"/>
+    <mergeCell ref="B6:F9"/>
+    <mergeCell ref="H6:L9"/>
+    <mergeCell ref="N6:R9"/>
+    <mergeCell ref="B12:F13"/>
+    <mergeCell ref="H12:L13"/>
+    <mergeCell ref="N12:R13"/>
+    <mergeCell ref="B14:F18"/>
+    <mergeCell ref="H14:L18"/>
+    <mergeCell ref="N14:R18"/>
+    <mergeCell ref="B19:F23"/>
+    <mergeCell ref="H19:L23"/>
+    <mergeCell ref="N19:R23"/>
+    <mergeCell ref="B38:F39"/>
+    <mergeCell ref="H38:L39"/>
+    <mergeCell ref="N38:R39"/>
+    <mergeCell ref="B40:F43"/>
+    <mergeCell ref="H40:L43"/>
+    <mergeCell ref="N40:R43"/>
+    <mergeCell ref="B46:F47"/>
+    <mergeCell ref="H46:L47"/>
+    <mergeCell ref="N46:R47"/>
     <mergeCell ref="N70:R70"/>
     <mergeCell ref="B48:F52"/>
     <mergeCell ref="H48:L52"/>
@@ -5027,30 +5040,6 @@
     <mergeCell ref="B53:F57"/>
     <mergeCell ref="H53:L57"/>
     <mergeCell ref="N53:R57"/>
-    <mergeCell ref="B40:F43"/>
-    <mergeCell ref="H40:L43"/>
-    <mergeCell ref="N40:R43"/>
-    <mergeCell ref="B46:F47"/>
-    <mergeCell ref="H46:L47"/>
-    <mergeCell ref="N46:R47"/>
-    <mergeCell ref="B19:F23"/>
-    <mergeCell ref="H19:L23"/>
-    <mergeCell ref="N19:R23"/>
-    <mergeCell ref="B38:F39"/>
-    <mergeCell ref="H38:L39"/>
-    <mergeCell ref="N38:R39"/>
-    <mergeCell ref="B12:F13"/>
-    <mergeCell ref="H12:L13"/>
-    <mergeCell ref="N12:R13"/>
-    <mergeCell ref="B14:F18"/>
-    <mergeCell ref="H14:L18"/>
-    <mergeCell ref="N14:R18"/>
-    <mergeCell ref="B4:F5"/>
-    <mergeCell ref="H4:L5"/>
-    <mergeCell ref="N4:R5"/>
-    <mergeCell ref="B6:F9"/>
-    <mergeCell ref="H6:L9"/>
-    <mergeCell ref="N6:R9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>

</xml_diff>

<commit_message>
one list for everyone
</commit_message>
<xml_diff>
--- a/input/multiassets.xlsx
+++ b/input/multiassets.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28502"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/935cc860ba0efd68/GitHub/myportfolio/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="159" documentId="13_ncr:1_{B10D7187-5546-4483-8DEF-63838578FBF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{58A08753-6DB4-4DEE-AE1A-D5B9D1BC1E94}"/>
+  <xr:revisionPtr revIDLastSave="171" documentId="13_ncr:1_{B10D7187-5546-4483-8DEF-63838578FBF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4330DA66-9903-445E-84CC-CE3DE94180C9}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
     <sheet name="bonds" sheetId="7" r:id="rId6"/>
     <sheet name="bond" sheetId="5" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -303,7 +303,49 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="508" uniqueCount="226">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="516" uniqueCount="231">
+  <si>
+    <t>Link</t>
+  </si>
+  <si>
+    <t>Index</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>ISIN</t>
+  </si>
+  <si>
+    <t>Ticker</t>
+  </si>
+  <si>
+    <t>Currency</t>
+  </si>
+  <si>
+    <t>Currency Hedging</t>
+  </si>
+  <si>
+    <t>Use of earnings</t>
+  </si>
+  <si>
+    <t>TER</t>
+  </si>
+  <si>
+    <t>Replication</t>
+  </si>
+  <si>
+    <t>Scenario macro coperto</t>
+  </si>
+  <si>
+    <t>Comments</t>
+  </si>
+  <si>
+    <t>iShares Core MSCI World UCITS ETF USD (Acc) | SWDA | IE00B4L5Y983</t>
+  </si>
+  <si>
+    <t>MSCI World</t>
+  </si>
   <si>
     <t>iShares Core MSCI World UCITS ETF USD</t>
   </si>
@@ -311,43 +353,268 @@
     <t>IE00B4L5Y983</t>
   </si>
   <si>
-    <t>ISIN</t>
-  </si>
-  <si>
-    <t>Currency Hedging</t>
-  </si>
-  <si>
-    <t>TER</t>
-  </si>
-  <si>
-    <t>Use of earnings</t>
-  </si>
-  <si>
-    <t>Name</t>
+    <t>IWDA.L</t>
+  </si>
+  <si>
+    <t>USD</t>
   </si>
   <si>
     <t>non-hedged</t>
   </si>
   <si>
-    <t>Replication</t>
+    <t>accumulating</t>
+  </si>
+  <si>
+    <t>sampling</t>
+  </si>
+  <si>
+    <t>Reflazione / Ripresa</t>
+  </si>
+  <si>
+    <t>Valuta indifferente nel lungo periodo. Meglio non hedgiati</t>
+  </si>
+  <si>
+    <t>iShares Edge MSCI World Momentum Factor UCITS ETF (Acc) | IWMO | IE00BP3QZ825</t>
+  </si>
+  <si>
+    <t>World Momentum</t>
+  </si>
+  <si>
+    <t>iShares Edge MSCI World Momentum Factor UCITS ETF</t>
+  </si>
+  <si>
+    <t>IE00BP3QZ825</t>
+  </si>
+  <si>
+    <t>IWMO.L</t>
+  </si>
+  <si>
+    <t>EUR</t>
+  </si>
+  <si>
+    <t>acc</t>
+  </si>
+  <si>
+    <t>full replication</t>
+  </si>
+  <si>
+    <t>iShares Edge MSCI USA Quality Factor UCITS ETF | QDVB | IE00BD1F4L37</t>
+  </si>
+  <si>
+    <t>US Quality</t>
+  </si>
+  <si>
+    <t>iShares Edge MSCI USA Quality Factor UCITS ETF</t>
+  </si>
+  <si>
+    <t>IE00BD1F4L37</t>
+  </si>
+  <si>
+    <t>QDVB.DE</t>
+  </si>
+  <si>
+    <t>iShares Edge MSCI World Minimum Volatility UCITS ETF USD (Acc) | MVOL | IE00B8FHGS14</t>
+  </si>
+  <si>
+    <t>World Low Volatility</t>
+  </si>
+  <si>
+    <t>iShares Edge MSCI World Minimum Volatility UCITS ETF USD (Acc)</t>
+  </si>
+  <si>
+    <t>IE00B8FHGS14</t>
+  </si>
+  <si>
+    <t>MVOL.L</t>
+  </si>
+  <si>
+    <t>Xtrackers MSCI World Health Care UCITS ETF 1C | XDWH | IE00BM67HK77</t>
+  </si>
+  <si>
+    <t>World Health Care</t>
+  </si>
+  <si>
+    <t>Xtrackers MSCI World Health Care UCITS ETF 1C</t>
+  </si>
+  <si>
+    <t>IE00BM67HK77</t>
+  </si>
+  <si>
+    <t>XDWH.MI</t>
+  </si>
+  <si>
+    <t>Xtrackers MSCI World Consumer Staples UCITS ETF 1C | XDWS | IE00BM67HN09</t>
+  </si>
+  <si>
+    <t>Consumer Staples Global</t>
+  </si>
+  <si>
+    <t>Xtrackers MSCI World Consumer Staples UCITS ETF (Acc)</t>
+  </si>
+  <si>
+    <t>XDWS.L</t>
+  </si>
+  <si>
+    <t>iShares MSCI World Small Cap UCITS ETF | IUSN | IE00BF4RFH31</t>
+  </si>
+  <si>
+    <t>Small Cap Global</t>
+  </si>
+  <si>
+    <t>iShares MSCI World Small Cap UCITS ETF</t>
+  </si>
+  <si>
+    <t>IE00BF4RFH31</t>
+  </si>
+  <si>
+    <t>WSML.L</t>
+  </si>
+  <si>
+    <t>iShares Euro Corporate Bond Large Cap UCITS ETF | IBCX | IE0032523478</t>
+  </si>
+  <si>
+    <t>EU Corp Large Cap bonds</t>
+  </si>
+  <si>
+    <t>iShares Euro Corporate Bond Large Cap UCITS ETF</t>
+  </si>
+  <si>
+    <t>IE0032523478</t>
+  </si>
+  <si>
+    <t>IBCX.AS</t>
+  </si>
+  <si>
+    <t>dist</t>
+  </si>
+  <si>
+    <t>0.2%</t>
+  </si>
+  <si>
+    <t>iShares Euro Government Bond 7-10yr UCITS ETF (Acc) | SXRQ | IE00B3VTN290</t>
+  </si>
+  <si>
+    <t>EU Gov bonds 7-10y</t>
+  </si>
+  <si>
+    <t>iShares € Govt Bond 7-10yr UCITS ETF EUR (Dist)</t>
+  </si>
+  <si>
+    <t>IE00B1FZS806</t>
+  </si>
+  <si>
+    <t>IBGM.AS</t>
+  </si>
+  <si>
+    <t>Depressione / Recessione</t>
+  </si>
+  <si>
+    <t>per i GVT si consiglia di utilizzare strumenti in euro per eliminare il rischio cambio e rilegare l'esposizione al dollaro nella componente dedicata. In euro per eliminare il rischio cambio e rilegare l'esposizione al dollaro nella componente dedicata.</t>
+  </si>
+  <si>
+    <t>iShares Euro Inflation Linked Government Bond UCITS ETF | IBCI | IE00B0M62X26</t>
+  </si>
+  <si>
+    <t>EU Inflation-Linked</t>
+  </si>
+  <si>
+    <t>iShares € Inflation Linked Govt Bond UCITS ETF EUR (Acc)</t>
+  </si>
+  <si>
+    <t>IE00B0M62X26</t>
+  </si>
+  <si>
+    <t>IBCI.AS</t>
+  </si>
+  <si>
+    <t>Amundi EUR Overnight Return UCITS ETF Acc (LEONIA.MI) Stock Price, News, Quote &amp; History - Yahoo Finance</t>
+  </si>
+  <si>
+    <t>EU Overnight</t>
+  </si>
+  <si>
+    <t>Amundi EUR Overnight Return UCITS ETF Acc</t>
+  </si>
+  <si>
+    <t>FR0010510800</t>
+  </si>
+  <si>
+    <t>LEONIA.MI</t>
+  </si>
+  <si>
+    <t>unfunded swap</t>
+  </si>
+  <si>
+    <t>quota cash</t>
+  </si>
+  <si>
+    <t>iShares USD Treasury Bond 0-1yr UCITS ETF USD (Dist) | IBCC | IE00BGR7L912</t>
+  </si>
+  <si>
+    <t>US Short Treasury</t>
+  </si>
+  <si>
+    <t>iShares USD Treasury Bond 0-1yr UCITS ETF (Dist)</t>
+  </si>
+  <si>
+    <t>IE00BGR7L912</t>
+  </si>
+  <si>
+    <t>IBTU.L</t>
+  </si>
+  <si>
+    <t>Recessione / Iperinflazione</t>
+  </si>
+  <si>
+    <t>Invesco Physical Gold A | SGLD | IE00B579F325</t>
+  </si>
+  <si>
+    <t>ETC GOLD</t>
+  </si>
+  <si>
+    <t>Invesco Physical Gold ETC</t>
+  </si>
+  <si>
+    <t>IE00B579F325</t>
+  </si>
+  <si>
+    <t>SGLD.AS</t>
+  </si>
+  <si>
+    <t>Reflazione / Inflazione</t>
+  </si>
+  <si>
+    <t>Sui Treasury, bisogna gestire rischio cambio e rischio tasso: se ci si espone ai Treasury 0-1y, si elimina il rischo tasso, mentre, nei casi di esposizine 1-3y, si potrebbe beneficiare del rischio tasso in fasi recessive. In linea generale, avendo altri strumenti deputati alla copertura delle depressioni/recessioni, la scelta 0-1y potrebbe essere la più efficiente.</t>
+  </si>
+  <si>
+    <t>SPY</t>
+  </si>
+  <si>
+    <t>Amundi S&amp;P 500 UCITS ETF</t>
+  </si>
+  <si>
+    <t>LU1681048804</t>
+  </si>
+  <si>
+    <t>500.PA</t>
+  </si>
+  <si>
+    <t>swap-based</t>
+  </si>
+  <si>
+    <t>MSCI EM</t>
   </si>
   <si>
     <t xml:space="preserve">Amundi MSCI Emerging Markets UCITS </t>
   </si>
   <si>
-    <t>Currency</t>
-  </si>
-  <si>
-    <t>USD</t>
-  </si>
-  <si>
     <t>LU1681045370</t>
   </si>
   <si>
-    <t>MSCI EM</t>
-  </si>
-  <si>
-    <t>MSCI World</t>
+    <t>AEEM.PA</t>
+  </si>
+  <si>
+    <t>Bloomberg Euro gvt bonds 7-10y</t>
   </si>
   <si>
     <t>iShares Euro Government Bond 7-10yr UCITS ETF (Acc)</t>
@@ -356,40 +623,157 @@
     <t>IE00B3VTN290</t>
   </si>
   <si>
-    <t>EUR</t>
-  </si>
-  <si>
-    <t>Bloomberg Euro gvt bonds 7-10y</t>
-  </si>
-  <si>
-    <t>Index</t>
+    <t>SXRQ.DE</t>
+  </si>
+  <si>
+    <t>Bloomberg Global Aggregate Bond</t>
+  </si>
+  <si>
+    <t>iShares Core Global Aggregate Bond UCITS ETF EUR Hedged (Acc)</t>
+  </si>
+  <si>
+    <t>IE00BDBRDM35</t>
+  </si>
+  <si>
+    <t>0GGH.L</t>
+  </si>
+  <si>
+    <t>hedged</t>
+  </si>
+  <si>
+    <t>Bloomberg Euro Inflation Linked</t>
+  </si>
+  <si>
+    <t>Lyxor Euro Government Inflation Linked Bnd</t>
+  </si>
+  <si>
+    <t>LU1650491282</t>
+  </si>
+  <si>
+    <t>EMI.MI</t>
+  </si>
+  <si>
+    <t>L'uso delle obbligazioni inflation linked deve essere ben compreso, perchè il loro potenziale diversificativo e protettivo è massimo in scenari reflattivi, non inflattivi (in cui, come il resto dei bonds, perdono valore al rialzo dei tassi reali). Meglio in EUR per comprire rischio cambio.</t>
+  </si>
+  <si>
+    <t>Bloomberg US Short Treasury</t>
+  </si>
+  <si>
+    <t>iShares USD Treasury Bond 0-1yr UCITS ETF (Acc)</t>
+  </si>
+  <si>
+    <t>IE00BGSF1X88</t>
+  </si>
+  <si>
+    <t>IB01.L</t>
+  </si>
+  <si>
+    <t>Deutsche Bank Euro Overnight Rate</t>
+  </si>
+  <si>
+    <t>Xtrackers II EUR Overnight Rate Swap UCITS ETF 1C</t>
+  </si>
+  <si>
+    <t>IE00B3BPCH51</t>
+  </si>
+  <si>
+    <t>XEON.F</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Maturity inferiore all'anno per coprire il portafoglio in fasi recessive, ad alta volatilità, oltre che in fasi di forte rialzo dei tassi di interesse. Euro per coprire</t>
+  </si>
+  <si>
+    <t>Invesco Physical Gold A</t>
+  </si>
+  <si>
+    <t>LU0290358497</t>
+  </si>
+  <si>
+    <t>SGLD.L</t>
+  </si>
+  <si>
+    <t>Bloomberg US 1-3 Year Treasury Bond</t>
+  </si>
+  <si>
+    <t>SPDR Bloomberg 1-3 Year US Treasury Bond UCITS ETF</t>
+  </si>
+  <si>
+    <t>IE00BC7GZJ81</t>
+  </si>
+  <si>
+    <t>TRS3.L</t>
+  </si>
+  <si>
+    <t>le scelte sui accumulating nei bond sono dovute principalmente alla grandezza del ptf, non avendo decina di k, è inutile puntare sui distributing di asset che pesano meno del 10%</t>
+  </si>
+  <si>
+    <t>iBoxx® EUR Liquid High Yield</t>
+  </si>
+  <si>
+    <t>iShares Global Government Bond UCITS ETF USD (Dist)</t>
+  </si>
+  <si>
+    <t>IE00B3F81K65</t>
+  </si>
+  <si>
+    <t>IGLO.L</t>
+  </si>
+  <si>
+    <t>distributing</t>
+  </si>
+  <si>
+    <t>Bloomberg US Inflation Linked</t>
+  </si>
+  <si>
+    <t>iShares USD TIPS UCITS ETF USD (ACC)</t>
+  </si>
+  <si>
+    <t>IE00B1FZSC47</t>
+  </si>
+  <si>
+    <t>ITPS.SW</t>
+  </si>
+  <si>
+    <t>viste le azioni in usd, è un'ulteriore componente in dollari che attenui la volatilità nei momenti difficili dei mercati.</t>
+  </si>
+  <si>
+    <t>FTSE Gvt Bonds Developed Markets</t>
+  </si>
+  <si>
+    <t>Xtrackers Global Government Bond UCITS ETF 1D EUR hedged</t>
+  </si>
+  <si>
+    <t>LU0690964092</t>
+  </si>
+  <si>
+    <t>XGVD.DE</t>
   </si>
   <si>
     <t>Bloomberg Euro gvt bonds 1-3y</t>
   </si>
   <si>
-    <t>Bloomberg Global Aggregate Bond</t>
-  </si>
-  <si>
-    <t>IE00BDBRDM35</t>
-  </si>
-  <si>
-    <t>iShares Core Global Aggregate Bond UCITS ETF EUR Hedged (Acc)</t>
-  </si>
-  <si>
-    <t>FTSE Gvt Bonds Developed Markets</t>
-  </si>
-  <si>
     <t>SPDR Bloomberg 1-3 Year Euro Government Bond UCITS ETF</t>
   </si>
   <si>
     <t>IE00B6YX5F63</t>
   </si>
   <si>
-    <t>Xtrackers Global Government Bond UCITS ETF 1D EUR hedged</t>
-  </si>
-  <si>
-    <t>LU0690964092</t>
+    <t>SYB3.DE</t>
+  </si>
+  <si>
+    <t>Bloomberg Global Aggregate Corporate</t>
+  </si>
+  <si>
+    <t>Vanguard USD Corporate Bond UCITS ETF Accumulating</t>
+  </si>
+  <si>
+    <t>IE00BGYWFK87</t>
+  </si>
+  <si>
+    <t>VDPA.L</t>
+  </si>
+  <si>
+    <t>L'indice Bloomberg Global Aggregate Corporate USD replica obbligazioni con valuta dollari statunitensi emesse nei mercati emergenti e sviluppati in tutto il mondo. Tutte le scadenze sono incluse. Rating: Investment Grade.</t>
   </si>
   <si>
     <t>iShares Global Government Bond UCITS ETF (Acc)</t>
@@ -398,19 +782,7 @@
     <t>IE00BYZ28V50</t>
   </si>
   <si>
-    <t>hedged</t>
-  </si>
-  <si>
-    <t>accumulating</t>
-  </si>
-  <si>
-    <t>distributing</t>
-  </si>
-  <si>
-    <t>sampling</t>
-  </si>
-  <si>
-    <t>swap-based</t>
+    <t>IGLA.L</t>
   </si>
   <si>
     <t>Vanguard EUR Corporate Bond UCITS ETF Accumulating</t>
@@ -419,178 +791,46 @@
     <t>IE00BGYWT403</t>
   </si>
   <si>
-    <t>Vanguard USD Corporate Bond UCITS ETF Accumulating</t>
-  </si>
-  <si>
-    <t>Bloomberg Global Aggregate Corporate</t>
-  </si>
-  <si>
-    <t>IE00BGYWFK87</t>
-  </si>
-  <si>
-    <t>iBoxx® EUR Liquid High Yield</t>
-  </si>
-  <si>
-    <t>iShares Global Government Bond UCITS ETF USD (Dist)</t>
-  </si>
-  <si>
-    <t>IE00B3F81K65</t>
-  </si>
-  <si>
-    <t>Comments</t>
-  </si>
-  <si>
-    <t>viste le azioni in usd, è un'ulteriore componente in dollari che attenui la volatilità nei momenti difficili dei mercati.</t>
-  </si>
-  <si>
-    <t>iShares USD TIPS UCITS ETF USD (ACC)</t>
-  </si>
-  <si>
-    <t>Bloomberg US Inflation Linked</t>
-  </si>
-  <si>
-    <t>IE00B1FZSC47</t>
-  </si>
-  <si>
-    <t>Lyxor Euro Government Inflation Linked Bnd</t>
-  </si>
-  <si>
-    <t>Bloomberg Euro Inflation Linked</t>
-  </si>
-  <si>
-    <t>LU1650491282</t>
-  </si>
-  <si>
-    <t>Bloomberg US 1-3 Year Treasury Bond</t>
-  </si>
-  <si>
-    <t>Bloomberg US Short Treasury</t>
-  </si>
-  <si>
-    <t>full replication</t>
-  </si>
-  <si>
-    <t>le scelte sui accumulating nei bond sono dovute principalmente alla grandezza del ptf, non avendo decina di k, è inutile puntare sui distributing di asset che pesano meno del 10%</t>
-  </si>
-  <si>
-    <t>Ticker</t>
-  </si>
-  <si>
-    <t>SXRQ.DE</t>
-  </si>
-  <si>
-    <t>EMI.MI</t>
-  </si>
-  <si>
-    <t>IWDA.L</t>
-  </si>
-  <si>
-    <t>AEEM.PA</t>
-  </si>
-  <si>
-    <t>XGVD.DE</t>
-  </si>
-  <si>
-    <t>IGLA.L</t>
-  </si>
-  <si>
-    <t>0GGH.L</t>
-  </si>
-  <si>
     <t>VECA.DE</t>
   </si>
   <si>
-    <t>VDPA.L</t>
-  </si>
-  <si>
-    <t>IGLO.L</t>
-  </si>
-  <si>
-    <t>ITPS.SW</t>
-  </si>
-  <si>
-    <t>SYB3.DE</t>
-  </si>
-  <si>
-    <t>IE00BGSF1X88</t>
-  </si>
-  <si>
-    <t>IB01.L</t>
-  </si>
-  <si>
-    <t>iShares USD Treasury Bond 0-1yr UCITS ETF (Acc)</t>
-  </si>
-  <si>
-    <t>TRS3.L</t>
-  </si>
-  <si>
-    <t>IE00BC7GZJ81</t>
-  </si>
-  <si>
-    <t>SPDR Bloomberg 1-3 Year US Treasury Bond UCITS ETF</t>
-  </si>
-  <si>
-    <t>ETC GOLD</t>
-  </si>
-  <si>
-    <t>SGLD.L</t>
-  </si>
-  <si>
-    <t>Invesco Physical Gold A</t>
-  </si>
-  <si>
-    <t>SPY</t>
-  </si>
-  <si>
-    <t>LU1681048804</t>
-  </si>
-  <si>
-    <t>500.PA</t>
-  </si>
-  <si>
-    <t>Amundi S&amp;P 500 UCITS ETF</t>
-  </si>
-  <si>
-    <t>Sui Treasury, bisogna gestire rischio cambio e rischio tasso: se ci si espone ai Treasury 0-1y, si elimina il rischo tasso, mentre, nei casi di esposizine 1-3y, si potrebbe beneficiare del rischio tasso in fasi recessive. In linea generale, avendo altri strumenti deputati alla copertura delle depressioni/recessioni, la scelta 0-1y potrebbe essere la più efficiente.</t>
-  </si>
-  <si>
-    <t>Scenario macro coperto</t>
-  </si>
-  <si>
-    <t>Depressione / Recessione</t>
-  </si>
-  <si>
-    <t>Recessione / Iperinflazione</t>
-  </si>
-  <si>
-    <t>Reflazione / Inflazione</t>
-  </si>
-  <si>
-    <t>L'uso delle obbligazioni inflation linked deve essere ben compreso, perchè il loro potenziale diversificativo e protettivo è massimo in scenari reflattivi, non inflattivi (in cui, come il resto dei bonds, perdono valore al rialzo dei tassi reali). Meglio in EUR per comprire rischio cambio.</t>
-  </si>
-  <si>
-    <t>per i GVT si consiglia di utilizzare strumenti in euro per eliminare il rischio cambio e rilegare l'esposizione al dollaro nella componente dedicata. In euro per eliminare il rischio cambio e rilegare l'esposizione al dollaro nella componente dedicata.</t>
-  </si>
-  <si>
-    <t>L'indice Bloomberg Global Aggregate Corporate USD replica obbligazioni con valuta dollari statunitensi emesse nei mercati emergenti e sviluppati in tutto il mondo. Tutte le scadenze sono incluse. Rating: Investment Grade.</t>
-  </si>
-  <si>
-    <t>Xtrackers II EUR Overnight Rate Swap UCITS ETF 1C</t>
-  </si>
-  <si>
-    <t>Deutsche Bank Euro Overnight Rate</t>
-  </si>
-  <si>
-    <t>IE00B3BPCH51</t>
-  </si>
-  <si>
-    <t>LU0290358497</t>
-  </si>
-  <si>
-    <t>XEON.F</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Maturity inferiore all'anno per coprire il portafoglio in fasi recessive, ad alta volatilità, oltre che in fasi di forte rialzo dei tassi di interesse. Euro per coprire</t>
+    <t>world quality</t>
+  </si>
+  <si>
+    <t>iShares Edge MSCI World Quality Factor UCITS ETF (Acc)</t>
+  </si>
+  <si>
+    <t>IE00BP3QZ601</t>
+  </si>
+  <si>
+    <t>IWQU.L</t>
+  </si>
+  <si>
+    <t>low volatility</t>
+  </si>
+  <si>
+    <t>US quality</t>
+  </si>
+  <si>
+    <t>IE00BM67HN09</t>
+  </si>
+  <si>
+    <t>Amundi Euro Inflation Expectations 2-10Y UCITS ETF Acc | INFL | LU1390062245</t>
+  </si>
+  <si>
+    <t>EU Break-Even 2-10y</t>
+  </si>
+  <si>
+    <t>Amundi Euro Inflation Expectations 2-10Y UCITS ETF Acc</t>
+  </si>
+  <si>
+    <t>LU1390062245</t>
+  </si>
+  <si>
+    <t>INFL.PA</t>
+  </si>
+  <si>
+    <t>swap</t>
   </si>
   <si>
     <t xml:space="preserve">COMPONENTE OBBLIGAZIONARIA </t>
@@ -1051,231 +1291,6 @@
   </si>
   <si>
     <t>0.79</t>
-  </si>
-  <si>
-    <t>Reflazione / Ripresa</t>
-  </si>
-  <si>
-    <t>Valuta indifferente nel lungo periodo. Meglio non hedgiati</t>
-  </si>
-  <si>
-    <t>Small Cap Global</t>
-  </si>
-  <si>
-    <t>iShares Edge MSCI World Momentum Factor UCITS ETF</t>
-  </si>
-  <si>
-    <t>IE00BP3QZ825</t>
-  </si>
-  <si>
-    <t>iShares MSCI World Small Cap UCITS ETF</t>
-  </si>
-  <si>
-    <t>WSML.L</t>
-  </si>
-  <si>
-    <t>Xtrackers MSCI World Consumer Staples UCITS ETF (Acc)</t>
-  </si>
-  <si>
-    <t>IE00BM67HN09</t>
-  </si>
-  <si>
-    <t>XDWS.L</t>
-  </si>
-  <si>
-    <t>IWMO.L</t>
-  </si>
-  <si>
-    <t>Link</t>
-  </si>
-  <si>
-    <t>Consumer Staples Global</t>
-  </si>
-  <si>
-    <t>Xtrackers MSCI World Consumer Staples UCITS ETF 1C | XDWS | IE00BM67HN09</t>
-  </si>
-  <si>
-    <t>iShares Edge MSCI World Momentum Factor UCITS ETF (Acc) | IWMO | IE00BP3QZ825</t>
-  </si>
-  <si>
-    <t>iShares MSCI World Small Cap UCITS ETF | IUSN | IE00BF4RFH31</t>
-  </si>
-  <si>
-    <t>iShares Euro Government Bond 7-10yr UCITS ETF (Acc) | SXRQ | IE00B3VTN290</t>
-  </si>
-  <si>
-    <t>IE00B1FZS806</t>
-  </si>
-  <si>
-    <t>EU Gov bonds 7-10y</t>
-  </si>
-  <si>
-    <t>US Short Treasury</t>
-  </si>
-  <si>
-    <t>dist</t>
-  </si>
-  <si>
-    <t>IBGM.AS</t>
-  </si>
-  <si>
-    <t>iShares € Govt Bond 7-10yr UCITS ETF EUR (Dist)</t>
-  </si>
-  <si>
-    <t>iShares USD Treasury Bond 0-1yr UCITS ETF USD (Dist) | IBCC | IE00BGR7L912</t>
-  </si>
-  <si>
-    <t>iShares USD Treasury Bond 0-1yr UCITS ETF (Dist)</t>
-  </si>
-  <si>
-    <t>IE00BGR7L912</t>
-  </si>
-  <si>
-    <t>IBTU.L</t>
-  </si>
-  <si>
-    <t>acc</t>
-  </si>
-  <si>
-    <t>IE00B579F325</t>
-  </si>
-  <si>
-    <t>Invesco Physical Gold ETC</t>
-  </si>
-  <si>
-    <t>SGLD.AS</t>
-  </si>
-  <si>
-    <t>Invesco Physical Gold A | SGLD | IE00B579F325</t>
-  </si>
-  <si>
-    <t>IE00BF4RFH31</t>
-  </si>
-  <si>
-    <t>IE00BP3QZ601</t>
-  </si>
-  <si>
-    <t>iShares Edge MSCI World Quality Factor UCITS ETF (Acc)</t>
-  </si>
-  <si>
-    <t>IWQU.L</t>
-  </si>
-  <si>
-    <t>iShares Edge MSCI World Minimum Volatility UCITS ETF USD (Acc)</t>
-  </si>
-  <si>
-    <t>IE00B8FHGS14</t>
-  </si>
-  <si>
-    <t>MVOL.L</t>
-  </si>
-  <si>
-    <t>low volatility</t>
-  </si>
-  <si>
-    <t>world quality</t>
-  </si>
-  <si>
-    <t>US quality</t>
-  </si>
-  <si>
-    <t>IE00BD1F4L37</t>
-  </si>
-  <si>
-    <t>QDVB.DE</t>
-  </si>
-  <si>
-    <t>iShares Edge MSCI USA Quality Factor UCITS ETF</t>
-  </si>
-  <si>
-    <t>World Momentum</t>
-  </si>
-  <si>
-    <t>US Quality</t>
-  </si>
-  <si>
-    <t>World Low Volatility</t>
-  </si>
-  <si>
-    <t>iShares Edge MSCI USA Quality Factor UCITS ETF | QDVB | IE00BD1F4L37</t>
-  </si>
-  <si>
-    <t>iShares Edge MSCI World Minimum Volatility UCITS ETF USD (Acc) | MVOL | IE00B8FHGS14</t>
-  </si>
-  <si>
-    <t>IBCX.AS</t>
-  </si>
-  <si>
-    <t>0.2%</t>
-  </si>
-  <si>
-    <t>iShares Euro Corporate Bond Large Cap UCITS ETF | IBCX | IE0032523478</t>
-  </si>
-  <si>
-    <t>iShares Euro Corporate Bond Large Cap UCITS ETF</t>
-  </si>
-  <si>
-    <t>EU Corp Large Cap bonds</t>
-  </si>
-  <si>
-    <t>IE0032523478</t>
-  </si>
-  <si>
-    <t>LEONIA.MI</t>
-  </si>
-  <si>
-    <t>Amundi EUR Overnight Return UCITS ETF Acc (LEONIA.MI) Stock Price, News, Quote &amp; History - Yahoo Finance</t>
-  </si>
-  <si>
-    <t>Amundi EUR Overnight Return UCITS ETF Acc</t>
-  </si>
-  <si>
-    <t>EU Overnight</t>
-  </si>
-  <si>
-    <t>FR0010510800</t>
-  </si>
-  <si>
-    <t>unfunded swap</t>
-  </si>
-  <si>
-    <t>quota cash</t>
-  </si>
-  <si>
-    <t>IE00B0M62X26</t>
-  </si>
-  <si>
-    <t>IBCI.AS</t>
-  </si>
-  <si>
-    <t>EU Inflation-Linked</t>
-  </si>
-  <si>
-    <t>iShares Euro Inflation Linked Government Bond UCITS ETF | IBCI | IE00B0M62X26</t>
-  </si>
-  <si>
-    <t>LU1390062245</t>
-  </si>
-  <si>
-    <t>iShares € Inflation Linked Govt Bond UCITS ETF EUR (Acc)</t>
-  </si>
-  <si>
-    <t>Amundi Euro Inflation Expectations 2-10Y UCITS ETF Acc | INFL | LU1390062245</t>
-  </si>
-  <si>
-    <t>EU Break-Even 2-10y</t>
-  </si>
-  <si>
-    <t>Amundi Euro Inflation Expectations 2-10Y UCITS ETF Acc</t>
-  </si>
-  <si>
-    <t>INFL.PA</t>
-  </si>
-  <si>
-    <t>swap</t>
-  </si>
-  <si>
-    <t>iShares Core MSCI World UCITS ETF USD (Acc) | SWDA | IE00B4L5Y983</t>
   </si>
 </sst>
 </file>
@@ -1705,21 +1720,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="102">
+  <cellXfs count="103">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1768,6 +1781,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1960,9 +1976,11 @@
     <xf numFmtId="0" fontId="7" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="4" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="5">
     <cellStyle name="Collegamento ipertestuale" xfId="3" builtinId="8"/>
+    <cellStyle name="Hyperlink" xfId="4" xr:uid="{00000000-000B-0000-0000-000008000000}"/>
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
     <cellStyle name="Normale 2" xfId="1" xr:uid="{72EA356F-0A49-47BB-9DAA-0B0102CDB9D4}"/>
     <cellStyle name="Valuta 2" xfId="2" xr:uid="{B87CA5A7-8DFB-4A60-8670-448CAC58448C}"/>
@@ -1978,10 +1996,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2247,494 +2261,524 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B015881-81C4-40D2-9396-65046E56EE7C}">
-  <dimension ref="A1:L13"/>
+  <dimension ref="A1:L14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.45"/>
   <cols>
-    <col min="1" max="1" width="39.9453125" customWidth="1"/>
-    <col min="2" max="2" width="52.7890625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="52.1015625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.41796875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.26171875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.9453125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.1015625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.26171875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="5.5234375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.89453125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="21.7890625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="255.578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="40" customWidth="1"/>
+    <col min="2" max="2" width="52.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="52.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="255.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" s="2" t="s">
-        <v>162</v>
+        <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12">
+      <c r="A2" s="35" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H2" t="s">
         <v>19</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12">
-      <c r="A2" s="36" t="s">
-        <v>225</v>
-      </c>
-      <c r="B2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D2" t="s">
-        <v>1</v>
-      </c>
-      <c r="E2" t="s">
-        <v>59</v>
-      </c>
-      <c r="F2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G2" t="s">
-        <v>7</v>
-      </c>
-      <c r="H2" t="s">
-        <v>32</v>
       </c>
       <c r="I2" s="1">
         <v>2E-3</v>
       </c>
       <c r="J2" t="s">
-        <v>34</v>
+        <v>20</v>
       </c>
       <c r="K2" t="s">
-        <v>151</v>
+        <v>21</v>
       </c>
       <c r="L2" t="s">
-        <v>152</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:12">
-      <c r="A3" s="36" t="s">
-        <v>165</v>
+      <c r="A3" s="35" t="s">
+        <v>23</v>
       </c>
       <c r="B3" t="s">
-        <v>196</v>
+        <v>24</v>
       </c>
       <c r="C3" t="s">
-        <v>154</v>
+        <v>25</v>
       </c>
       <c r="D3" t="s">
-        <v>155</v>
+        <v>26</v>
       </c>
       <c r="E3" t="s">
-        <v>161</v>
+        <v>27</v>
       </c>
       <c r="F3" t="s">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="G3" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="H3" t="s">
-        <v>178</v>
+        <v>29</v>
       </c>
       <c r="I3" s="1">
         <v>2.5000000000000001E-3</v>
       </c>
       <c r="J3" t="s">
-        <v>54</v>
+        <v>30</v>
       </c>
       <c r="K3" t="s">
-        <v>151</v>
+        <v>21</v>
       </c>
       <c r="L3" t="s">
-        <v>152</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:12">
-      <c r="A4" s="36" t="s">
-        <v>199</v>
+      <c r="A4" s="35" t="s">
+        <v>31</v>
       </c>
       <c r="B4" t="s">
-        <v>197</v>
+        <v>32</v>
       </c>
       <c r="C4" t="s">
-        <v>195</v>
+        <v>33</v>
       </c>
       <c r="D4" t="s">
-        <v>193</v>
+        <v>34</v>
       </c>
       <c r="E4" t="s">
-        <v>194</v>
+        <v>35</v>
       </c>
       <c r="F4" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="G4" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="H4" t="s">
-        <v>32</v>
+        <v>19</v>
       </c>
       <c r="I4" s="1">
         <v>2E-3</v>
       </c>
       <c r="J4" t="s">
-        <v>54</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:12">
-      <c r="A5" s="36" t="s">
-        <v>200</v>
+      <c r="A5" s="35" t="s">
+        <v>36</v>
       </c>
       <c r="B5" t="s">
-        <v>198</v>
+        <v>37</v>
       </c>
       <c r="C5" t="s">
-        <v>187</v>
+        <v>38</v>
       </c>
       <c r="D5" t="s">
-        <v>188</v>
+        <v>39</v>
       </c>
       <c r="E5" t="s">
-        <v>189</v>
+        <v>40</v>
       </c>
       <c r="F5" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="G5" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="H5" t="s">
-        <v>32</v>
+        <v>19</v>
       </c>
       <c r="I5" s="1">
         <v>3.0000000000000001E-3</v>
       </c>
       <c r="J5" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12">
-      <c r="A6" s="36" t="s">
-        <v>164</v>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="15">
+      <c r="A6" s="102" t="s">
+        <v>41</v>
       </c>
       <c r="B6" t="s">
-        <v>163</v>
+        <v>42</v>
       </c>
       <c r="C6" t="s">
-        <v>158</v>
+        <v>43</v>
       </c>
       <c r="D6" t="s">
-        <v>159</v>
+        <v>44</v>
       </c>
       <c r="E6" t="s">
-        <v>160</v>
+        <v>45</v>
       </c>
       <c r="F6" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="G6" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="H6" t="s">
-        <v>178</v>
+        <v>19</v>
       </c>
       <c r="I6" s="1">
         <v>2.5000000000000001E-3</v>
       </c>
-      <c r="J6" t="s">
+    </row>
+    <row r="7" spans="1:12">
+      <c r="A7" s="35" t="s">
+        <v>46</v>
+      </c>
+      <c r="B7" t="s">
+        <v>47</v>
+      </c>
+      <c r="C7" t="s">
+        <v>48</v>
+      </c>
+      <c r="D7" t="s">
+        <v>44</v>
+      </c>
+      <c r="E7" t="s">
+        <v>49</v>
+      </c>
+      <c r="F7" t="s">
+        <v>17</v>
+      </c>
+      <c r="G7" t="s">
+        <v>18</v>
+      </c>
+      <c r="H7" t="s">
+        <v>29</v>
+      </c>
+      <c r="I7" s="1">
+        <v>2.5000000000000001E-3</v>
+      </c>
+      <c r="J7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12">
+      <c r="A8" s="35" t="s">
+        <v>50</v>
+      </c>
+      <c r="B8" t="s">
+        <v>51</v>
+      </c>
+      <c r="C8" t="s">
+        <v>52</v>
+      </c>
+      <c r="D8" t="s">
+        <v>53</v>
+      </c>
+      <c r="E8" t="s">
         <v>54</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12">
-      <c r="A7" s="36" t="s">
-        <v>166</v>
-      </c>
-      <c r="B7" t="s">
-        <v>153</v>
-      </c>
-      <c r="C7" t="s">
-        <v>156</v>
-      </c>
-      <c r="D7" t="s">
-        <v>183</v>
-      </c>
-      <c r="E7" t="s">
-        <v>157</v>
-      </c>
-      <c r="F7" t="s">
-        <v>11</v>
-      </c>
-      <c r="G7" t="s">
-        <v>7</v>
-      </c>
-      <c r="H7" t="s">
-        <v>178</v>
-      </c>
-      <c r="I7" s="1">
-        <v>3.5000000000000001E-3</v>
-      </c>
-      <c r="J7" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12">
-      <c r="A8" s="36" t="s">
-        <v>203</v>
-      </c>
-      <c r="B8" t="s">
-        <v>205</v>
-      </c>
-      <c r="C8" t="s">
-        <v>204</v>
-      </c>
-      <c r="D8" t="s">
-        <v>206</v>
-      </c>
-      <c r="E8" t="s">
-        <v>201</v>
       </c>
       <c r="F8" t="s">
         <v>17</v>
       </c>
       <c r="G8" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="H8" t="s">
-        <v>171</v>
-      </c>
-      <c r="I8" s="1" t="s">
-        <v>202</v>
+        <v>29</v>
+      </c>
+      <c r="I8" s="1">
+        <v>3.5000000000000001E-3</v>
       </c>
       <c r="J8" t="s">
-        <v>34</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:12">
-      <c r="A9" s="36" t="s">
-        <v>167</v>
+      <c r="A9" s="35" t="s">
+        <v>55</v>
       </c>
       <c r="B9" t="s">
-        <v>169</v>
+        <v>56</v>
       </c>
       <c r="C9" t="s">
-        <v>173</v>
+        <v>57</v>
       </c>
       <c r="D9" t="s">
-        <v>168</v>
+        <v>58</v>
       </c>
       <c r="E9" t="s">
-        <v>172</v>
+        <v>59</v>
       </c>
       <c r="F9" t="s">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="G9" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="H9" t="s">
-        <v>171</v>
-      </c>
-      <c r="I9" s="1">
+        <v>60</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="J9" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12">
+      <c r="A10" s="35" t="s">
+        <v>62</v>
+      </c>
+      <c r="B10" t="s">
+        <v>63</v>
+      </c>
+      <c r="C10" t="s">
+        <v>64</v>
+      </c>
+      <c r="D10" t="s">
+        <v>65</v>
+      </c>
+      <c r="E10" t="s">
+        <v>66</v>
+      </c>
+      <c r="F10" t="s">
+        <v>28</v>
+      </c>
+      <c r="G10" t="s">
+        <v>18</v>
+      </c>
+      <c r="H10" t="s">
+        <v>60</v>
+      </c>
+      <c r="I10" s="1">
         <v>1.5E-3</v>
       </c>
-      <c r="J9" t="s">
-        <v>34</v>
-      </c>
-      <c r="K9" t="s">
+      <c r="J10" t="s">
+        <v>20</v>
+      </c>
+      <c r="K10" t="s">
+        <v>67</v>
+      </c>
+      <c r="L10" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12">
+      <c r="A11" s="35" t="s">
+        <v>69</v>
+      </c>
+      <c r="B11" t="s">
+        <v>70</v>
+      </c>
+      <c r="C11" t="s">
+        <v>71</v>
+      </c>
+      <c r="D11" t="s">
+        <v>72</v>
+      </c>
+      <c r="E11" t="s">
+        <v>73</v>
+      </c>
+      <c r="F11" t="s">
+        <v>28</v>
+      </c>
+      <c r="G11" t="s">
+        <v>18</v>
+      </c>
+      <c r="H11" t="s">
+        <v>29</v>
+      </c>
+      <c r="I11" s="1">
+        <v>8.9999999999999998E-4</v>
+      </c>
+      <c r="J11" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12">
+      <c r="A12" s="35" t="s">
+        <v>74</v>
+      </c>
+      <c r="B12" t="s">
+        <v>75</v>
+      </c>
+      <c r="C12" t="s">
+        <v>76</v>
+      </c>
+      <c r="D12" t="s">
+        <v>77</v>
+      </c>
+      <c r="E12" t="s">
+        <v>78</v>
+      </c>
+      <c r="F12" t="s">
+        <v>28</v>
+      </c>
+      <c r="G12" t="s">
+        <v>18</v>
+      </c>
+      <c r="H12" t="s">
+        <v>29</v>
+      </c>
+      <c r="I12" s="1">
+        <v>1E-3</v>
+      </c>
+      <c r="J12" t="s">
+        <v>79</v>
+      </c>
+      <c r="K12" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12">
+      <c r="A13" s="35" t="s">
+        <v>81</v>
+      </c>
+      <c r="B13" t="s">
+        <v>82</v>
+      </c>
+      <c r="C13" t="s">
+        <v>83</v>
+      </c>
+      <c r="D13" t="s">
         <v>84</v>
       </c>
-      <c r="L9" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12">
-      <c r="A10" s="36" t="s">
-        <v>217</v>
-      </c>
-      <c r="B10" t="s">
-        <v>216</v>
-      </c>
-      <c r="C10" t="s">
-        <v>219</v>
-      </c>
-      <c r="D10" t="s">
-        <v>214</v>
-      </c>
-      <c r="E10" t="s">
-        <v>215</v>
-      </c>
-      <c r="F10" t="s">
-        <v>17</v>
-      </c>
-      <c r="G10" t="s">
-        <v>7</v>
-      </c>
-      <c r="H10" t="s">
-        <v>178</v>
-      </c>
-      <c r="I10" s="1">
-        <v>8.9999999999999998E-4</v>
-      </c>
-      <c r="J10" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12">
-      <c r="A11" s="36" t="s">
-        <v>208</v>
-      </c>
-      <c r="B11" t="s">
-        <v>210</v>
-      </c>
-      <c r="C11" t="s">
-        <v>209</v>
-      </c>
-      <c r="D11" t="s">
-        <v>211</v>
-      </c>
-      <c r="E11" t="s">
-        <v>207</v>
-      </c>
-      <c r="F11" t="s">
-        <v>17</v>
-      </c>
-      <c r="G11" t="s">
-        <v>7</v>
-      </c>
-      <c r="H11" t="s">
-        <v>178</v>
-      </c>
-      <c r="I11" s="1">
-        <v>1E-3</v>
-      </c>
-      <c r="J11" t="s">
-        <v>212</v>
-      </c>
-      <c r="K11" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12">
-      <c r="A12" s="36" t="s">
-        <v>174</v>
-      </c>
-      <c r="B12" t="s">
-        <v>170</v>
-      </c>
-      <c r="C12" t="s">
-        <v>175</v>
-      </c>
-      <c r="D12" t="s">
-        <v>176</v>
-      </c>
-      <c r="E12" t="s">
-        <v>177</v>
-      </c>
-      <c r="F12" t="s">
-        <v>11</v>
-      </c>
-      <c r="G12" t="s">
-        <v>7</v>
-      </c>
-      <c r="H12" t="s">
-        <v>171</v>
-      </c>
-      <c r="I12" s="1">
-        <v>6.9999999999999999E-4</v>
-      </c>
-      <c r="J12" t="s">
-        <v>34</v>
-      </c>
-      <c r="K12" t="s">
+      <c r="E13" t="s">
         <v>85</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12">
-      <c r="A13" s="36" t="s">
-        <v>182</v>
-      </c>
-      <c r="B13" t="s">
-        <v>75</v>
-      </c>
-      <c r="C13" t="s">
-        <v>180</v>
-      </c>
-      <c r="D13" t="s">
-        <v>179</v>
-      </c>
-      <c r="E13" t="s">
-        <v>181</v>
       </c>
       <c r="F13" t="s">
         <v>17</v>
       </c>
       <c r="G13" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="H13" t="s">
-        <v>178</v>
+        <v>60</v>
       </c>
       <c r="I13" s="1">
-        <v>1.1999999999999999E-3</v>
+        <v>6.9999999999999999E-4</v>
       </c>
       <c r="J13" t="s">
-        <v>54</v>
+        <v>20</v>
       </c>
       <c r="K13" t="s">
         <v>86</v>
       </c>
-      <c r="L13" t="s">
-        <v>82</v>
+    </row>
+    <row r="14" spans="1:12">
+      <c r="A14" s="35" t="s">
+        <v>87</v>
+      </c>
+      <c r="B14" t="s">
+        <v>88</v>
+      </c>
+      <c r="C14" t="s">
+        <v>89</v>
+      </c>
+      <c r="D14" t="s">
+        <v>90</v>
+      </c>
+      <c r="E14" t="s">
+        <v>91</v>
+      </c>
+      <c r="F14" t="s">
+        <v>28</v>
+      </c>
+      <c r="G14" t="s">
+        <v>18</v>
+      </c>
+      <c r="H14" t="s">
+        <v>29</v>
+      </c>
+      <c r="I14" s="1">
+        <v>1.1999999999999999E-3</v>
+      </c>
+      <c r="J14" t="s">
+        <v>30</v>
+      </c>
+      <c r="K14" t="s">
+        <v>92</v>
+      </c>
+      <c r="L14" t="s">
+        <v>93</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A9" r:id="rId1" display="https://www.justetf.com/it/etf-profile.html?isin=IE00B3VTN290" xr:uid="{6AB80B8F-0CAF-4297-B9BB-D72ED9AFBF01}"/>
-    <hyperlink ref="A12" r:id="rId2" display="https://www.justetf.com/it/etf-profile.html?isin=IE00BGR7L912" xr:uid="{69029A56-B54E-49FD-A0F5-77171229A26E}"/>
-    <hyperlink ref="A13" r:id="rId3" display="https://www.justetf.com/it/etf-profile.html?isin=IE00B579F325" xr:uid="{42CB0A67-6EA5-4F8A-A191-29BAAE4A4956}"/>
+    <hyperlink ref="A10" r:id="rId1" display="https://www.justetf.com/it/etf-profile.html?isin=IE00B3VTN290" xr:uid="{6AB80B8F-0CAF-4297-B9BB-D72ED9AFBF01}"/>
+    <hyperlink ref="A13" r:id="rId2" display="https://www.justetf.com/it/etf-profile.html?isin=IE00BGR7L912" xr:uid="{69029A56-B54E-49FD-A0F5-77171229A26E}"/>
+    <hyperlink ref="A14" r:id="rId3" display="https://www.justetf.com/it/etf-profile.html?isin=IE00B579F325" xr:uid="{42CB0A67-6EA5-4F8A-A191-29BAAE4A4956}"/>
     <hyperlink ref="A4" r:id="rId4" display="https://www.justetf.com/it/etf-profile.html?isin=IE00BD1F4L37" xr:uid="{DF84D7C7-B8F6-477A-8C9A-D4997B54C865}"/>
     <hyperlink ref="A5" r:id="rId5" display="https://www.justetf.com/it/etf-profile.html?isin=IE00B8FHGS14" xr:uid="{47A684AB-EAC0-4609-B6F5-2C135D16A87D}"/>
-    <hyperlink ref="A11" r:id="rId6" display="https://finance.yahoo.com/quote/LEONIA.MI/" xr:uid="{C03B49D3-5D8D-4719-818C-85A9CCE78BAE}"/>
-    <hyperlink ref="A10" r:id="rId7" display="https://www.justetf.com/it/etf-profile.html?isin=IE00B0M62X26" xr:uid="{80E603FC-0B0D-4EAD-9D73-152F6C249FED}"/>
+    <hyperlink ref="A12" r:id="rId6" display="https://finance.yahoo.com/quote/LEONIA.MI/" xr:uid="{C03B49D3-5D8D-4719-818C-85A9CCE78BAE}"/>
+    <hyperlink ref="A11" r:id="rId7" display="https://www.justetf.com/it/etf-profile.html?isin=IE00B0M62X26" xr:uid="{80E603FC-0B0D-4EAD-9D73-152F6C249FED}"/>
     <hyperlink ref="A2" r:id="rId8" display="https://www.justetf.com/it/etf-profile.html?isin=IE00B4L5Y983" xr:uid="{07C799E5-4B70-419F-8A83-D91DFAD88307}"/>
     <hyperlink ref="A3" r:id="rId9" display="https://www.justetf.com/it/etf-profile.html?isin=IE00BP3QZ825" xr:uid="{ED793FF2-3042-4018-9FA6-08360F193E0B}"/>
-    <hyperlink ref="A6" r:id="rId10" display="https://www.justetf.com/it/etf-profile.html?isin=IE00BM67HN09" xr:uid="{2EEFD69B-BBC2-44B7-BDD8-699CB046D272}"/>
-    <hyperlink ref="A7" r:id="rId11" display="https://www.justetf.com/it/etf-profile.html?isin=IE00BF4RFH31" xr:uid="{04A5FBD1-1EA4-45D6-A88A-DC1C0D39B403}"/>
-    <hyperlink ref="A8" r:id="rId12" display="https://www.justetf.com/it/etf-profile.html?isin=IE0032523478" xr:uid="{408B8EA9-ABA3-409D-8344-122D3BE0F3B9}"/>
+    <hyperlink ref="A7" r:id="rId10" display="https://www.justetf.com/it/etf-profile.html?isin=IE00BM67HN09" xr:uid="{2EEFD69B-BBC2-44B7-BDD8-699CB046D272}"/>
+    <hyperlink ref="A8" r:id="rId11" display="https://www.justetf.com/it/etf-profile.html?isin=IE00BF4RFH31" xr:uid="{04A5FBD1-1EA4-45D6-A88A-DC1C0D39B403}"/>
+    <hyperlink ref="A9" r:id="rId12" display="https://www.justetf.com/it/etf-profile.html?isin=IE0032523478" xr:uid="{408B8EA9-ABA3-409D-8344-122D3BE0F3B9}"/>
+    <hyperlink ref="A6" r:id="rId13" xr:uid="{62F5217A-B11D-43D5-9707-F13957F40612}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2748,402 +2792,402 @@
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.45"/>
   <cols>
-    <col min="1" max="1" width="31.9453125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="55.41796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.41796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.41796875" customWidth="1"/>
-    <col min="5" max="5" width="11.9453125" customWidth="1"/>
-    <col min="6" max="6" width="17.41796875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.7890625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.7890625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="21.7890625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="32" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="55.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.42578125" customWidth="1"/>
+    <col min="5" max="5" width="12" customWidth="1"/>
+    <col min="6" max="6" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="21.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" s="2" t="s">
-        <v>162</v>
+        <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>19</v>
+        <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="F1" s="2" t="s">
+      <c r="H1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="G1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>83</v>
-      </c>
       <c r="L1" s="2" t="s">
-        <v>44</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:12">
-      <c r="A2" s="36" t="s">
-        <v>165</v>
+      <c r="A2" s="35" t="s">
+        <v>23</v>
       </c>
       <c r="B2" t="s">
-        <v>196</v>
+        <v>24</v>
       </c>
       <c r="C2" t="s">
-        <v>154</v>
+        <v>25</v>
       </c>
       <c r="D2" t="s">
-        <v>155</v>
+        <v>26</v>
       </c>
       <c r="E2" t="s">
-        <v>161</v>
+        <v>27</v>
       </c>
       <c r="F2" t="s">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="G2" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="H2" t="s">
-        <v>178</v>
+        <v>29</v>
       </c>
       <c r="I2" s="1">
         <v>2.5000000000000001E-3</v>
       </c>
       <c r="J2" t="s">
-        <v>54</v>
+        <v>30</v>
       </c>
       <c r="K2" t="s">
-        <v>151</v>
+        <v>21</v>
       </c>
       <c r="L2" t="s">
-        <v>152</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:12">
       <c r="B3" t="s">
-        <v>78</v>
+        <v>94</v>
       </c>
       <c r="C3" t="s">
-        <v>81</v>
+        <v>95</v>
       </c>
       <c r="D3" t="s">
-        <v>79</v>
+        <v>96</v>
       </c>
       <c r="E3" t="s">
-        <v>80</v>
+        <v>97</v>
       </c>
       <c r="F3" t="s">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="G3" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="H3" t="s">
-        <v>32</v>
+        <v>19</v>
       </c>
       <c r="I3" s="1">
         <v>1.5E-3</v>
       </c>
       <c r="J3" t="s">
-        <v>35</v>
+        <v>98</v>
       </c>
       <c r="K3" t="s">
-        <v>151</v>
+        <v>21</v>
       </c>
       <c r="L3" t="s">
-        <v>152</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:12">
       <c r="B4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" t="s">
         <v>14</v>
       </c>
-      <c r="C4" t="s">
-        <v>0</v>
-      </c>
       <c r="D4" t="s">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="E4" t="s">
-        <v>59</v>
+        <v>16</v>
       </c>
       <c r="F4" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="G4" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="H4" t="s">
-        <v>32</v>
+        <v>19</v>
       </c>
       <c r="I4" s="1">
         <v>2E-3</v>
       </c>
       <c r="J4" t="s">
-        <v>34</v>
+        <v>20</v>
       </c>
       <c r="K4" t="s">
-        <v>151</v>
+        <v>21</v>
       </c>
       <c r="L4" t="s">
-        <v>152</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:12">
       <c r="B5" t="s">
-        <v>13</v>
+        <v>99</v>
       </c>
       <c r="C5" t="s">
-        <v>9</v>
+        <v>100</v>
       </c>
       <c r="D5" t="s">
-        <v>12</v>
+        <v>101</v>
       </c>
       <c r="E5" t="s">
-        <v>60</v>
+        <v>102</v>
       </c>
       <c r="F5" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="G5" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="H5" t="s">
-        <v>32</v>
+        <v>19</v>
       </c>
       <c r="I5" s="1">
         <v>2E-3</v>
       </c>
       <c r="J5" t="s">
-        <v>35</v>
+        <v>98</v>
       </c>
       <c r="K5" t="s">
-        <v>151</v>
+        <v>21</v>
       </c>
       <c r="L5" t="s">
-        <v>152</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:12">
       <c r="B6" t="s">
+        <v>103</v>
+      </c>
+      <c r="C6" t="s">
+        <v>104</v>
+      </c>
+      <c r="D6" t="s">
+        <v>105</v>
+      </c>
+      <c r="E6" t="s">
+        <v>106</v>
+      </c>
+      <c r="F6" t="s">
+        <v>28</v>
+      </c>
+      <c r="G6" t="s">
         <v>18</v>
       </c>
-      <c r="C6" t="s">
-        <v>15</v>
-      </c>
-      <c r="D6" t="s">
-        <v>16</v>
-      </c>
-      <c r="E6" t="s">
-        <v>57</v>
-      </c>
-      <c r="F6" t="s">
-        <v>17</v>
-      </c>
-      <c r="G6" t="s">
-        <v>7</v>
-      </c>
       <c r="H6" t="s">
-        <v>32</v>
+        <v>19</v>
       </c>
       <c r="I6" s="1">
         <v>1.5E-3</v>
       </c>
       <c r="J6" t="s">
-        <v>34</v>
+        <v>20</v>
       </c>
       <c r="K6" t="s">
-        <v>84</v>
+        <v>67</v>
       </c>
       <c r="L6" t="s">
-        <v>88</v>
+        <v>68</v>
       </c>
     </row>
     <row r="7" spans="1:12">
       <c r="B7" t="s">
-        <v>21</v>
+        <v>107</v>
       </c>
       <c r="C7" t="s">
-        <v>23</v>
+        <v>108</v>
       </c>
       <c r="D7" t="s">
-        <v>22</v>
+        <v>109</v>
       </c>
       <c r="E7" t="s">
-        <v>63</v>
+        <v>110</v>
       </c>
       <c r="F7" t="s">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="G7" t="s">
-        <v>31</v>
+        <v>111</v>
       </c>
       <c r="H7" t="s">
-        <v>32</v>
+        <v>19</v>
       </c>
       <c r="I7" s="1">
         <v>1E-3</v>
       </c>
       <c r="J7" t="s">
-        <v>34</v>
+        <v>20</v>
       </c>
       <c r="K7" t="s">
-        <v>84</v>
+        <v>67</v>
       </c>
     </row>
     <row r="8" spans="1:12">
       <c r="B8" t="s">
-        <v>50</v>
+        <v>112</v>
       </c>
       <c r="C8" t="s">
-        <v>49</v>
+        <v>113</v>
       </c>
       <c r="D8" t="s">
-        <v>51</v>
+        <v>114</v>
       </c>
       <c r="E8" t="s">
-        <v>58</v>
+        <v>115</v>
       </c>
       <c r="F8" t="s">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="G8" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="H8" t="s">
-        <v>32</v>
+        <v>19</v>
       </c>
       <c r="I8" s="1">
         <v>8.9999999999999998E-4</v>
       </c>
       <c r="J8" t="s">
-        <v>34</v>
+        <v>20</v>
       </c>
       <c r="K8" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="L8" t="s">
-        <v>87</v>
+        <v>116</v>
       </c>
     </row>
     <row r="9" spans="1:12">
       <c r="B9" t="s">
-        <v>53</v>
+        <v>117</v>
       </c>
       <c r="C9" t="s">
-        <v>71</v>
+        <v>118</v>
       </c>
       <c r="D9" t="s">
-        <v>69</v>
+        <v>119</v>
       </c>
       <c r="E9" t="s">
-        <v>70</v>
+        <v>120</v>
       </c>
       <c r="F9" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="G9" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="H9" t="s">
-        <v>32</v>
+        <v>19</v>
       </c>
       <c r="I9" s="1">
         <v>6.9999999999999999E-4</v>
       </c>
       <c r="J9" t="s">
-        <v>34</v>
+        <v>20</v>
       </c>
       <c r="K9" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="10" spans="1:12">
       <c r="B10" t="s">
-        <v>91</v>
+        <v>121</v>
       </c>
       <c r="C10" t="s">
-        <v>90</v>
+        <v>122</v>
       </c>
       <c r="D10" t="s">
-        <v>92</v>
+        <v>123</v>
       </c>
       <c r="E10" t="s">
-        <v>94</v>
+        <v>124</v>
       </c>
       <c r="F10" t="s">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="G10" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="H10" t="s">
-        <v>32</v>
+        <v>19</v>
       </c>
       <c r="I10" s="1">
         <v>1.5E-3</v>
       </c>
       <c r="J10" t="s">
-        <v>34</v>
+        <v>20</v>
       </c>
       <c r="K10" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="L10" t="s">
-        <v>95</v>
+        <v>125</v>
       </c>
     </row>
     <row r="11" spans="1:12">
       <c r="B11" t="s">
-        <v>75</v>
+        <v>88</v>
       </c>
       <c r="C11" t="s">
-        <v>77</v>
+        <v>126</v>
       </c>
       <c r="D11" t="s">
-        <v>93</v>
+        <v>127</v>
       </c>
       <c r="E11" t="s">
-        <v>76</v>
+        <v>128</v>
       </c>
       <c r="F11" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="G11" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="H11" t="s">
-        <v>32</v>
+        <v>19</v>
       </c>
       <c r="I11" s="1">
         <v>1.1999999999999999E-3</v>
       </c>
       <c r="J11" t="s">
-        <v>54</v>
+        <v>30</v>
       </c>
       <c r="K11" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="L11" t="s">
-        <v>82</v>
+        <v>93</v>
       </c>
     </row>
     <row r="12" spans="1:12">
@@ -3165,472 +3209,472 @@
       <selection activeCell="A13" sqref="A13:J15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.45"/>
   <cols>
-    <col min="2" max="2" width="37.68359375" customWidth="1"/>
-    <col min="3" max="3" width="52.7890625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="37.7109375" customWidth="1"/>
+    <col min="3" max="3" width="52.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
       <c r="B1" s="2" t="s">
-        <v>19</v>
+        <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="F1" s="2" t="s">
+      <c r="H1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="G1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>83</v>
-      </c>
       <c r="L1" s="2" t="s">
-        <v>44</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:12">
       <c r="B2" t="s">
-        <v>52</v>
+        <v>129</v>
       </c>
       <c r="C2" t="s">
-        <v>74</v>
+        <v>130</v>
       </c>
       <c r="D2" t="s">
-        <v>73</v>
+        <v>131</v>
       </c>
       <c r="E2" t="s">
-        <v>72</v>
+        <v>132</v>
       </c>
       <c r="F2" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="G2" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="H2" t="s">
-        <v>32</v>
+        <v>19</v>
       </c>
       <c r="I2" s="1">
         <v>6.9999999999999999E-4</v>
       </c>
       <c r="J2" t="s">
-        <v>54</v>
+        <v>30</v>
       </c>
       <c r="L2" t="s">
-        <v>55</v>
+        <v>133</v>
       </c>
     </row>
     <row r="3" spans="1:12">
       <c r="B3" t="s">
-        <v>41</v>
+        <v>134</v>
       </c>
       <c r="C3" t="s">
-        <v>42</v>
+        <v>135</v>
       </c>
       <c r="D3" t="s">
-        <v>43</v>
+        <v>136</v>
       </c>
       <c r="E3" t="s">
-        <v>66</v>
+        <v>137</v>
       </c>
       <c r="F3" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="G3" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="H3" t="s">
-        <v>33</v>
+        <v>138</v>
       </c>
       <c r="I3" s="1">
         <v>2E-3</v>
       </c>
       <c r="J3" t="s">
-        <v>34</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:12">
       <c r="B4" t="s">
-        <v>47</v>
+        <v>139</v>
       </c>
       <c r="C4" t="s">
-        <v>46</v>
+        <v>140</v>
       </c>
       <c r="D4" t="s">
-        <v>48</v>
+        <v>141</v>
       </c>
       <c r="E4" t="s">
-        <v>67</v>
+        <v>142</v>
       </c>
       <c r="F4" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="G4" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="H4" t="s">
-        <v>32</v>
+        <v>19</v>
       </c>
       <c r="I4" s="1">
         <v>1E-3</v>
       </c>
       <c r="J4" t="s">
-        <v>34</v>
+        <v>20</v>
       </c>
       <c r="L4" t="s">
-        <v>45</v>
+        <v>143</v>
       </c>
     </row>
     <row r="5" spans="1:12">
       <c r="B5" t="s">
-        <v>24</v>
+        <v>144</v>
       </c>
       <c r="C5" t="s">
-        <v>27</v>
+        <v>145</v>
       </c>
       <c r="D5" t="s">
+        <v>146</v>
+      </c>
+      <c r="E5" t="s">
+        <v>147</v>
+      </c>
+      <c r="F5" t="s">
         <v>28</v>
       </c>
-      <c r="E5" t="s">
-        <v>61</v>
-      </c>
-      <c r="F5" t="s">
-        <v>17</v>
-      </c>
       <c r="G5" t="s">
-        <v>31</v>
+        <v>111</v>
       </c>
       <c r="H5" t="s">
-        <v>33</v>
+        <v>138</v>
       </c>
       <c r="I5" s="1">
         <v>2.5000000000000001E-3</v>
       </c>
       <c r="J5" t="s">
-        <v>34</v>
+        <v>20</v>
       </c>
       <c r="K5" t="s">
-        <v>84</v>
+        <v>67</v>
       </c>
     </row>
     <row r="6" spans="1:12">
       <c r="B6" t="s">
-        <v>20</v>
+        <v>148</v>
       </c>
       <c r="C6" t="s">
-        <v>25</v>
+        <v>149</v>
       </c>
       <c r="D6" t="s">
-        <v>26</v>
+        <v>150</v>
       </c>
       <c r="E6" t="s">
-        <v>68</v>
+        <v>151</v>
       </c>
       <c r="F6" t="s">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="G6" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="H6" t="s">
-        <v>33</v>
+        <v>138</v>
       </c>
       <c r="I6" s="1">
         <v>1.5E-3</v>
       </c>
       <c r="J6" t="s">
-        <v>34</v>
+        <v>20</v>
       </c>
       <c r="K6" t="s">
-        <v>84</v>
+        <v>67</v>
       </c>
     </row>
     <row r="7" spans="1:12">
       <c r="B7" t="s">
-        <v>39</v>
+        <v>152</v>
       </c>
       <c r="C7" t="s">
-        <v>38</v>
+        <v>153</v>
       </c>
       <c r="D7" t="s">
-        <v>40</v>
+        <v>154</v>
       </c>
       <c r="E7" t="s">
-        <v>65</v>
+        <v>155</v>
       </c>
       <c r="F7" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="G7" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="H7" t="s">
-        <v>32</v>
+        <v>19</v>
       </c>
       <c r="I7" s="1">
         <v>8.9999999999999998E-4</v>
       </c>
       <c r="J7" t="s">
-        <v>34</v>
+        <v>20</v>
       </c>
       <c r="L7" t="s">
-        <v>89</v>
+        <v>156</v>
       </c>
     </row>
     <row r="8" spans="1:12">
       <c r="C8" t="s">
-        <v>29</v>
+        <v>157</v>
       </c>
       <c r="D8" t="s">
-        <v>30</v>
+        <v>158</v>
       </c>
       <c r="E8" t="s">
-        <v>62</v>
+        <v>159</v>
       </c>
       <c r="F8" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="G8" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="H8" t="s">
-        <v>32</v>
+        <v>19</v>
       </c>
       <c r="I8" s="1">
         <v>2E-3</v>
       </c>
       <c r="J8" t="s">
-        <v>34</v>
+        <v>20</v>
       </c>
       <c r="K8" t="s">
-        <v>84</v>
+        <v>67</v>
       </c>
     </row>
     <row r="9" spans="1:12">
       <c r="C9" t="s">
-        <v>36</v>
+        <v>160</v>
       </c>
       <c r="D9" t="s">
-        <v>37</v>
+        <v>161</v>
       </c>
       <c r="E9" t="s">
-        <v>64</v>
+        <v>162</v>
       </c>
       <c r="F9" t="s">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="G9" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="H9" t="s">
-        <v>32</v>
+        <v>19</v>
       </c>
       <c r="I9" s="1">
         <v>8.9999999999999998E-4</v>
       </c>
       <c r="J9" t="s">
-        <v>34</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:12">
       <c r="B10" t="s">
-        <v>191</v>
+        <v>163</v>
       </c>
       <c r="C10" t="s">
-        <v>185</v>
+        <v>164</v>
       </c>
       <c r="D10" t="s">
-        <v>184</v>
+        <v>165</v>
       </c>
       <c r="E10" t="s">
-        <v>186</v>
+        <v>166</v>
       </c>
       <c r="F10" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="G10" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="H10" t="s">
-        <v>32</v>
+        <v>19</v>
       </c>
       <c r="I10" s="1">
         <v>2.5000000000000001E-3</v>
       </c>
       <c r="J10" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" ht="14.7" customHeight="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="14.65" customHeight="1">
       <c r="B11" t="s">
-        <v>190</v>
-      </c>
-      <c r="C11" s="37" t="s">
-        <v>187</v>
+        <v>167</v>
+      </c>
+      <c r="C11" s="36" t="s">
+        <v>38</v>
       </c>
       <c r="D11" t="s">
-        <v>188</v>
+        <v>39</v>
       </c>
       <c r="E11" t="s">
-        <v>189</v>
+        <v>40</v>
       </c>
       <c r="F11" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="G11" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="H11" t="s">
-        <v>32</v>
+        <v>19</v>
       </c>
       <c r="I11" s="1">
         <v>3.0000000000000001E-3</v>
       </c>
       <c r="J11" t="s">
-        <v>34</v>
+        <v>20</v>
       </c>
     </row>
     <row r="12" spans="1:12">
       <c r="B12" t="s">
-        <v>192</v>
+        <v>168</v>
       </c>
       <c r="C12" t="s">
-        <v>195</v>
+        <v>33</v>
       </c>
       <c r="D12" t="s">
-        <v>193</v>
+        <v>34</v>
       </c>
       <c r="E12" t="s">
-        <v>194</v>
+        <v>35</v>
       </c>
       <c r="F12" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="G12" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="H12" t="s">
-        <v>32</v>
+        <v>19</v>
       </c>
       <c r="I12" s="1">
         <v>2E-3</v>
       </c>
       <c r="J12" t="s">
-        <v>54</v>
+        <v>30</v>
       </c>
     </row>
     <row r="13" spans="1:12">
-      <c r="A13" s="36" t="s">
-        <v>164</v>
+      <c r="A13" s="35" t="s">
+        <v>46</v>
       </c>
       <c r="B13" t="s">
-        <v>163</v>
+        <v>47</v>
       </c>
       <c r="C13" t="s">
-        <v>158</v>
+        <v>48</v>
       </c>
       <c r="D13" t="s">
-        <v>159</v>
+        <v>169</v>
       </c>
       <c r="E13" t="s">
-        <v>160</v>
+        <v>49</v>
       </c>
       <c r="F13" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="G13" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="H13" t="s">
-        <v>178</v>
+        <v>29</v>
       </c>
       <c r="I13" s="1">
         <v>2.5000000000000001E-3</v>
       </c>
       <c r="J13" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12">
+      <c r="A14" s="35" t="s">
+        <v>50</v>
+      </c>
+      <c r="B14" t="s">
+        <v>51</v>
+      </c>
+      <c r="C14" t="s">
+        <v>52</v>
+      </c>
+      <c r="D14" t="s">
+        <v>53</v>
+      </c>
+      <c r="E14" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="14" spans="1:12">
-      <c r="A14" s="36" t="s">
-        <v>166</v>
-      </c>
-      <c r="B14" t="s">
-        <v>153</v>
-      </c>
-      <c r="C14" t="s">
-        <v>156</v>
-      </c>
-      <c r="D14" t="s">
-        <v>183</v>
-      </c>
-      <c r="E14" t="s">
-        <v>157</v>
-      </c>
       <c r="F14" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="G14" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="H14" t="s">
-        <v>178</v>
+        <v>29</v>
       </c>
       <c r="I14" s="1">
         <v>3.5000000000000001E-3</v>
       </c>
       <c r="J14" t="s">
-        <v>34</v>
+        <v>20</v>
       </c>
     </row>
     <row r="15" spans="1:12">
-      <c r="A15" s="36" t="s">
-        <v>203</v>
+      <c r="A15" s="35" t="s">
+        <v>55</v>
       </c>
       <c r="B15" t="s">
-        <v>205</v>
+        <v>56</v>
       </c>
       <c r="C15" t="s">
-        <v>204</v>
+        <v>57</v>
       </c>
       <c r="D15" t="s">
-        <v>206</v>
+        <v>58</v>
       </c>
       <c r="E15" t="s">
-        <v>201</v>
+        <v>59</v>
       </c>
       <c r="F15" t="s">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="G15" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="H15" t="s">
-        <v>171</v>
+        <v>60</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>202</v>
+        <v>61</v>
       </c>
       <c r="J15" t="s">
-        <v>34</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -3645,19 +3689,19 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{939D994C-0E7B-435F-BB4C-7162BD8072E3}">
-  <dimension ref="A1:B13"/>
+  <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.45"/>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="str" cm="1">
-        <f t="array" ref="A1:A13">overview!E1:E13</f>
+        <f t="array" ref="A1:A14">overview!E1:E14</f>
         <v>Ticker</v>
       </c>
       <c r="B1" t="str" cm="1">
-        <f t="array" ref="B1:B13">overview!B1:B13</f>
+        <f t="array" ref="B1:B14">overview!B1:B14</f>
         <v>Index</v>
       </c>
     </row>
@@ -3695,65 +3739,73 @@
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="str">
-        <v>XDWS.L</v>
+        <v>XDWH.MI</v>
       </c>
       <c r="B6" t="str">
-        <v>Consumer Staples Global</v>
+        <v>World Health Care</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="str">
-        <v>WSML.L</v>
+        <v>XDWS.L</v>
       </c>
       <c r="B7" t="str">
-        <v>Small Cap Global</v>
+        <v>Consumer Staples Global</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="str">
-        <v>IBCX.AS</v>
+        <v>WSML.L</v>
       </c>
       <c r="B8" t="str">
-        <v>EU Corp Large Cap bonds</v>
+        <v>Small Cap Global</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="str">
-        <v>IBGM.AS</v>
+        <v>IBCX.AS</v>
       </c>
       <c r="B9" t="str">
-        <v>EU Gov bonds 7-10y</v>
+        <v>EU Corp Large Cap bonds</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="str">
-        <v>IBCI.AS</v>
+        <v>IBGM.AS</v>
       </c>
       <c r="B10" t="str">
-        <v>EU Inflation-Linked</v>
+        <v>EU Gov bonds 7-10y</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="str">
-        <v>LEONIA.MI</v>
+        <v>IBCI.AS</v>
       </c>
       <c r="B11" t="str">
-        <v>EU Overnight</v>
+        <v>EU Inflation-Linked</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" t="str">
-        <v>IBTU.L</v>
+        <v>LEONIA.MI</v>
       </c>
       <c r="B12" t="str">
-        <v>US Short Treasury</v>
+        <v>EU Overnight</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" t="str">
+        <v>IBTU.L</v>
+      </c>
+      <c r="B13" t="str">
+        <v>US Short Treasury</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" t="str">
         <v>SGLD.AS</v>
       </c>
-      <c r="B13" t="str">
+      <c r="B14" t="str">
         <v>ETC GOLD</v>
       </c>
     </row>
@@ -3764,17 +3816,17 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA57C457-A80C-477F-8A3E-0F8DB96F6511}">
-  <dimension ref="A1:A13"/>
+  <dimension ref="A1:A14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.45"/>
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="str" cm="1">
-        <f t="array" ref="A1:A13">overview!C1:C13</f>
+        <f t="array" ref="A1:A14">overview!C1:C14</f>
         <v>Name</v>
       </c>
     </row>
@@ -3800,41 +3852,46 @@
     </row>
     <row r="6" spans="1:1">
       <c r="A6" t="str">
-        <v>Xtrackers MSCI World Consumer Staples UCITS ETF (Acc)</v>
+        <v>Xtrackers MSCI World Health Care UCITS ETF 1C</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" t="str">
-        <v>iShares MSCI World Small Cap UCITS ETF</v>
+        <v>Xtrackers MSCI World Consumer Staples UCITS ETF (Acc)</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8" t="str">
-        <v>iShares Euro Corporate Bond Large Cap UCITS ETF</v>
+        <v>iShares MSCI World Small Cap UCITS ETF</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9" t="str">
-        <v>iShares € Govt Bond 7-10yr UCITS ETF EUR (Dist)</v>
+        <v>iShares Euro Corporate Bond Large Cap UCITS ETF</v>
       </c>
     </row>
     <row r="10" spans="1:1">
       <c r="A10" t="str">
-        <v>iShares € Inflation Linked Govt Bond UCITS ETF EUR (Acc)</v>
+        <v>iShares € Govt Bond 7-10yr UCITS ETF EUR (Dist)</v>
       </c>
     </row>
     <row r="11" spans="1:1">
       <c r="A11" t="str">
-        <v>Amundi EUR Overnight Return UCITS ETF Acc</v>
+        <v>iShares € Inflation Linked Govt Bond UCITS ETF EUR (Acc)</v>
       </c>
     </row>
     <row r="12" spans="1:1">
       <c r="A12" t="str">
-        <v>iShares USD Treasury Bond 0-1yr UCITS ETF (Dist)</v>
+        <v>Amundi EUR Overnight Return UCITS ETF Acc</v>
       </c>
     </row>
     <row r="13" spans="1:1">
       <c r="A13" t="str">
+        <v>iShares USD Treasury Bond 0-1yr UCITS ETF (Dist)</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1">
+      <c r="A14" t="str">
         <v>Invesco Physical Gold ETC</v>
       </c>
     </row>
@@ -3851,214 +3908,214 @@
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.45"/>
   <cols>
-    <col min="1" max="1" width="87.83984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="87.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
-      <c r="A1" s="36" t="s">
-        <v>167</v>
+      <c r="A1" s="35" t="s">
+        <v>62</v>
       </c>
       <c r="B1" t="s">
-        <v>169</v>
+        <v>63</v>
       </c>
       <c r="C1" t="s">
-        <v>173</v>
+        <v>64</v>
       </c>
       <c r="D1" t="s">
-        <v>168</v>
+        <v>65</v>
       </c>
       <c r="E1" t="s">
-        <v>172</v>
+        <v>66</v>
       </c>
       <c r="F1" t="s">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="G1" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="H1" t="s">
-        <v>171</v>
+        <v>60</v>
       </c>
       <c r="I1" s="1">
         <v>1.5E-3</v>
       </c>
       <c r="J1" t="s">
-        <v>34</v>
+        <v>20</v>
       </c>
       <c r="K1" t="s">
-        <v>84</v>
+        <v>67</v>
       </c>
       <c r="L1" t="s">
-        <v>88</v>
+        <v>68</v>
       </c>
     </row>
     <row r="2" spans="1:12">
-      <c r="A2" s="36" t="s">
-        <v>203</v>
+      <c r="A2" s="35" t="s">
+        <v>55</v>
       </c>
       <c r="B2" t="s">
-        <v>205</v>
+        <v>56</v>
       </c>
       <c r="C2" t="s">
-        <v>204</v>
+        <v>57</v>
       </c>
       <c r="D2" t="s">
-        <v>206</v>
+        <v>58</v>
       </c>
       <c r="E2" t="s">
-        <v>201</v>
+        <v>59</v>
       </c>
       <c r="F2" t="s">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="G2" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="H2" t="s">
-        <v>171</v>
+        <v>60</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>202</v>
+        <v>61</v>
       </c>
       <c r="J2" t="s">
-        <v>34</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:12">
-      <c r="A3" s="36" t="s">
-        <v>217</v>
+      <c r="A3" s="35" t="s">
+        <v>69</v>
       </c>
       <c r="B3" t="s">
-        <v>216</v>
+        <v>70</v>
       </c>
       <c r="C3" t="s">
-        <v>219</v>
+        <v>71</v>
       </c>
       <c r="D3" t="s">
-        <v>214</v>
+        <v>72</v>
       </c>
       <c r="E3" t="s">
-        <v>215</v>
+        <v>73</v>
       </c>
       <c r="F3" t="s">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="G3" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="H3" t="s">
-        <v>178</v>
+        <v>29</v>
       </c>
       <c r="I3" s="1">
         <v>8.9999999999999998E-4</v>
       </c>
       <c r="J3" t="s">
-        <v>34</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:12">
-      <c r="A4" s="36" t="s">
-        <v>220</v>
+      <c r="A4" s="35" t="s">
+        <v>170</v>
       </c>
       <c r="B4" t="s">
-        <v>221</v>
+        <v>171</v>
       </c>
       <c r="C4" t="s">
-        <v>222</v>
+        <v>172</v>
       </c>
       <c r="D4" t="s">
-        <v>218</v>
+        <v>173</v>
       </c>
       <c r="E4" t="s">
-        <v>223</v>
+        <v>174</v>
       </c>
       <c r="F4" t="s">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="G4" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="H4" t="s">
-        <v>178</v>
+        <v>29</v>
       </c>
       <c r="I4" s="1">
         <v>2.5000000000000001E-3</v>
       </c>
       <c r="J4" t="s">
-        <v>224</v>
+        <v>175</v>
       </c>
     </row>
     <row r="5" spans="1:12">
-      <c r="A5" s="36" t="s">
-        <v>208</v>
+      <c r="A5" s="35" t="s">
+        <v>74</v>
       </c>
       <c r="B5" t="s">
-        <v>210</v>
+        <v>75</v>
       </c>
       <c r="C5" t="s">
-        <v>209</v>
+        <v>76</v>
       </c>
       <c r="D5" t="s">
-        <v>211</v>
+        <v>77</v>
       </c>
       <c r="E5" t="s">
-        <v>207</v>
+        <v>78</v>
       </c>
       <c r="F5" t="s">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="G5" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="H5" t="s">
-        <v>178</v>
+        <v>29</v>
       </c>
       <c r="I5" s="1">
         <v>1E-3</v>
       </c>
       <c r="J5" t="s">
-        <v>212</v>
+        <v>79</v>
       </c>
       <c r="K5" t="s">
-        <v>213</v>
+        <v>80</v>
       </c>
     </row>
     <row r="6" spans="1:12">
-      <c r="A6" s="36" t="s">
-        <v>174</v>
+      <c r="A6" s="35" t="s">
+        <v>81</v>
       </c>
       <c r="B6" t="s">
-        <v>170</v>
+        <v>82</v>
       </c>
       <c r="C6" t="s">
-        <v>175</v>
+        <v>83</v>
       </c>
       <c r="D6" t="s">
-        <v>176</v>
+        <v>84</v>
       </c>
       <c r="E6" t="s">
-        <v>177</v>
+        <v>85</v>
       </c>
       <c r="F6" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="G6" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="H6" t="s">
-        <v>171</v>
+        <v>60</v>
       </c>
       <c r="I6" s="1">
         <v>6.9999999999999999E-4</v>
       </c>
       <c r="J6" t="s">
-        <v>34</v>
+        <v>20</v>
       </c>
       <c r="K6" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
   </sheetData>
@@ -4082,34 +4139,34 @@
       <selection activeCell="W12" sqref="W12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.578125" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="14.45"/>
   <sheetData>
-    <row r="1" spans="1:18" ht="25.2">
+    <row r="1" spans="1:18" ht="25.15">
       <c r="A1" s="4" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="2" spans="1:18" ht="25.2">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" ht="25.15">
       <c r="A2" s="4"/>
     </row>
-    <row r="3" spans="1:18" ht="14.7" thickBot="1"/>
-    <row r="4" spans="1:18" ht="16" customHeight="1">
+    <row r="3" spans="1:18" ht="14.65" thickBot="1"/>
+    <row r="4" spans="1:18" ht="15.95" customHeight="1">
       <c r="B4" s="38" t="s">
-        <v>97</v>
+        <v>177</v>
       </c>
       <c r="C4" s="39"/>
       <c r="D4" s="39"/>
       <c r="E4" s="39"/>
       <c r="F4" s="40"/>
       <c r="H4" s="44" t="s">
-        <v>98</v>
+        <v>178</v>
       </c>
       <c r="I4" s="45"/>
       <c r="J4" s="45"/>
       <c r="K4" s="45"/>
       <c r="L4" s="46"/>
       <c r="N4" s="50" t="s">
-        <v>99</v>
+        <v>179</v>
       </c>
       <c r="O4" s="51"/>
       <c r="P4" s="51"/>
@@ -4135,21 +4192,21 @@
     </row>
     <row r="6" spans="1:18">
       <c r="B6" s="56" t="s">
-        <v>100</v>
+        <v>180</v>
       </c>
       <c r="C6" s="57"/>
       <c r="D6" s="57"/>
       <c r="E6" s="57"/>
       <c r="F6" s="58"/>
       <c r="H6" s="56" t="s">
-        <v>101</v>
+        <v>181</v>
       </c>
       <c r="I6" s="57"/>
       <c r="J6" s="57"/>
       <c r="K6" s="57"/>
       <c r="L6" s="58"/>
       <c r="N6" s="56" t="s">
-        <v>101</v>
+        <v>181</v>
       </c>
       <c r="O6" s="57"/>
       <c r="P6" s="57"/>
@@ -4208,47 +4265,47 @@
       <c r="R9" s="64"/>
     </row>
     <row r="10" spans="1:18">
-      <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
-      <c r="H10" s="5"/>
-      <c r="I10" s="5"/>
-      <c r="J10" s="5"/>
-      <c r="K10" s="5"/>
-      <c r="L10" s="5"/>
-      <c r="N10" s="5"/>
-      <c r="O10" s="5"/>
-      <c r="P10" s="5"/>
-      <c r="Q10" s="5"/>
-      <c r="R10" s="5"/>
-    </row>
-    <row r="11" spans="1:18" ht="14.7" thickBot="1"/>
-    <row r="12" spans="1:18" ht="16" customHeight="1">
+      <c r="B10" s="37"/>
+      <c r="C10" s="37"/>
+      <c r="D10" s="37"/>
+      <c r="E10" s="37"/>
+      <c r="F10" s="37"/>
+      <c r="H10" s="37"/>
+      <c r="I10" s="37"/>
+      <c r="J10" s="37"/>
+      <c r="K10" s="37"/>
+      <c r="L10" s="37"/>
+      <c r="N10" s="37"/>
+      <c r="O10" s="37"/>
+      <c r="P10" s="37"/>
+      <c r="Q10" s="37"/>
+      <c r="R10" s="37"/>
+    </row>
+    <row r="11" spans="1:18" ht="14.65" thickBot="1"/>
+    <row r="12" spans="1:18" ht="15.95" customHeight="1">
       <c r="B12" s="38" t="s">
-        <v>102</v>
+        <v>182</v>
       </c>
       <c r="C12" s="39"/>
       <c r="D12" s="39"/>
       <c r="E12" s="39"/>
       <c r="F12" s="40"/>
       <c r="H12" s="65" t="s">
-        <v>102</v>
+        <v>182</v>
       </c>
       <c r="I12" s="66"/>
       <c r="J12" s="66"/>
       <c r="K12" s="66"/>
       <c r="L12" s="67"/>
       <c r="N12" s="71" t="s">
-        <v>102</v>
+        <v>182</v>
       </c>
       <c r="O12" s="72"/>
       <c r="P12" s="72"/>
       <c r="Q12" s="72"/>
       <c r="R12" s="73"/>
     </row>
-    <row r="13" spans="1:18" ht="16" customHeight="1">
+    <row r="13" spans="1:18" ht="15.95" customHeight="1">
       <c r="B13" s="41"/>
       <c r="C13" s="42"/>
       <c r="D13" s="42"/>
@@ -4265,23 +4322,23 @@
       <c r="Q13" s="75"/>
       <c r="R13" s="76"/>
     </row>
-    <row r="14" spans="1:18" ht="16" customHeight="1">
+    <row r="14" spans="1:18" ht="15.95" customHeight="1">
       <c r="B14" s="77" t="s">
-        <v>103</v>
+        <v>183</v>
       </c>
       <c r="C14" s="78"/>
       <c r="D14" s="78"/>
       <c r="E14" s="78"/>
       <c r="F14" s="79"/>
       <c r="H14" s="77" t="s">
-        <v>104</v>
+        <v>184</v>
       </c>
       <c r="I14" s="78"/>
       <c r="J14" s="78"/>
       <c r="K14" s="78"/>
       <c r="L14" s="79"/>
       <c r="N14" s="77" t="s">
-        <v>105</v>
+        <v>185</v>
       </c>
       <c r="O14" s="78"/>
       <c r="P14" s="78"/>
@@ -4356,23 +4413,23 @@
       <c r="Q18" s="84"/>
       <c r="R18" s="85"/>
     </row>
-    <row r="19" spans="2:18" ht="16" customHeight="1">
+    <row r="19" spans="2:18" ht="15.95" customHeight="1">
       <c r="B19" s="77" t="s">
-        <v>106</v>
+        <v>186</v>
       </c>
       <c r="C19" s="78"/>
       <c r="D19" s="78"/>
       <c r="E19" s="78"/>
       <c r="F19" s="79"/>
       <c r="H19" s="77" t="s">
-        <v>106</v>
+        <v>186</v>
       </c>
       <c r="I19" s="78"/>
       <c r="J19" s="78"/>
       <c r="K19" s="78"/>
       <c r="L19" s="79"/>
       <c r="N19" s="77" t="s">
-        <v>107</v>
+        <v>187</v>
       </c>
       <c r="O19" s="78"/>
       <c r="P19" s="78"/>
@@ -4447,193 +4504,193 @@
       <c r="Q23" s="84"/>
       <c r="R23" s="85"/>
     </row>
-    <row r="26" spans="2:18" ht="18.3">
-      <c r="B26" s="6" t="s">
-        <v>108</v>
-      </c>
-      <c r="C26" s="7"/>
-      <c r="D26" s="7"/>
-      <c r="E26" s="7"/>
-      <c r="F26" s="8"/>
-      <c r="H26" s="6" t="s">
-        <v>108</v>
-      </c>
-      <c r="I26" s="7"/>
-      <c r="J26" s="7"/>
-      <c r="K26" s="7"/>
-      <c r="L26" s="8"/>
-      <c r="N26" s="6" t="s">
-        <v>108</v>
-      </c>
-      <c r="O26" s="7"/>
-      <c r="P26" s="7"/>
-      <c r="Q26" s="7"/>
-      <c r="R26" s="8"/>
+    <row r="26" spans="2:18" ht="18.399999999999999">
+      <c r="B26" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="C26" s="6"/>
+      <c r="D26" s="6"/>
+      <c r="E26" s="6"/>
+      <c r="F26" s="7"/>
+      <c r="H26" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="I26" s="6"/>
+      <c r="J26" s="6"/>
+      <c r="K26" s="6"/>
+      <c r="L26" s="7"/>
+      <c r="N26" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="O26" s="6"/>
+      <c r="P26" s="6"/>
+      <c r="Q26" s="6"/>
+      <c r="R26" s="7"/>
     </row>
     <row r="27" spans="2:18">
-      <c r="B27" s="9"/>
-      <c r="C27" s="10"/>
-      <c r="D27" s="10"/>
-      <c r="E27" s="10"/>
-      <c r="F27" s="11"/>
-      <c r="H27" s="9"/>
-      <c r="I27" s="10"/>
-      <c r="J27" s="10"/>
-      <c r="K27" s="10"/>
-      <c r="L27" s="11"/>
-      <c r="N27" s="9"/>
-      <c r="O27" s="10"/>
-      <c r="P27" s="10"/>
-      <c r="Q27" s="10"/>
-      <c r="R27" s="11"/>
+      <c r="B27" s="8"/>
+      <c r="C27" s="9"/>
+      <c r="D27" s="9"/>
+      <c r="E27" s="9"/>
+      <c r="F27" s="10"/>
+      <c r="H27" s="8"/>
+      <c r="I27" s="9"/>
+      <c r="J27" s="9"/>
+      <c r="K27" s="9"/>
+      <c r="L27" s="10"/>
+      <c r="N27" s="8"/>
+      <c r="O27" s="9"/>
+      <c r="P27" s="9"/>
+      <c r="Q27" s="9"/>
+      <c r="R27" s="10"/>
     </row>
     <row r="28" spans="2:18">
-      <c r="B28" s="9" t="s">
-        <v>109</v>
-      </c>
-      <c r="C28" s="10"/>
-      <c r="D28" s="10"/>
-      <c r="E28" s="10"/>
-      <c r="F28" s="11"/>
-      <c r="H28" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="I28" s="10"/>
-      <c r="J28" s="10"/>
-      <c r="K28" s="10"/>
-      <c r="L28" s="11"/>
-      <c r="N28" s="9" t="s">
-        <v>110</v>
-      </c>
-      <c r="O28" s="10"/>
-      <c r="P28" s="10"/>
-      <c r="Q28" s="10"/>
-      <c r="R28" s="11"/>
+      <c r="B28" s="8" t="s">
+        <v>189</v>
+      </c>
+      <c r="C28" s="9"/>
+      <c r="D28" s="9"/>
+      <c r="E28" s="9"/>
+      <c r="F28" s="10"/>
+      <c r="H28" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="I28" s="9"/>
+      <c r="J28" s="9"/>
+      <c r="K28" s="9"/>
+      <c r="L28" s="10"/>
+      <c r="N28" s="8" t="s">
+        <v>190</v>
+      </c>
+      <c r="O28" s="9"/>
+      <c r="P28" s="9"/>
+      <c r="Q28" s="9"/>
+      <c r="R28" s="10"/>
     </row>
     <row r="29" spans="2:18">
-      <c r="B29" s="9"/>
-      <c r="C29" s="10"/>
-      <c r="D29" s="10"/>
-      <c r="E29" s="10"/>
-      <c r="F29" s="11"/>
-      <c r="H29" s="9"/>
-      <c r="I29" s="10"/>
-      <c r="J29" s="10"/>
-      <c r="K29" s="10"/>
-      <c r="L29" s="11"/>
-      <c r="N29" s="9" t="s">
-        <v>111</v>
-      </c>
-      <c r="O29" s="10"/>
-      <c r="P29" s="10"/>
-      <c r="Q29" s="10"/>
-      <c r="R29" s="11"/>
+      <c r="B29" s="8"/>
+      <c r="C29" s="9"/>
+      <c r="D29" s="9"/>
+      <c r="E29" s="9"/>
+      <c r="F29" s="10"/>
+      <c r="H29" s="8"/>
+      <c r="I29" s="9"/>
+      <c r="J29" s="9"/>
+      <c r="K29" s="9"/>
+      <c r="L29" s="10"/>
+      <c r="N29" s="8" t="s">
+        <v>191</v>
+      </c>
+      <c r="O29" s="9"/>
+      <c r="P29" s="9"/>
+      <c r="Q29" s="9"/>
+      <c r="R29" s="10"/>
     </row>
     <row r="30" spans="2:18">
-      <c r="B30" s="9" t="s">
-        <v>112</v>
-      </c>
-      <c r="C30" s="10"/>
-      <c r="D30" s="10"/>
-      <c r="E30" s="10"/>
-      <c r="F30" s="11"/>
-      <c r="H30" s="9" t="s">
-        <v>113</v>
-      </c>
-      <c r="I30" s="10"/>
-      <c r="J30" s="10"/>
-      <c r="K30" s="10"/>
-      <c r="L30" s="11"/>
-      <c r="N30" s="9"/>
-      <c r="O30" s="10"/>
-      <c r="P30" s="10"/>
-      <c r="Q30" s="10"/>
-      <c r="R30" s="11"/>
+      <c r="B30" s="8" t="s">
+        <v>192</v>
+      </c>
+      <c r="C30" s="9"/>
+      <c r="D30" s="9"/>
+      <c r="E30" s="9"/>
+      <c r="F30" s="10"/>
+      <c r="H30" s="8" t="s">
+        <v>193</v>
+      </c>
+      <c r="I30" s="9"/>
+      <c r="J30" s="9"/>
+      <c r="K30" s="9"/>
+      <c r="L30" s="10"/>
+      <c r="N30" s="8"/>
+      <c r="O30" s="9"/>
+      <c r="P30" s="9"/>
+      <c r="Q30" s="9"/>
+      <c r="R30" s="10"/>
     </row>
     <row r="31" spans="2:18">
-      <c r="B31" s="9"/>
-      <c r="C31" s="10"/>
-      <c r="D31" s="10"/>
-      <c r="E31" s="10"/>
-      <c r="F31" s="11"/>
-      <c r="H31" s="9"/>
-      <c r="I31" s="10"/>
-      <c r="J31" s="10"/>
-      <c r="K31" s="10"/>
-      <c r="L31" s="11"/>
-      <c r="N31" s="9" t="s">
-        <v>114</v>
-      </c>
-      <c r="O31" s="10"/>
-      <c r="P31" s="10"/>
-      <c r="Q31" s="10"/>
-      <c r="R31" s="11"/>
+      <c r="B31" s="8"/>
+      <c r="C31" s="9"/>
+      <c r="D31" s="9"/>
+      <c r="E31" s="9"/>
+      <c r="F31" s="10"/>
+      <c r="H31" s="8"/>
+      <c r="I31" s="9"/>
+      <c r="J31" s="9"/>
+      <c r="K31" s="9"/>
+      <c r="L31" s="10"/>
+      <c r="N31" s="8" t="s">
+        <v>194</v>
+      </c>
+      <c r="O31" s="9"/>
+      <c r="P31" s="9"/>
+      <c r="Q31" s="9"/>
+      <c r="R31" s="10"/>
     </row>
     <row r="32" spans="2:18">
-      <c r="B32" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="C32" s="10"/>
-      <c r="D32" s="10"/>
-      <c r="E32" s="10"/>
-      <c r="F32" s="11"/>
-      <c r="H32" s="9" t="s">
-        <v>115</v>
-      </c>
-      <c r="I32" s="10"/>
-      <c r="J32" s="10"/>
-      <c r="K32" s="10"/>
-      <c r="L32" s="11"/>
-      <c r="N32" s="9" t="s">
-        <v>116</v>
-      </c>
-      <c r="O32" s="10"/>
-      <c r="P32" s="10"/>
-      <c r="Q32" s="10"/>
-      <c r="R32" s="11"/>
+      <c r="B32" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="C32" s="9"/>
+      <c r="D32" s="9"/>
+      <c r="E32" s="9"/>
+      <c r="F32" s="10"/>
+      <c r="H32" s="8" t="s">
+        <v>195</v>
+      </c>
+      <c r="I32" s="9"/>
+      <c r="J32" s="9"/>
+      <c r="K32" s="9"/>
+      <c r="L32" s="10"/>
+      <c r="N32" s="8" t="s">
+        <v>196</v>
+      </c>
+      <c r="O32" s="9"/>
+      <c r="P32" s="9"/>
+      <c r="Q32" s="9"/>
+      <c r="R32" s="10"/>
     </row>
     <row r="33" spans="2:18">
-      <c r="B33" s="12"/>
-      <c r="C33" s="13"/>
-      <c r="D33" s="13"/>
-      <c r="E33" s="13"/>
-      <c r="F33" s="14"/>
-      <c r="H33" s="12"/>
-      <c r="I33" s="13"/>
-      <c r="J33" s="13"/>
-      <c r="K33" s="13"/>
-      <c r="L33" s="14"/>
-      <c r="N33" s="12"/>
-      <c r="O33" s="13"/>
-      <c r="P33" s="13"/>
-      <c r="Q33" s="13"/>
-      <c r="R33" s="14"/>
-    </row>
-    <row r="37" spans="2:18" ht="14.7" thickBot="1"/>
+      <c r="B33" s="11"/>
+      <c r="C33" s="12"/>
+      <c r="D33" s="12"/>
+      <c r="E33" s="12"/>
+      <c r="F33" s="13"/>
+      <c r="H33" s="11"/>
+      <c r="I33" s="12"/>
+      <c r="J33" s="12"/>
+      <c r="K33" s="12"/>
+      <c r="L33" s="13"/>
+      <c r="N33" s="11"/>
+      <c r="O33" s="12"/>
+      <c r="P33" s="12"/>
+      <c r="Q33" s="12"/>
+      <c r="R33" s="13"/>
+    </row>
+    <row r="37" spans="2:18" ht="14.65" thickBot="1"/>
     <row r="38" spans="2:18">
       <c r="B38" s="38" t="s">
-        <v>117</v>
+        <v>197</v>
       </c>
       <c r="C38" s="39"/>
       <c r="D38" s="39"/>
       <c r="E38" s="39"/>
       <c r="F38" s="40"/>
       <c r="H38" s="86" t="s">
-        <v>118</v>
+        <v>198</v>
       </c>
       <c r="I38" s="87"/>
       <c r="J38" s="87"/>
       <c r="K38" s="87"/>
       <c r="L38" s="88"/>
       <c r="N38" s="50" t="s">
-        <v>119</v>
+        <v>199</v>
       </c>
       <c r="O38" s="51"/>
       <c r="P38" s="51"/>
       <c r="Q38" s="51"/>
       <c r="R38" s="52"/>
     </row>
-    <row r="39" spans="2:18" ht="14.7" thickBot="1">
+    <row r="39" spans="2:18" ht="14.65" thickBot="1">
       <c r="B39" s="41"/>
       <c r="C39" s="42"/>
       <c r="D39" s="42"/>
@@ -4652,21 +4709,21 @@
     </row>
     <row r="40" spans="2:18">
       <c r="B40" s="56" t="s">
-        <v>120</v>
+        <v>200</v>
       </c>
       <c r="C40" s="57"/>
       <c r="D40" s="57"/>
       <c r="E40" s="57"/>
       <c r="F40" s="58"/>
       <c r="H40" s="56" t="s">
-        <v>121</v>
+        <v>201</v>
       </c>
       <c r="I40" s="57"/>
       <c r="J40" s="57"/>
       <c r="K40" s="57"/>
       <c r="L40" s="58"/>
       <c r="N40" s="56" t="s">
-        <v>122</v>
+        <v>202</v>
       </c>
       <c r="O40" s="57"/>
       <c r="P40" s="57"/>
@@ -4724,31 +4781,31 @@
       <c r="Q43" s="63"/>
       <c r="R43" s="64"/>
     </row>
-    <row r="45" spans="2:18" ht="14.7" thickBot="1"/>
-    <row r="46" spans="2:18" ht="16" customHeight="1">
+    <row r="45" spans="2:18" ht="14.65" thickBot="1"/>
+    <row r="46" spans="2:18" ht="15.95" customHeight="1">
       <c r="B46" s="38" t="s">
-        <v>102</v>
+        <v>182</v>
       </c>
       <c r="C46" s="39"/>
       <c r="D46" s="39"/>
       <c r="E46" s="39"/>
       <c r="F46" s="40"/>
       <c r="H46" s="92" t="s">
-        <v>102</v>
+        <v>182</v>
       </c>
       <c r="I46" s="93"/>
       <c r="J46" s="93"/>
       <c r="K46" s="93"/>
       <c r="L46" s="94"/>
       <c r="N46" s="50" t="s">
-        <v>102</v>
+        <v>182</v>
       </c>
       <c r="O46" s="51"/>
       <c r="P46" s="51"/>
       <c r="Q46" s="51"/>
       <c r="R46" s="52"/>
     </row>
-    <row r="47" spans="2:18" ht="16" customHeight="1" thickBot="1">
+    <row r="47" spans="2:18" ht="15.95" customHeight="1" thickBot="1">
       <c r="B47" s="41"/>
       <c r="C47" s="42"/>
       <c r="D47" s="42"/>
@@ -4767,21 +4824,21 @@
     </row>
     <row r="48" spans="2:18">
       <c r="B48" s="77" t="s">
-        <v>123</v>
+        <v>203</v>
       </c>
       <c r="C48" s="78"/>
       <c r="D48" s="78"/>
       <c r="E48" s="78"/>
       <c r="F48" s="79"/>
       <c r="H48" s="101" t="s">
-        <v>124</v>
+        <v>204</v>
       </c>
       <c r="I48" s="78"/>
       <c r="J48" s="78"/>
       <c r="K48" s="78"/>
       <c r="L48" s="79"/>
       <c r="N48" s="77" t="s">
-        <v>125</v>
+        <v>205</v>
       </c>
       <c r="O48" s="78"/>
       <c r="P48" s="78"/>
@@ -4858,21 +4915,21 @@
     </row>
     <row r="53" spans="2:18">
       <c r="B53" s="77" t="s">
-        <v>126</v>
+        <v>206</v>
       </c>
       <c r="C53" s="78"/>
       <c r="D53" s="78"/>
       <c r="E53" s="78"/>
       <c r="F53" s="79"/>
       <c r="H53" s="77" t="s">
-        <v>127</v>
+        <v>207</v>
       </c>
       <c r="I53" s="78"/>
       <c r="J53" s="78"/>
       <c r="K53" s="78"/>
       <c r="L53" s="79"/>
       <c r="N53" s="77" t="s">
-        <v>128</v>
+        <v>208</v>
       </c>
       <c r="O53" s="78"/>
       <c r="P53" s="78"/>
@@ -4947,179 +5004,179 @@
       <c r="Q57" s="84"/>
       <c r="R57" s="85"/>
     </row>
-    <row r="60" spans="2:18" ht="18.3">
-      <c r="B60" s="6" t="s">
-        <v>108</v>
-      </c>
-      <c r="C60" s="7"/>
-      <c r="D60" s="7"/>
-      <c r="E60" s="7"/>
-      <c r="F60" s="8"/>
-      <c r="H60" s="6" t="s">
-        <v>108</v>
-      </c>
-      <c r="I60" s="7"/>
-      <c r="J60" s="7"/>
-      <c r="K60" s="7"/>
-      <c r="L60" s="8"/>
-      <c r="N60" s="6" t="s">
-        <v>108</v>
-      </c>
-      <c r="O60" s="7"/>
-      <c r="P60" s="7"/>
-      <c r="Q60" s="7"/>
-      <c r="R60" s="8"/>
+    <row r="60" spans="2:18" ht="18.399999999999999">
+      <c r="B60" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="C60" s="6"/>
+      <c r="D60" s="6"/>
+      <c r="E60" s="6"/>
+      <c r="F60" s="7"/>
+      <c r="H60" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="I60" s="6"/>
+      <c r="J60" s="6"/>
+      <c r="K60" s="6"/>
+      <c r="L60" s="7"/>
+      <c r="N60" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="O60" s="6"/>
+      <c r="P60" s="6"/>
+      <c r="Q60" s="6"/>
+      <c r="R60" s="7"/>
     </row>
     <row r="61" spans="2:18">
-      <c r="B61" s="9"/>
-      <c r="C61" s="10"/>
-      <c r="D61" s="10"/>
-      <c r="E61" s="10"/>
-      <c r="F61" s="11"/>
-      <c r="H61" s="9"/>
-      <c r="I61" s="10"/>
-      <c r="J61" s="10"/>
-      <c r="K61" s="10"/>
-      <c r="L61" s="11"/>
-      <c r="N61" s="15" t="s">
-        <v>129</v>
-      </c>
-      <c r="O61" s="16"/>
-      <c r="P61" s="16"/>
-      <c r="Q61" s="16"/>
-      <c r="R61" s="17"/>
+      <c r="B61" s="8"/>
+      <c r="C61" s="9"/>
+      <c r="D61" s="9"/>
+      <c r="E61" s="9"/>
+      <c r="F61" s="10"/>
+      <c r="H61" s="8"/>
+      <c r="I61" s="9"/>
+      <c r="J61" s="9"/>
+      <c r="K61" s="9"/>
+      <c r="L61" s="10"/>
+      <c r="N61" s="14" t="s">
+        <v>209</v>
+      </c>
+      <c r="O61" s="15"/>
+      <c r="P61" s="15"/>
+      <c r="Q61" s="15"/>
+      <c r="R61" s="16"/>
     </row>
     <row r="62" spans="2:18">
-      <c r="B62" s="9" t="s">
-        <v>130</v>
-      </c>
-      <c r="C62" s="10"/>
-      <c r="D62" s="10"/>
-      <c r="E62" s="10"/>
-      <c r="F62" s="11"/>
-      <c r="H62" s="9" t="s">
-        <v>131</v>
-      </c>
-      <c r="I62" s="10"/>
-      <c r="J62" s="10"/>
-      <c r="K62" s="10"/>
-      <c r="L62" s="11"/>
-      <c r="N62" s="15" t="s">
-        <v>132</v>
-      </c>
-      <c r="O62" s="16"/>
-      <c r="P62" s="16"/>
-      <c r="Q62" s="16"/>
-      <c r="R62" s="17"/>
+      <c r="B62" s="8" t="s">
+        <v>210</v>
+      </c>
+      <c r="C62" s="9"/>
+      <c r="D62" s="9"/>
+      <c r="E62" s="9"/>
+      <c r="F62" s="10"/>
+      <c r="H62" s="8" t="s">
+        <v>211</v>
+      </c>
+      <c r="I62" s="9"/>
+      <c r="J62" s="9"/>
+      <c r="K62" s="9"/>
+      <c r="L62" s="10"/>
+      <c r="N62" s="14" t="s">
+        <v>212</v>
+      </c>
+      <c r="O62" s="15"/>
+      <c r="P62" s="15"/>
+      <c r="Q62" s="15"/>
+      <c r="R62" s="16"/>
     </row>
     <row r="63" spans="2:18">
-      <c r="B63" s="9"/>
-      <c r="C63" s="10"/>
-      <c r="D63" s="10"/>
-      <c r="E63" s="10"/>
-      <c r="F63" s="11"/>
-      <c r="H63" s="9" t="s">
-        <v>133</v>
-      </c>
-      <c r="I63" s="10"/>
-      <c r="J63" s="10"/>
-      <c r="K63" s="10"/>
-      <c r="L63" s="11"/>
-      <c r="N63" s="15" t="s">
-        <v>134</v>
-      </c>
-      <c r="O63" s="16"/>
-      <c r="P63" s="16"/>
-      <c r="Q63" s="16"/>
-      <c r="R63" s="17"/>
+      <c r="B63" s="8"/>
+      <c r="C63" s="9"/>
+      <c r="D63" s="9"/>
+      <c r="E63" s="9"/>
+      <c r="F63" s="10"/>
+      <c r="H63" s="8" t="s">
+        <v>213</v>
+      </c>
+      <c r="I63" s="9"/>
+      <c r="J63" s="9"/>
+      <c r="K63" s="9"/>
+      <c r="L63" s="10"/>
+      <c r="N63" s="14" t="s">
+        <v>214</v>
+      </c>
+      <c r="O63" s="15"/>
+      <c r="P63" s="15"/>
+      <c r="Q63" s="15"/>
+      <c r="R63" s="16"/>
     </row>
     <row r="64" spans="2:18">
-      <c r="B64" s="9" t="s">
-        <v>135</v>
-      </c>
-      <c r="C64" s="10"/>
-      <c r="D64" s="10"/>
-      <c r="E64" s="10"/>
-      <c r="F64" s="11"/>
-      <c r="H64" s="18"/>
-      <c r="I64" s="10"/>
-      <c r="J64" s="10"/>
-      <c r="K64" s="10"/>
-      <c r="L64" s="11"/>
-      <c r="N64" s="19" t="s">
-        <v>136</v>
-      </c>
-      <c r="O64" s="20"/>
-      <c r="P64" s="20"/>
-      <c r="Q64" s="20"/>
-      <c r="R64" s="21"/>
+      <c r="B64" s="8" t="s">
+        <v>215</v>
+      </c>
+      <c r="C64" s="9"/>
+      <c r="D64" s="9"/>
+      <c r="E64" s="9"/>
+      <c r="F64" s="10"/>
+      <c r="H64" s="17"/>
+      <c r="I64" s="9"/>
+      <c r="J64" s="9"/>
+      <c r="K64" s="9"/>
+      <c r="L64" s="10"/>
+      <c r="N64" s="18" t="s">
+        <v>216</v>
+      </c>
+      <c r="O64" s="19"/>
+      <c r="P64" s="19"/>
+      <c r="Q64" s="19"/>
+      <c r="R64" s="20"/>
     </row>
     <row r="65" spans="2:18">
-      <c r="B65" s="9"/>
-      <c r="C65" s="10"/>
-      <c r="D65" s="10"/>
-      <c r="E65" s="10"/>
-      <c r="F65" s="11"/>
-      <c r="H65" s="9" t="s">
-        <v>137</v>
-      </c>
-      <c r="I65" s="10"/>
-      <c r="J65" s="10"/>
-      <c r="K65" s="10"/>
-      <c r="L65" s="11"/>
-      <c r="N65" s="19" t="s">
-        <v>138</v>
-      </c>
-      <c r="O65" s="20"/>
-      <c r="P65" s="20"/>
-      <c r="Q65" s="20"/>
-      <c r="R65" s="21"/>
+      <c r="B65" s="8"/>
+      <c r="C65" s="9"/>
+      <c r="D65" s="9"/>
+      <c r="E65" s="9"/>
+      <c r="F65" s="10"/>
+      <c r="H65" s="8" t="s">
+        <v>217</v>
+      </c>
+      <c r="I65" s="9"/>
+      <c r="J65" s="9"/>
+      <c r="K65" s="9"/>
+      <c r="L65" s="10"/>
+      <c r="N65" s="18" t="s">
+        <v>218</v>
+      </c>
+      <c r="O65" s="19"/>
+      <c r="P65" s="19"/>
+      <c r="Q65" s="19"/>
+      <c r="R65" s="20"/>
     </row>
     <row r="66" spans="2:18" ht="15.6">
-      <c r="B66" s="9" t="s">
-        <v>139</v>
-      </c>
-      <c r="C66" s="10"/>
-      <c r="D66" s="10"/>
-      <c r="E66" s="10"/>
-      <c r="F66" s="11"/>
-      <c r="H66" s="9" t="s">
-        <v>140</v>
-      </c>
-      <c r="I66" s="10"/>
-      <c r="J66" s="10"/>
-      <c r="K66" s="10"/>
-      <c r="L66" s="11"/>
-      <c r="N66" s="22" t="s">
-        <v>141</v>
-      </c>
-      <c r="O66" s="23"/>
-      <c r="P66" s="23"/>
-      <c r="Q66" s="23"/>
-      <c r="R66" s="24"/>
+      <c r="B66" s="8" t="s">
+        <v>219</v>
+      </c>
+      <c r="C66" s="9"/>
+      <c r="D66" s="9"/>
+      <c r="E66" s="9"/>
+      <c r="F66" s="10"/>
+      <c r="H66" s="8" t="s">
+        <v>220</v>
+      </c>
+      <c r="I66" s="9"/>
+      <c r="J66" s="9"/>
+      <c r="K66" s="9"/>
+      <c r="L66" s="10"/>
+      <c r="N66" s="21" t="s">
+        <v>221</v>
+      </c>
+      <c r="O66" s="22"/>
+      <c r="P66" s="22"/>
+      <c r="Q66" s="22"/>
+      <c r="R66" s="23"/>
     </row>
     <row r="67" spans="2:18" ht="15.6">
-      <c r="B67" s="12"/>
-      <c r="C67" s="13"/>
-      <c r="D67" s="13"/>
-      <c r="E67" s="13"/>
-      <c r="F67" s="14"/>
-      <c r="H67" s="12"/>
-      <c r="I67" s="13"/>
-      <c r="J67" s="13"/>
-      <c r="K67" s="13"/>
-      <c r="L67" s="14"/>
-      <c r="N67" s="25" t="s">
-        <v>142</v>
-      </c>
-      <c r="O67" s="26"/>
-      <c r="P67" s="26"/>
-      <c r="Q67" s="26"/>
-      <c r="R67" s="27"/>
+      <c r="B67" s="11"/>
+      <c r="C67" s="12"/>
+      <c r="D67" s="12"/>
+      <c r="E67" s="12"/>
+      <c r="F67" s="13"/>
+      <c r="H67" s="11"/>
+      <c r="I67" s="12"/>
+      <c r="J67" s="12"/>
+      <c r="K67" s="12"/>
+      <c r="L67" s="13"/>
+      <c r="N67" s="24" t="s">
+        <v>222</v>
+      </c>
+      <c r="O67" s="25"/>
+      <c r="P67" s="25"/>
+      <c r="Q67" s="25"/>
+      <c r="R67" s="26"/>
     </row>
     <row r="70" spans="2:18" ht="15.6">
       <c r="N70" s="98" t="s">
-        <v>143</v>
+        <v>223</v>
       </c>
       <c r="O70" s="99"/>
       <c r="P70" s="99"/>
@@ -5127,73 +5184,73 @@
       <c r="R70" s="100"/>
     </row>
     <row r="71" spans="2:18" ht="32.1" customHeight="1">
-      <c r="N71" s="28"/>
-      <c r="O71" s="29" t="s">
-        <v>144</v>
-      </c>
-      <c r="P71" s="29" t="s">
-        <v>145</v>
-      </c>
-      <c r="Q71" s="29" t="s">
-        <v>146</v>
-      </c>
-      <c r="R71" s="30" t="s">
-        <v>147</v>
+      <c r="N71" s="27"/>
+      <c r="O71" s="28" t="s">
+        <v>224</v>
+      </c>
+      <c r="P71" s="28" t="s">
+        <v>225</v>
+      </c>
+      <c r="Q71" s="28" t="s">
+        <v>226</v>
+      </c>
+      <c r="R71" s="29" t="s">
+        <v>227</v>
       </c>
     </row>
     <row r="72" spans="2:18" ht="32.1" customHeight="1">
-      <c r="N72" s="29" t="s">
-        <v>144</v>
-      </c>
-      <c r="O72" s="31">
+      <c r="N72" s="28" t="s">
+        <v>224</v>
+      </c>
+      <c r="O72" s="30">
         <v>0</v>
       </c>
-      <c r="P72" s="31"/>
-      <c r="Q72" s="31"/>
-      <c r="R72" s="32" t="s">
-        <v>148</v>
+      <c r="P72" s="30"/>
+      <c r="Q72" s="30"/>
+      <c r="R72" s="31" t="s">
+        <v>228</v>
       </c>
     </row>
     <row r="73" spans="2:18" ht="32.1" customHeight="1">
-      <c r="N73" s="29" t="s">
-        <v>145</v>
-      </c>
-      <c r="O73" s="31"/>
-      <c r="P73" s="31">
+      <c r="N73" s="28" t="s">
+        <v>225</v>
+      </c>
+      <c r="O73" s="30"/>
+      <c r="P73" s="30">
         <v>0</v>
       </c>
-      <c r="Q73" s="31"/>
-      <c r="R73" s="33" t="s">
-        <v>149</v>
+      <c r="Q73" s="30"/>
+      <c r="R73" s="32" t="s">
+        <v>229</v>
       </c>
     </row>
     <row r="74" spans="2:18" ht="32.1" customHeight="1">
-      <c r="N74" s="29" t="s">
-        <v>146</v>
-      </c>
-      <c r="O74" s="31"/>
-      <c r="P74" s="31"/>
-      <c r="Q74" s="31">
+      <c r="N74" s="28" t="s">
+        <v>226</v>
+      </c>
+      <c r="O74" s="30"/>
+      <c r="P74" s="30"/>
+      <c r="Q74" s="30">
         <v>0</v>
       </c>
-      <c r="R74" s="34" t="s">
-        <v>150</v>
+      <c r="R74" s="33" t="s">
+        <v>230</v>
       </c>
     </row>
     <row r="75" spans="2:18" ht="32.1" customHeight="1">
-      <c r="N75" s="30" t="s">
-        <v>147</v>
-      </c>
-      <c r="O75" s="32" t="s">
-        <v>148</v>
-      </c>
-      <c r="P75" s="35" t="s">
-        <v>149</v>
-      </c>
-      <c r="Q75" s="34" t="s">
-        <v>150</v>
-      </c>
-      <c r="R75" s="31">
+      <c r="N75" s="29" t="s">
+        <v>227</v>
+      </c>
+      <c r="O75" s="31" t="s">
+        <v>228</v>
+      </c>
+      <c r="P75" s="34" t="s">
+        <v>229</v>
+      </c>
+      <c r="Q75" s="33" t="s">
+        <v>230</v>
+      </c>
+      <c r="R75" s="30">
         <v>0</v>
       </c>
     </row>

</xml_diff>